<commit_message>
finaliza jornada QH 01-12-2014
</commit_message>
<xml_diff>
--- a/Documentacion/indicadores revisión junio 11 2014.xlsx
+++ b/Documentacion/indicadores revisión junio 11 2014.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="Ajustes" sheetId="1" r:id="rId1"/>
@@ -1020,8 +1020,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -1170,7 +1170,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1198,6 +1198,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1284,9 +1290,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1362,9 +1368,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1432,21 +1435,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1471,15 +1483,22 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -1807,17 +1826,17 @@
   <dimension ref="B1:R41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.5703125" style="6" customWidth="1"/>
     <col min="2" max="2" width="32" style="1" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="44" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.5703125" style="3" customWidth="1"/>
     <col min="5" max="5" width="30.140625" style="4" customWidth="1"/>
     <col min="6" max="6" width="31" style="4" customWidth="1"/>
@@ -1832,10 +1851,10 @@
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="57"/>
+      <c r="D2" s="59"/>
       <c r="E2" s="8" t="s">
         <v>2</v>
       </c>
@@ -1851,36 +1870,36 @@
       <c r="I2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="55" t="s">
+      <c r="J2" s="54" t="s">
         <v>147</v>
       </c>
-      <c r="K2" s="55" t="s">
+      <c r="K2" s="54" t="s">
         <v>156</v>
       </c>
-      <c r="L2" s="55" t="s">
+      <c r="L2" s="54" t="s">
         <v>149</v>
       </c>
-      <c r="M2" s="55" t="s">
+      <c r="M2" s="54" t="s">
         <v>159</v>
       </c>
-      <c r="N2" s="55" t="s">
+      <c r="N2" s="54" t="s">
         <v>148</v>
       </c>
-      <c r="O2" s="55" t="s">
+      <c r="O2" s="54" t="s">
         <v>153</v>
       </c>
-      <c r="P2" s="55" t="s">
+      <c r="P2" s="54" t="s">
         <v>150</v>
       </c>
-      <c r="Q2" s="55" t="s">
+      <c r="Q2" s="54" t="s">
         <v>151</v>
       </c>
-      <c r="R2" s="55" t="s">
+      <c r="R2" s="54" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="3" spans="2:18" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="55" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="11" t="s">
@@ -1892,16 +1911,16 @@
       <c r="E3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="58" t="s">
+      <c r="F3" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="60" t="s">
+      <c r="G3" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="60" t="s">
+      <c r="H3" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="62" t="s">
+      <c r="I3" s="64" t="s">
         <v>14</v>
       </c>
       <c r="J3" s="23" t="s">
@@ -1931,7 +1950,7 @@
       <c r="R3" s="23"/>
     </row>
     <row r="4" spans="2:18" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="65" t="s">
+      <c r="B4" s="56" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="15" t="s">
@@ -1943,10 +1962,10 @@
       <c r="E4" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="59"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
-      <c r="I4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
       <c r="J4" s="23" t="s">
         <v>152</v>
       </c>
@@ -1974,7 +1993,7 @@
       <c r="R4" s="23"/>
     </row>
     <row r="5" spans="2:18" ht="104.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="57" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="15" t="s">
@@ -1989,9 +2008,9 @@
       <c r="F5" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
-      <c r="I5" s="61"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
       <c r="J5" s="23" t="s">
         <v>152</v>
       </c>
@@ -2175,56 +2194,56 @@
       </c>
       <c r="R8" s="23"/>
     </row>
-    <row r="9" spans="2:18" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="14" t="s">
+    <row r="9" spans="2:18" s="71" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="66" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="68" t="s">
         <v>158</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="69" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="24" t="s">
+      <c r="G9" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="24" t="s">
+      <c r="H9" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="I9" s="24" t="s">
+      <c r="I9" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="J9" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="K9" s="23" t="s">
+      <c r="J9" s="67" t="s">
+        <v>152</v>
+      </c>
+      <c r="K9" s="67" t="s">
         <v>157</v>
       </c>
-      <c r="L9" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="M9" s="23" t="s">
+      <c r="L9" s="67" t="s">
+        <v>152</v>
+      </c>
+      <c r="M9" s="67" t="s">
         <v>157</v>
       </c>
-      <c r="N9" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="O9" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="P9" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q9" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="R9" s="23"/>
+      <c r="N9" s="67" t="s">
+        <v>152</v>
+      </c>
+      <c r="O9" s="67" t="s">
+        <v>152</v>
+      </c>
+      <c r="P9" s="67" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q9" s="67" t="s">
+        <v>152</v>
+      </c>
+      <c r="R9" s="67"/>
     </row>
     <row r="10" spans="2:18" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="22" t="s">
@@ -2277,45 +2296,45 @@
       </c>
       <c r="R10" s="23"/>
     </row>
-    <row r="11" spans="2:18" s="30" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="28" t="s">
+    <row r="11" spans="2:18" s="29" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="63" t="s">
+      <c r="D11" s="65" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="56" t="s">
+      <c r="E11" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="F11" s="63" t="s">
+      <c r="F11" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="63" t="s">
+      <c r="G11" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="H11" s="56" t="s">
+      <c r="H11" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="I11" s="56" t="s">
+      <c r="I11" s="58" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="2:18" s="30" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="28" t="s">
+    <row r="12" spans="2:18" s="29" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="63"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="63"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="56"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="65"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="58"/>
+      <c r="I12" s="58"/>
     </row>
     <row r="13" spans="2:18" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="22" t="s">
@@ -2327,7 +2346,7 @@
       <c r="D13" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="31" t="s">
+      <c r="E13" s="30" t="s">
         <v>70</v>
       </c>
       <c r="F13" s="17" t="s">
@@ -2399,7 +2418,7 @@
       <c r="B16" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="31" t="s">
         <v>86</v>
       </c>
       <c r="D16" s="15" t="s">
@@ -2425,10 +2444,10 @@
       <c r="B17" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="33" t="s">
+      <c r="C17" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="32" t="s">
         <v>93</v>
       </c>
       <c r="E17" s="17" t="s">
@@ -2447,78 +2466,78 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="2:9" s="30" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="28" t="s">
+    <row r="18" spans="2:9" s="29" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="D18" s="34" t="s">
+      <c r="D18" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="E18" s="35" t="s">
+      <c r="E18" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="F18" s="36" t="s">
+      <c r="F18" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="G18" s="37" t="s">
+      <c r="G18" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="H18" s="37" t="s">
+      <c r="H18" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="I18" s="37" t="s">
+      <c r="I18" s="36" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="2:9" s="30" customFormat="1" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="38" t="s">
+    <row r="19" spans="2:9" s="29" customFormat="1" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="C19" s="38" t="s">
+      <c r="C19" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="D19" s="38" t="s">
+      <c r="D19" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="E19" s="38" t="s">
+      <c r="E19" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="F19" s="35" t="s">
+      <c r="F19" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="G19" s="37" t="s">
+      <c r="G19" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="36" t="s">
         <v>108</v>
       </c>
       <c r="I19" s="26" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="2:9" s="30" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="38" t="s">
+    <row r="20" spans="2:9" s="29" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="C20" s="38" t="s">
+      <c r="C20" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="D20" s="38" t="s">
+      <c r="D20" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="E20" s="38" t="s">
+      <c r="E20" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="F20" s="38" t="s">
+      <c r="F20" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="G20" s="37" t="s">
+      <c r="G20" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="H20" s="37" t="s">
+      <c r="H20" s="36" t="s">
         <v>108</v>
       </c>
       <c r="I20" s="26" t="s">
@@ -2526,19 +2545,19 @@
       </c>
     </row>
     <row r="21" spans="2:9" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="38" t="s">
+      <c r="B21" s="37" t="s">
         <v>114</v>
       </c>
-      <c r="C21" s="39" t="s">
+      <c r="C21" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="D21" s="40" t="s">
+      <c r="D21" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="E21" s="41" t="s">
+      <c r="E21" s="40" t="s">
         <v>117</v>
       </c>
-      <c r="F21" s="42" t="s">
+      <c r="F21" s="41" t="s">
         <v>118</v>
       </c>
       <c r="G21" s="24" t="s">
@@ -2551,34 +2570,34 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="2:9" s="30" customFormat="1" ht="137.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="43" t="s">
+    <row r="22" spans="2:9" s="29" customFormat="1" ht="137.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="C22" s="33" t="s">
+      <c r="C22" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="D22" s="44" t="s">
+      <c r="D22" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="E22" s="41" t="s">
+      <c r="E22" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="F22" s="38" t="s">
+      <c r="F22" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="G22" s="37" t="s">
+      <c r="G22" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="H22" s="33" t="s">
+      <c r="H22" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="I22" s="44" t="s">
+      <c r="I22" s="43" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="23" spans="2:9" ht="137.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="45" t="s">
+      <c r="B23" s="44" t="s">
         <v>124</v>
       </c>
       <c r="C23" s="15" t="s">
@@ -2603,52 +2622,52 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="2:9" s="30" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="46" t="s">
+    <row r="24" spans="2:9" s="29" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="45" t="s">
         <v>129</v>
       </c>
-      <c r="C24" s="33" t="s">
+      <c r="C24" s="32" t="s">
         <v>130</v>
       </c>
-      <c r="D24" s="37" t="s">
+      <c r="D24" s="36" t="s">
         <v>131</v>
       </c>
-      <c r="E24" s="36" t="s">
+      <c r="E24" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="F24" s="36" t="s">
+      <c r="F24" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="G24" s="37" t="s">
+      <c r="G24" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="H24" s="37" t="s">
+      <c r="H24" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="I24" s="37" t="s">
+      <c r="I24" s="36" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="2:9" s="30" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:9" s="29" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="C25" s="33" t="s">
+      <c r="C25" s="32" t="s">
         <v>136</v>
       </c>
       <c r="D25" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="E25" s="37" t="s">
+      <c r="E25" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="F25" s="36" t="s">
+      <c r="F25" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="G25" s="37" t="s">
+      <c r="G25" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="H25" s="37" t="s">
+      <c r="H25" s="36" t="s">
         <v>140</v>
       </c>
       <c r="I25" s="24" t="s">
@@ -2656,52 +2675,52 @@
       </c>
     </row>
     <row r="26" spans="2:9" ht="102.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="46" t="s">
         <v>141</v>
       </c>
-      <c r="C26" s="48" t="s">
+      <c r="C26" s="47" t="s">
         <v>142</v>
       </c>
       <c r="D26" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="E26" s="44" t="s">
+      <c r="E26" s="43" t="s">
         <v>144</v>
       </c>
-      <c r="F26" s="49" t="s">
+      <c r="F26" s="48" t="s">
         <v>145</v>
       </c>
-      <c r="G26" s="50" t="s">
+      <c r="G26" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="H26" s="50" t="s">
+      <c r="H26" s="49" t="s">
         <v>146</v>
       </c>
-      <c r="I26" s="50" t="s">
+      <c r="I26" s="49" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F34" s="51"/>
+      <c r="F34" s="50"/>
     </row>
     <row r="35" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D35" s="52"/>
-      <c r="F35" s="51"/>
+      <c r="D35" s="51"/>
+      <c r="F35" s="50"/>
     </row>
     <row r="36" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F36" s="51"/>
+      <c r="F36" s="50"/>
     </row>
     <row r="37" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F37" s="51"/>
+      <c r="F37" s="50"/>
     </row>
     <row r="38" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F38" s="53"/>
+      <c r="F38" s="52"/>
     </row>
     <row r="40" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F40" s="54"/>
+      <c r="F40" s="53"/>
     </row>
     <row r="41" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F41" s="53"/>
+      <c r="F41" s="52"/>
     </row>
   </sheetData>
   <autoFilter ref="B2:I26">

</xml_diff>

<commit_message>
finaliza jornada QH 04-12-2014
</commit_message>
<xml_diff>
--- a/Documentacion/indicadores revisión junio 11 2014.xlsx
+++ b/Documentacion/indicadores revisión junio 11 2014.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="162">
   <si>
     <t>NOMBRE INDICADOR</t>
   </si>
@@ -1013,6 +1013,12 @@
   </si>
   <si>
     <t>Requiere posicion completa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">productos </t>
+  </si>
+  <si>
+    <t>importaciones</t>
   </si>
 </sst>
 </file>
@@ -1170,7 +1176,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1186,12 +1192,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1450,55 +1450,55 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -1829,7 +1829,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K8" sqref="K8"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1851,10 +1851,10 @@
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="59" t="s">
+      <c r="C2" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="59"/>
+      <c r="D2" s="64"/>
       <c r="E2" s="8" t="s">
         <v>2</v>
       </c>
@@ -1911,16 +1911,16 @@
       <c r="E3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="60" t="s">
+      <c r="F3" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="62" t="s">
+      <c r="G3" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="62" t="s">
+      <c r="H3" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="64" t="s">
+      <c r="I3" s="69" t="s">
         <v>14</v>
       </c>
       <c r="J3" s="23" t="s">
@@ -1962,10 +1962,10 @@
       <c r="E4" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="61"/>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63"/>
-      <c r="I4" s="63"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
       <c r="J4" s="23" t="s">
         <v>152</v>
       </c>
@@ -1993,7 +1993,7 @@
       <c r="R4" s="23"/>
     </row>
     <row r="5" spans="2:18" ht="104.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="71" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="15" t="s">
@@ -2008,9 +2008,9 @@
       <c r="F5" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="63"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
       <c r="J5" s="23" t="s">
         <v>152</v>
       </c>
@@ -2194,59 +2194,59 @@
       </c>
       <c r="R8" s="23"/>
     </row>
-    <row r="9" spans="2:18" s="71" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="66" t="s">
+    <row r="9" spans="2:18" s="62" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="67" t="s">
+      <c r="C9" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="68" t="s">
+      <c r="D9" s="59" t="s">
         <v>158</v>
       </c>
-      <c r="E9" s="69" t="s">
+      <c r="E9" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="69" t="s">
+      <c r="F9" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="70" t="s">
+      <c r="G9" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="70" t="s">
+      <c r="H9" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="I9" s="70" t="s">
+      <c r="I9" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="J9" s="67" t="s">
-        <v>152</v>
-      </c>
-      <c r="K9" s="67" t="s">
+      <c r="J9" s="58" t="s">
+        <v>152</v>
+      </c>
+      <c r="K9" s="58" t="s">
         <v>157</v>
       </c>
-      <c r="L9" s="67" t="s">
-        <v>152</v>
-      </c>
-      <c r="M9" s="67" t="s">
+      <c r="L9" s="58" t="s">
+        <v>152</v>
+      </c>
+      <c r="M9" s="58" t="s">
         <v>157</v>
       </c>
-      <c r="N9" s="67" t="s">
-        <v>152</v>
-      </c>
-      <c r="O9" s="67" t="s">
-        <v>152</v>
-      </c>
-      <c r="P9" s="67" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q9" s="67" t="s">
-        <v>152</v>
-      </c>
-      <c r="R9" s="67"/>
+      <c r="N9" s="58" t="s">
+        <v>152</v>
+      </c>
+      <c r="O9" s="58" t="s">
+        <v>152</v>
+      </c>
+      <c r="P9" s="58" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q9" s="58" t="s">
+        <v>152</v>
+      </c>
+      <c r="R9" s="58"/>
     </row>
     <row r="10" spans="2:18" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="56" t="s">
         <v>52</v>
       </c>
       <c r="C10" s="15" t="s">
@@ -2303,23 +2303,36 @@
       <c r="C11" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="65" t="s">
+      <c r="D11" s="70" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="58" t="s">
+      <c r="E11" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="F11" s="65" t="s">
+      <c r="F11" s="70" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="65" t="s">
+      <c r="G11" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="H11" s="58" t="s">
+      <c r="H11" s="63" t="s">
         <v>45</v>
       </c>
-      <c r="I11" s="58" t="s">
+      <c r="I11" s="63" t="s">
         <v>31</v>
+      </c>
+      <c r="J11" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="K11" s="29">
+        <v>15</v>
+      </c>
+      <c r="L11" s="29">
+        <v>20</v>
+      </c>
+      <c r="M11" s="29">
+        <f>L11*L12</f>
+        <v>500000000</v>
       </c>
     </row>
     <row r="12" spans="2:18" s="29" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.2">
@@ -2329,15 +2342,32 @@
       <c r="C12" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="65"/>
-      <c r="E12" s="58"/>
-      <c r="F12" s="65"/>
-      <c r="G12" s="65"/>
-      <c r="H12" s="58"/>
-      <c r="I12" s="58"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="70"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="63"/>
+      <c r="J12" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="K12" s="29">
+        <v>1500000</v>
+      </c>
+      <c r="L12" s="29">
+        <v>25000000</v>
+      </c>
+      <c r="M12" s="29">
+        <f>K12*K11</f>
+        <v>22500000</v>
+      </c>
+      <c r="N12" s="29">
+        <f>M12-M11</f>
+        <v>-477500000</v>
+      </c>
     </row>
     <row r="13" spans="2:18" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="56" t="s">
         <v>67</v>
       </c>
       <c r="C13" s="15" t="s">

</xml_diff>

<commit_message>
finaliza jornada QH 05-12-2014
</commit_message>
<xml_diff>
--- a/Documentacion/indicadores revisión junio 11 2014.xlsx
+++ b/Documentacion/indicadores revisión junio 11 2014.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="173">
   <si>
     <t>NOMBRE INDICADOR</t>
   </si>
@@ -1047,15 +1047,22 @@
   </si>
   <si>
     <t>part 2014 Exp 2</t>
+  </si>
+  <si>
+    <t>aclarar sector minero energetico</t>
+  </si>
+  <si>
+    <t>definir</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.000%"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -1212,7 +1219,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1240,6 +1247,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1324,11 +1337,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1365,9 +1379,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1471,16 +1482,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1511,6 +1522,9 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1535,13 +1549,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1864,11 +1883,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1909,36 +1928,36 @@
       <c r="I2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="54" t="s">
+      <c r="J2" s="53" t="s">
         <v>147</v>
       </c>
-      <c r="K2" s="54" t="s">
+      <c r="K2" s="53" t="s">
         <v>156</v>
       </c>
-      <c r="L2" s="54" t="s">
+      <c r="L2" s="53" t="s">
         <v>149</v>
       </c>
-      <c r="M2" s="54" t="s">
+      <c r="M2" s="53" t="s">
         <v>159</v>
       </c>
-      <c r="N2" s="54" t="s">
+      <c r="N2" s="53" t="s">
         <v>148</v>
       </c>
-      <c r="O2" s="54" t="s">
+      <c r="O2" s="53" t="s">
         <v>153</v>
       </c>
-      <c r="P2" s="54" t="s">
+      <c r="P2" s="53" t="s">
         <v>150</v>
       </c>
-      <c r="Q2" s="54" t="s">
+      <c r="Q2" s="53" t="s">
         <v>151</v>
       </c>
-      <c r="R2" s="54" t="s">
+      <c r="R2" s="53" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="3" spans="2:18" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="54" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="11" t="s">
@@ -1962,384 +1981,384 @@
       <c r="I3" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="K3" s="23" t="s">
+      <c r="J3" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="K3" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="L3" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="M3" s="23" t="s">
+      <c r="L3" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="M3" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="N3" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="O3" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="P3" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q3" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="R3" s="23"/>
+      <c r="N3" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="O3" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="P3" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q3" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="R3" s="22"/>
     </row>
     <row r="4" spans="2:18" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="16" t="s">
         <v>18</v>
       </c>
       <c r="F4" s="67"/>
       <c r="G4" s="69"/>
       <c r="H4" s="69"/>
       <c r="I4" s="69"/>
-      <c r="J4" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="K4" s="23" t="s">
+      <c r="J4" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="K4" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="L4" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="M4" s="23" t="s">
+      <c r="L4" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="M4" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="N4" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="O4" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="P4" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q4" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="R4" s="23"/>
+      <c r="N4" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="O4" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="P4" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q4" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="R4" s="22"/>
     </row>
     <row r="5" spans="2:18" ht="104.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G5" s="69"/>
       <c r="H5" s="69"/>
       <c r="I5" s="69"/>
-      <c r="J5" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="K5" s="23" t="s">
+      <c r="J5" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="K5" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="L5" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="M5" s="23" t="s">
+      <c r="L5" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="M5" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="N5" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="O5" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="P5" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q5" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="R5" s="23"/>
+      <c r="N5" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="O5" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="P5" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q5" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="R5" s="22"/>
     </row>
     <row r="6" spans="2:18" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="H6" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="24" t="s">
+      <c r="I6" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="J6" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="K6" s="23" t="s">
+      <c r="J6" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="K6" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="L6" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="M6" s="23" t="s">
+      <c r="L6" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="M6" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="N6" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="O6" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="P6" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q6" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="R6" s="23" t="s">
+      <c r="N6" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="O6" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="P6" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q6" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="R6" s="22" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="7" spans="2:18" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="24" t="s">
+      <c r="G7" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="24" t="s">
+      <c r="H7" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="24" t="s">
+      <c r="I7" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="J7" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="K7" s="23" t="s">
+      <c r="J7" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="K7" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="L7" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="M7" s="23" t="s">
+      <c r="L7" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="M7" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="N7" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="O7" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="P7" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q7" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="R7" s="23" t="s">
+      <c r="N7" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="O7" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="P7" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q7" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="R7" s="22" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="8" spans="2:18" ht="114" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="G8" s="26" t="s">
+      <c r="G8" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="H8" s="24" t="s">
+      <c r="H8" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="I8" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="J8" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="K8" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="L8" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="M8" s="23" t="s">
+      <c r="J8" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="K8" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="L8" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="M8" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="N8" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="O8" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="P8" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q8" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="R8" s="23"/>
-    </row>
-    <row r="9" spans="2:18" s="62" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="57" t="s">
+      <c r="N8" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="O8" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="P8" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q8" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="R8" s="22"/>
+    </row>
+    <row r="9" spans="2:18" s="61" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="58" t="s">
+      <c r="C9" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="59" t="s">
+      <c r="D9" s="58" t="s">
         <v>158</v>
       </c>
-      <c r="E9" s="60" t="s">
+      <c r="E9" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="60" t="s">
+      <c r="F9" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="61" t="s">
+      <c r="G9" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="61" t="s">
+      <c r="H9" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="I9" s="61" t="s">
+      <c r="I9" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="J9" s="58" t="s">
-        <v>152</v>
-      </c>
-      <c r="K9" s="58" t="s">
+      <c r="J9" s="57" t="s">
+        <v>152</v>
+      </c>
+      <c r="K9" s="57" t="s">
         <v>157</v>
       </c>
-      <c r="L9" s="58" t="s">
-        <v>152</v>
-      </c>
-      <c r="M9" s="58" t="s">
+      <c r="L9" s="57" t="s">
+        <v>152</v>
+      </c>
+      <c r="M9" s="57" t="s">
         <v>157</v>
       </c>
-      <c r="N9" s="58" t="s">
-        <v>152</v>
-      </c>
-      <c r="O9" s="58" t="s">
-        <v>152</v>
-      </c>
-      <c r="P9" s="58" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q9" s="58" t="s">
-        <v>152</v>
-      </c>
-      <c r="R9" s="58"/>
+      <c r="N9" s="57" t="s">
+        <v>152</v>
+      </c>
+      <c r="O9" s="57" t="s">
+        <v>152</v>
+      </c>
+      <c r="P9" s="57" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q9" s="57" t="s">
+        <v>152</v>
+      </c>
+      <c r="R9" s="57"/>
     </row>
     <row r="10" spans="2:18" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="F10" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="G10" s="24" t="s">
+      <c r="G10" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="H10" s="15" t="s">
+      <c r="H10" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="I10" s="26" t="s">
+      <c r="I10" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="J10" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="K10" s="23" t="s">
+      <c r="J10" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="K10" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="L10" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="M10" s="23" t="s">
+      <c r="L10" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="M10" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="N10" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="O10" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="P10" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q10" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="R10" s="23"/>
-    </row>
-    <row r="11" spans="2:18" s="29" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="27" t="s">
+      <c r="N10" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="O10" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="P10" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q10" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="R10" s="22"/>
+    </row>
+    <row r="11" spans="2:18" s="28" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="27" t="s">
         <v>60</v>
       </c>
       <c r="D11" s="71" t="s">
@@ -2360,25 +2379,25 @@
       <c r="I11" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="J11" s="29" t="s">
+      <c r="J11" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="K11" s="29">
+      <c r="K11" s="28">
         <v>15</v>
       </c>
-      <c r="L11" s="29">
+      <c r="L11" s="28">
         <v>20</v>
       </c>
-      <c r="M11" s="29">
+      <c r="M11" s="28">
         <f>L11*L12</f>
         <v>500000000</v>
       </c>
     </row>
-    <row r="12" spans="2:18" s="29" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="27" t="s">
+    <row r="12" spans="2:18" s="28" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="27" t="s">
         <v>66</v>
       </c>
       <c r="D12" s="71"/>
@@ -2387,409 +2406,415 @@
       <c r="G12" s="71"/>
       <c r="H12" s="64"/>
       <c r="I12" s="64"/>
-      <c r="J12" s="29" t="s">
+      <c r="J12" s="28" t="s">
         <v>161</v>
       </c>
-      <c r="K12" s="29">
+      <c r="K12" s="28">
         <v>1500000</v>
       </c>
-      <c r="L12" s="29">
+      <c r="L12" s="28">
         <v>25000000</v>
       </c>
-      <c r="M12" s="29">
+      <c r="M12" s="28">
         <f>K12*K11</f>
         <v>22500000</v>
       </c>
-      <c r="N12" s="29">
+      <c r="N12" s="28">
         <f>M12-M11</f>
         <v>-477500000</v>
       </c>
     </row>
     <row r="13" spans="2:18" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="E13" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="G13" s="24" t="s">
+      <c r="G13" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="24" t="s">
+      <c r="H13" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="I13" s="24" t="s">
+      <c r="I13" s="23" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="14" spans="2:18" ht="144" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="F14" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="G14" s="24" t="s">
+      <c r="G14" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="H14" s="24" t="s">
+      <c r="H14" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="I14" s="24" t="s">
+      <c r="I14" s="23" t="s">
         <v>72</v>
       </c>
+      <c r="J14" s="74" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="15" spans="2:18" ht="144" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="G15" s="24" t="s">
+      <c r="G15" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="H15" s="15" t="s">
+      <c r="H15" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="I15" s="26" t="s">
+      <c r="I15" s="25" t="s">
         <v>31</v>
       </c>
+      <c r="J15" s="6" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="16" spans="2:18" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="G16" s="26" t="s">
+      <c r="G16" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="H16" s="24" t="s">
+      <c r="H16" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="I16" s="24" t="s">
+      <c r="I16" s="23" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="153" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="32" t="s">
+      <c r="C17" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="D17" s="32" t="s">
+      <c r="D17" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E17" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F17" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="G17" s="24" t="s">
+      <c r="G17" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="H17" s="24" t="s">
+      <c r="H17" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="I17" s="24" t="s">
+      <c r="I17" s="23" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="2:9" s="29" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="27" t="s">
+    <row r="18" spans="2:9" s="28" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="D18" s="33" t="s">
+      <c r="D18" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="E18" s="34" t="s">
+      <c r="E18" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="F18" s="35" t="s">
+      <c r="F18" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="G18" s="36" t="s">
+      <c r="G18" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="H18" s="36" t="s">
+      <c r="H18" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="I18" s="36" t="s">
+      <c r="I18" s="35" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="2:9" s="29" customFormat="1" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="37" t="s">
+    <row r="19" spans="2:9" s="28" customFormat="1" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="D19" s="37" t="s">
+      <c r="D19" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="E19" s="37" t="s">
+      <c r="E19" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="F19" s="34" t="s">
+      <c r="F19" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="G19" s="36" t="s">
+      <c r="G19" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="H19" s="36" t="s">
+      <c r="H19" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="I19" s="26" t="s">
+      <c r="I19" s="25" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="2:9" s="29" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="37" t="s">
+    <row r="20" spans="2:9" s="28" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="C20" s="37" t="s">
+      <c r="C20" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="D20" s="37" t="s">
+      <c r="D20" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="E20" s="37" t="s">
+      <c r="E20" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="F20" s="37" t="s">
+      <c r="F20" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="G20" s="36" t="s">
+      <c r="G20" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="H20" s="36" t="s">
+      <c r="H20" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="I20" s="26" t="s">
+      <c r="I20" s="25" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="21" spans="2:9" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="C21" s="38" t="s">
+      <c r="C21" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="D21" s="39" t="s">
+      <c r="D21" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="E21" s="40" t="s">
+      <c r="E21" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="F21" s="41" t="s">
+      <c r="F21" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="G21" s="24" t="s">
+      <c r="G21" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="H21" s="15" t="s">
+      <c r="H21" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="I21" s="26" t="s">
+      <c r="I21" s="25" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="2:9" s="29" customFormat="1" ht="137.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="42" t="s">
+    <row r="22" spans="2:9" s="28" customFormat="1" ht="137.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="41" t="s">
         <v>119</v>
       </c>
-      <c r="C22" s="32" t="s">
+      <c r="C22" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="D22" s="43" t="s">
+      <c r="D22" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="E22" s="40" t="s">
+      <c r="E22" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="F22" s="37" t="s">
+      <c r="F22" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="G22" s="36" t="s">
+      <c r="G22" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="H22" s="32" t="s">
+      <c r="H22" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="I22" s="43" t="s">
+      <c r="I22" s="42" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="23" spans="2:9" ht="137.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="44" t="s">
+      <c r="B23" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="D23" s="26" t="s">
+      <c r="D23" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="E23" s="26" t="s">
+      <c r="E23" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="F23" s="17" t="s">
+      <c r="F23" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="G23" s="24" t="s">
+      <c r="G23" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="H23" s="15" t="s">
+      <c r="H23" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="I23" s="26" t="s">
+      <c r="I23" s="25" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="2:9" s="29" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="45" t="s">
+    <row r="24" spans="2:9" s="28" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="C24" s="32" t="s">
+      <c r="C24" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="D24" s="36" t="s">
+      <c r="D24" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="E24" s="35" t="s">
+      <c r="E24" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="F24" s="35" t="s">
+      <c r="F24" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="G24" s="36" t="s">
+      <c r="G24" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="H24" s="36" t="s">
+      <c r="H24" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="I24" s="36" t="s">
+      <c r="I24" s="35" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="2:9" s="29" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="22" t="s">
+    <row r="25" spans="2:9" s="28" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="C25" s="32" t="s">
+      <c r="C25" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="D25" s="26" t="s">
+      <c r="D25" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="E25" s="36" t="s">
+      <c r="E25" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="F25" s="35" t="s">
+      <c r="F25" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="G25" s="36" t="s">
+      <c r="G25" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="H25" s="36" t="s">
+      <c r="H25" s="35" t="s">
         <v>140</v>
       </c>
-      <c r="I25" s="24" t="s">
+      <c r="I25" s="23" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="26" spans="2:9" ht="102.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="46" t="s">
+      <c r="B26" s="45" t="s">
         <v>141</v>
       </c>
-      <c r="C26" s="47" t="s">
+      <c r="C26" s="46" t="s">
         <v>142</v>
       </c>
-      <c r="D26" s="26" t="s">
+      <c r="D26" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="E26" s="43" t="s">
+      <c r="E26" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="F26" s="48" t="s">
+      <c r="F26" s="47" t="s">
         <v>145</v>
       </c>
-      <c r="G26" s="49" t="s">
+      <c r="G26" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="H26" s="49" t="s">
+      <c r="H26" s="48" t="s">
         <v>146</v>
       </c>
-      <c r="I26" s="49" t="s">
+      <c r="I26" s="48" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F34" s="50"/>
+      <c r="F34" s="49"/>
     </row>
     <row r="35" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D35" s="51"/>
-      <c r="F35" s="50"/>
+      <c r="D35" s="50"/>
+      <c r="F35" s="49"/>
     </row>
     <row r="36" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F36" s="50"/>
+      <c r="F36" s="49"/>
     </row>
     <row r="37" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F37" s="50"/>
+      <c r="F37" s="49"/>
     </row>
     <row r="38" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F38" s="52"/>
+      <c r="F38" s="51"/>
     </row>
     <row r="40" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F40" s="53"/>
+      <c r="F40" s="52"/>
     </row>
     <row r="41" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F41" s="52"/>
+      <c r="F41" s="51"/>
     </row>
   </sheetData>
   <autoFilter ref="B2:I26">
@@ -2820,7 +2845,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2831,40 +2856,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="63" t="s">
         <v>162</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="63" t="s">
         <v>163</v>
       </c>
-      <c r="C1" s="72">
+      <c r="C1" s="63">
         <v>2012</v>
       </c>
-      <c r="D1" s="72">
+      <c r="D1" s="63">
         <v>2013</v>
       </c>
-      <c r="E1" s="72">
+      <c r="E1" s="63">
         <v>2014</v>
       </c>
-      <c r="F1" s="72" t="s">
+      <c r="F1" s="63" t="s">
         <v>164</v>
       </c>
-      <c r="G1" s="72" t="s">
+      <c r="G1" s="63" t="s">
         <v>165</v>
       </c>
-      <c r="H1" s="72" t="s">
+      <c r="H1" s="63" t="s">
         <v>166</v>
       </c>
-      <c r="I1" s="72" t="s">
+      <c r="I1" s="63" t="s">
         <v>167</v>
       </c>
-      <c r="J1" s="72" t="s">
+      <c r="J1" s="63" t="s">
         <v>168</v>
       </c>
-      <c r="K1" s="72" t="s">
+      <c r="K1" s="63" t="s">
         <v>169</v>
       </c>
-      <c r="L1" s="72" t="s">
+      <c r="L1" s="63" t="s">
         <v>170</v>
       </c>
     </row>
@@ -3953,15 +3978,15 @@
         <f t="shared" ref="I26" si="9">SUM(I2:I25)</f>
         <v>0.99999999999999967</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="72">
         <f t="shared" ref="J26" si="10">SUM(J2:J25)</f>
         <v>0.40073400270852677</v>
       </c>
-      <c r="K26">
+      <c r="K26" s="72">
         <f t="shared" ref="K26" si="11">SUM(K2:K25)</f>
         <v>0.4171276762746271</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="72">
         <f t="shared" ref="L26" si="12">SUM(L2:L25)</f>
         <v>0.36706596430163779</v>
       </c>

</xml_diff>

<commit_message>
finaliza jornada QH 09-12-2014
</commit_message>
<xml_diff>
--- a/Documentacion/indicadores revisión junio 11 2014.xlsx
+++ b/Documentacion/indicadores revisión junio 11 2014.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6435"/>
   </bookViews>
   <sheets>
     <sheet name="Ajustes" sheetId="1" r:id="rId1"/>
@@ -852,207 +852,207 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">Exportaciones agropecuarias NO tradicionales (Banano, Flores, café) (Xant1) -Total exportaciones Agrícolas (TXA)
+</t>
+  </si>
+  <si>
+    <t>Donde XAnt = exportaciones no tradicionales y TXA =  total exportaciones agrícolas</t>
+  </si>
+  <si>
+    <t>Las exportaciones agropecuarias no tradicionales en relación al dinamismo de las exportaciones agropecuarias totales.</t>
+  </si>
+  <si>
+    <t>Identificar el crecimiento real del sector agrícola sin los productos que ya están posicionados en el exterior.</t>
+  </si>
+  <si>
+    <t>Consumo aparente</t>
+  </si>
+  <si>
+    <t>((Producción nacional (P) + importaciones (M) - exportaciones (X)  )</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   Donde P = producción, M= importaciones y X = exportaciones.  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Las variables se deben calcular con respecto a VOL. (Cantidades NO valores en $.</t>
+    </r>
+  </si>
+  <si>
+    <t>Insumo esencial para el cálculo de la autosuficiencia alimentaria de un bien x o de todo el sector agrícola</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Es un aproximado del consumo que tiene el país respecto a un bien x
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>AGRONET solo sector agrícola  y Quintero Hermanos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coeficiente de Autosuficiencia Alimentaria </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Producción (en VOL-Cantidades) / Consumo aparente
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Donde C = consumo, P = producción </t>
+  </si>
+  <si>
+    <t>Muestra el grado de dependencia o independencia que se tiene frente a las importaciones de un bien x,  para abastecer el mercado nacional</t>
+  </si>
+  <si>
+    <t>Establece cuanto del consumo aparente se cubre con producción nacional</t>
+  </si>
+  <si>
+    <t>AGRONET solo sector agrícola,  se excluye partidas de las cuales no haya información y Quintero Hermanos</t>
+  </si>
+  <si>
+    <t>Posición de Colombia entre los proveedores de un producto específico a un mercado de destino.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definición del puesto que ocupa Colombia entre los proveedores de un producto específico en un mercado de destino (conteo del numero de proveedores de un producto a un mercado de destino)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              Conteo de los países proveedores y posición de Colombia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ubicación de Colombia como proveedor de un producto en un mercado  mercado específico.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mide el posicionamiento de Colombia en las importaciones de un producto de un mercado específico. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Quintero her. - DANE                               </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DATOS REQUERIDOS:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">      Exportaciones agropecuarias de COL x part. e Importaciones de un socio comercial por part.</t>
+    </r>
+  </si>
+  <si>
+    <t>requiere pais</t>
+  </si>
+  <si>
+    <t>requiere peso neto</t>
+  </si>
+  <si>
+    <t>requiere producto</t>
+  </si>
+  <si>
+    <t>impo</t>
+  </si>
+  <si>
+    <t>expo</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>Requiere valor fob</t>
+  </si>
+  <si>
+    <t>adicional</t>
+  </si>
+  <si>
+    <t>producccion</t>
+  </si>
+  <si>
+    <t>requiere empresas</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>donde Xij : Exportaciones del bien i realizadas por el país j, Mij : Importaciones del bien i realizadas por el país j, Xin: Exportaciones del bien i realizadas por COLOMBIA al resto del mundo o un mercado específico.</t>
+  </si>
+  <si>
+    <t>Requiere posicion completa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">productos </t>
+  </si>
+  <si>
+    <t>importaciones</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>id_capitulo</t>
+  </si>
+  <si>
+    <t>valorfob</t>
+  </si>
+  <si>
+    <t>part 2012</t>
+  </si>
+  <si>
+    <t>part 2013</t>
+  </si>
+  <si>
+    <t>part 2014</t>
+  </si>
+  <si>
+    <t>part 2012 Exp 2</t>
+  </si>
+  <si>
+    <t>part 2013 Exp 2</t>
+  </si>
+  <si>
+    <t>part 2014 Exp 2</t>
+  </si>
+  <si>
+    <t>aclarar sector minero energetico</t>
+  </si>
+  <si>
+    <t>definir</t>
+  </si>
+  <si>
     <t xml:space="preserve">Relación del crecimiento promedio anual de las exportaciones agropecuarias  y agroindustriales no tradicionales  y el crecimiento promedio anual del total de las exportaciones agropecuarias y agroindustriales.
  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exportaciones agropecuarias NO tradicionales (Banano, Flores, café) (Xant1) -Total exportaciones Agrícolas (TXA)
-</t>
-  </si>
-  <si>
-    <t>Donde XAnt = exportaciones no tradicionales y TXA =  total exportaciones agrícolas</t>
-  </si>
-  <si>
-    <t>Las exportaciones agropecuarias no tradicionales en relación al dinamismo de las exportaciones agropecuarias totales.</t>
-  </si>
-  <si>
-    <t>Identificar el crecimiento real del sector agrícola sin los productos que ya están posicionados en el exterior.</t>
-  </si>
-  <si>
-    <t>Consumo aparente</t>
-  </si>
-  <si>
-    <t>((Producción nacional (P) + importaciones (M) - exportaciones (X)  )</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">   Donde P = producción, M= importaciones y X = exportaciones.  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Las variables se deben calcular con respecto a VOL. (Cantidades NO valores en $.</t>
-    </r>
-  </si>
-  <si>
-    <t>Insumo esencial para el cálculo de la autosuficiencia alimentaria de un bien x o de todo el sector agrícola</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Es un aproximado del consumo que tiene el país respecto a un bien x
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <t>AGRONET solo sector agrícola  y Quintero Hermanos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coeficiente de Autosuficiencia Alimentaria </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Producción (en VOL-Cantidades) / Consumo aparente
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Donde C = consumo, P = producción </t>
-  </si>
-  <si>
-    <t>Muestra el grado de dependencia o independencia que se tiene frente a las importaciones de un bien x,  para abastecer el mercado nacional</t>
-  </si>
-  <si>
-    <t>Establece cuanto del consumo aparente se cubre con producción nacional</t>
-  </si>
-  <si>
-    <t>AGRONET solo sector agrícola,  se excluye partidas de las cuales no haya información y Quintero Hermanos</t>
-  </si>
-  <si>
-    <t>Posición de Colombia entre los proveedores de un producto específico a un mercado de destino.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Definición del puesto que ocupa Colombia entre los proveedores de un producto específico en un mercado de destino (conteo del numero de proveedores de un producto a un mercado de destino)
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">              Conteo de los países proveedores y posición de Colombia </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ubicación de Colombia como proveedor de un producto en un mercado  mercado específico.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mide el posicionamiento de Colombia en las importaciones de un producto de un mercado específico. </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Quintero her. - DANE                               </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DATOS REQUERIDOS:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">      Exportaciones agropecuarias de COL x part. e Importaciones de un socio comercial por part.</t>
-    </r>
-  </si>
-  <si>
-    <t>requiere pais</t>
-  </si>
-  <si>
-    <t>requiere peso neto</t>
-  </si>
-  <si>
-    <t>requiere producto</t>
-  </si>
-  <si>
-    <t>impo</t>
-  </si>
-  <si>
-    <t>expo</t>
-  </si>
-  <si>
-    <t>SI</t>
-  </si>
-  <si>
-    <t>Requiere valor fob</t>
-  </si>
-  <si>
-    <t>adicional</t>
-  </si>
-  <si>
-    <t>producccion</t>
-  </si>
-  <si>
-    <t>requiere empresas</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>donde Xij : Exportaciones del bien i realizadas por el país j, Mij : Importaciones del bien i realizadas por el país j, Xin: Exportaciones del bien i realizadas por COLOMBIA al resto del mundo o un mercado específico.</t>
-  </si>
-  <si>
-    <t>Requiere posicion completa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">productos </t>
-  </si>
-  <si>
-    <t>importaciones</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>id_capitulo</t>
-  </si>
-  <si>
-    <t>valorfob</t>
-  </si>
-  <si>
-    <t>part 2012</t>
-  </si>
-  <si>
-    <t>part 2013</t>
-  </si>
-  <si>
-    <t>part 2014</t>
-  </si>
-  <si>
-    <t>part 2012 Exp 2</t>
-  </si>
-  <si>
-    <t>part 2013 Exp 2</t>
-  </si>
-  <si>
-    <t>part 2014 Exp 2</t>
-  </si>
-  <si>
-    <t>aclarar sector minero energetico</t>
-  </si>
-  <si>
-    <t>definir</t>
   </si>
 </sst>
 </file>
@@ -1060,9 +1060,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.000%"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -1339,10 +1339,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1461,9 +1461,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1476,16 +1473,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1497,32 +1494,25 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1547,9 +1537,22 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -1878,10 +1881,10 @@
   <dimension ref="B1:R41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomRight" activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1903,10 +1906,10 @@
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="65"/>
+      <c r="D2" s="61"/>
       <c r="E2" s="8" t="s">
         <v>2</v>
       </c>
@@ -1922,36 +1925,36 @@
       <c r="I2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="51" t="s">
+      <c r="J2" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="K2" s="50" t="s">
+        <v>155</v>
+      </c>
+      <c r="L2" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="M2" s="50" t="s">
+        <v>158</v>
+      </c>
+      <c r="N2" s="50" t="s">
         <v>147</v>
       </c>
-      <c r="K2" s="51" t="s">
-        <v>156</v>
-      </c>
-      <c r="L2" s="51" t="s">
+      <c r="O2" s="50" t="s">
+        <v>152</v>
+      </c>
+      <c r="P2" s="50" t="s">
         <v>149</v>
       </c>
-      <c r="M2" s="51" t="s">
-        <v>159</v>
-      </c>
-      <c r="N2" s="51" t="s">
-        <v>148</v>
-      </c>
-      <c r="O2" s="51" t="s">
+      <c r="Q2" s="50" t="s">
+        <v>150</v>
+      </c>
+      <c r="R2" s="50" t="s">
         <v>153</v>
       </c>
-      <c r="P2" s="51" t="s">
-        <v>150</v>
-      </c>
-      <c r="Q2" s="51" t="s">
-        <v>151</v>
-      </c>
-      <c r="R2" s="51" t="s">
-        <v>154</v>
-      </c>
     </row>
     <row r="3" spans="2:18" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="51" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="11" t="s">
@@ -1963,46 +1966,46 @@
       <c r="E3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="66" t="s">
+      <c r="F3" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="68" t="s">
+      <c r="G3" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="68" t="s">
+      <c r="H3" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="70" t="s">
+      <c r="I3" s="66" t="s">
         <v>14</v>
       </c>
       <c r="J3" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K3" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L3" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M3" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N3" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="O3" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P3" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q3" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="R3" s="21"/>
     </row>
     <row r="4" spans="2:18" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="52" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="14" t="s">
@@ -2014,38 +2017,38 @@
       <c r="E4" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="67"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
       <c r="J4" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K4" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L4" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M4" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N4" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="O4" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P4" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q4" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="R4" s="21"/>
     </row>
     <row r="5" spans="2:18" ht="104.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="53" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="14" t="s">
@@ -2060,32 +2063,32 @@
       <c r="F5" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
       <c r="J5" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K5" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L5" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M5" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N5" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="O5" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P5" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q5" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="R5" s="21"/>
     </row>
@@ -2115,31 +2118,31 @@
         <v>31</v>
       </c>
       <c r="J6" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K6" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L6" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M6" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N6" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="O6" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P6" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q6" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="R6" s="21" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="2:18" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2168,35 +2171,35 @@
         <v>31</v>
       </c>
       <c r="J7" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K7" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L7" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M7" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N7" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="O7" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P7" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q7" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="R7" s="21" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="2:18" ht="114" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="60" t="s">
+      <c r="B8" s="53" t="s">
         <v>39</v>
       </c>
       <c r="C8" s="23" t="s">
@@ -2221,84 +2224,84 @@
         <v>46</v>
       </c>
       <c r="J8" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K8" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L8" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M8" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="N8" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="O8" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="P8" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q8" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="R8" s="21"/>
+    </row>
+    <row r="9" spans="2:18" s="27" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="58" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="59" t="s">
         <v>157</v>
       </c>
-      <c r="N8" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="O8" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="P8" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q8" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="R8" s="21"/>
-    </row>
-    <row r="9" spans="2:18" s="59" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="54" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="55" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="56" t="s">
-        <v>158</v>
-      </c>
-      <c r="E9" s="57" t="s">
+      <c r="E9" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="57" t="s">
+      <c r="F9" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="58" t="s">
+      <c r="G9" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="58" t="s">
+      <c r="H9" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="I9" s="58" t="s">
+      <c r="I9" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="J9" s="55" t="s">
-        <v>152</v>
-      </c>
-      <c r="K9" s="55" t="s">
-        <v>157</v>
-      </c>
-      <c r="L9" s="55" t="s">
-        <v>152</v>
-      </c>
-      <c r="M9" s="55" t="s">
-        <v>157</v>
-      </c>
-      <c r="N9" s="55" t="s">
-        <v>152</v>
-      </c>
-      <c r="O9" s="55" t="s">
-        <v>152</v>
-      </c>
-      <c r="P9" s="55" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q9" s="55" t="s">
-        <v>152</v>
-      </c>
-      <c r="R9" s="55"/>
+      <c r="J9" s="58" t="s">
+        <v>151</v>
+      </c>
+      <c r="K9" s="58" t="s">
+        <v>156</v>
+      </c>
+      <c r="L9" s="58" t="s">
+        <v>151</v>
+      </c>
+      <c r="M9" s="58" t="s">
+        <v>156</v>
+      </c>
+      <c r="N9" s="58" t="s">
+        <v>151</v>
+      </c>
+      <c r="O9" s="58" t="s">
+        <v>151</v>
+      </c>
+      <c r="P9" s="58" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q9" s="58" t="s">
+        <v>151</v>
+      </c>
+      <c r="R9" s="58"/>
     </row>
     <row r="10" spans="2:18" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="53" t="s">
+      <c r="B10" s="52" t="s">
         <v>52</v>
       </c>
       <c r="C10" s="14" t="s">
@@ -2323,28 +2326,28 @@
         <v>31</v>
       </c>
       <c r="J10" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K10" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L10" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M10" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N10" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="O10" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P10" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q10" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="R10" s="21"/>
     </row>
@@ -2355,26 +2358,26 @@
       <c r="C11" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="71" t="s">
+      <c r="D11" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="64" t="s">
+      <c r="E11" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="F11" s="71" t="s">
+      <c r="F11" s="67" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="71" t="s">
+      <c r="G11" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="H11" s="64" t="s">
+      <c r="H11" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="I11" s="64" t="s">
+      <c r="I11" s="60" t="s">
         <v>31</v>
       </c>
       <c r="J11" s="27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K11" s="27">
         <v>15</v>
@@ -2394,14 +2397,14 @@
       <c r="C12" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="71"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="71"/>
-      <c r="H12" s="64"/>
-      <c r="I12" s="64"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="60"/>
       <c r="J12" s="27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K12" s="27">
         <v>1500000</v>
@@ -2419,7 +2422,7 @@
       </c>
     </row>
     <row r="13" spans="2:18" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="53" t="s">
+      <c r="B13" s="52" t="s">
         <v>67</v>
       </c>
       <c r="C13" s="14" t="s">
@@ -2445,7 +2448,7 @@
       </c>
     </row>
     <row r="14" spans="2:18" ht="144" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="53" t="s">
+      <c r="B14" s="52" t="s">
         <v>73</v>
       </c>
       <c r="C14" s="14" t="s">
@@ -2469,12 +2472,12 @@
       <c r="I14" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="J14" s="63" t="s">
-        <v>171</v>
+      <c r="J14" s="56" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="2:18" ht="144" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="60" t="s">
+      <c r="B15" s="53" t="s">
         <v>80</v>
       </c>
       <c r="C15" s="14" t="s">
@@ -2499,11 +2502,11 @@
         <v>31</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16" spans="2:18" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="B16" s="60" t="s">
+      <c r="B16" s="53" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="29" t="s">
@@ -2529,7 +2532,7 @@
       </c>
     </row>
     <row r="17" spans="2:9" ht="153" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="53" t="s">
+      <c r="B17" s="52" t="s">
         <v>91</v>
       </c>
       <c r="C17" s="30" t="s">
@@ -2684,53 +2687,53 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="137.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="42" t="s">
+    <row r="23" spans="2:9" s="73" customFormat="1" ht="137.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="68" t="s">
+        <v>172</v>
+      </c>
+      <c r="C23" s="69" t="s">
         <v>124</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="D23" s="70" t="s">
         <v>125</v>
       </c>
-      <c r="D23" s="24" t="s">
+      <c r="E23" s="70" t="s">
         <v>126</v>
       </c>
-      <c r="E23" s="24" t="s">
+      <c r="F23" s="71" t="s">
         <v>127</v>
       </c>
-      <c r="F23" s="16" t="s">
+      <c r="G23" s="72" t="s">
+        <v>57</v>
+      </c>
+      <c r="H23" s="69" t="s">
+        <v>58</v>
+      </c>
+      <c r="I23" s="70" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" s="27" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="42" t="s">
         <v>128</v>
       </c>
-      <c r="G23" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="H23" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="I23" s="24" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" s="27" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="43" t="s">
+      <c r="C24" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="C24" s="30" t="s">
+      <c r="D24" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="D24" s="34" t="s">
+      <c r="E24" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="E24" s="33" t="s">
+      <c r="F24" s="33" t="s">
         <v>132</v>
-      </c>
-      <c r="F24" s="33" t="s">
-        <v>133</v>
       </c>
       <c r="G24" s="34" t="s">
         <v>12</v>
       </c>
       <c r="H24" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I24" s="34" t="s">
         <v>31</v>
@@ -2738,77 +2741,77 @@
     </row>
     <row r="25" spans="2:9" s="27" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="C25" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="C25" s="30" t="s">
+      <c r="D25" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="D25" s="24" t="s">
+      <c r="E25" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="E25" s="34" t="s">
+      <c r="F25" s="33" t="s">
         <v>138</v>
-      </c>
-      <c r="F25" s="33" t="s">
-        <v>139</v>
       </c>
       <c r="G25" s="34" t="s">
         <v>12</v>
       </c>
       <c r="H25" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I25" s="22" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="26" spans="2:9" ht="102.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="72" t="s">
+      <c r="B26" s="57" t="s">
+        <v>140</v>
+      </c>
+      <c r="C26" s="43" t="s">
         <v>141</v>
       </c>
-      <c r="C26" s="44" t="s">
+      <c r="D26" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="D26" s="24" t="s">
+      <c r="E26" s="41" t="s">
         <v>143</v>
       </c>
-      <c r="E26" s="41" t="s">
+      <c r="F26" s="44" t="s">
         <v>144</v>
       </c>
-      <c r="F26" s="45" t="s">
+      <c r="G26" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="H26" s="45" t="s">
         <v>145</v>
       </c>
-      <c r="G26" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="H26" s="46" t="s">
-        <v>146</v>
-      </c>
-      <c r="I26" s="46" t="s">
+      <c r="I26" s="45" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F34" s="47"/>
+      <c r="F34" s="46"/>
     </row>
     <row r="35" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D35" s="48"/>
-      <c r="F35" s="47"/>
+      <c r="D35" s="47"/>
+      <c r="F35" s="46"/>
     </row>
     <row r="36" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F36" s="47"/>
+      <c r="F36" s="46"/>
     </row>
     <row r="37" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F37" s="47"/>
+      <c r="F37" s="46"/>
     </row>
     <row r="38" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F38" s="49"/>
+      <c r="F38" s="48"/>
     </row>
     <row r="40" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F40" s="50"/>
+      <c r="F40" s="49"/>
     </row>
     <row r="41" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F41" s="49"/>
+      <c r="F41" s="48"/>
     </row>
   </sheetData>
   <autoFilter ref="B2:I26">
@@ -2839,7 +2842,7 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="L2" sqref="L2:L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2850,41 +2853,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="54" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="54" t="s">
         <v>162</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="C1" s="54">
+        <v>2012</v>
+      </c>
+      <c r="D1" s="54">
+        <v>2013</v>
+      </c>
+      <c r="E1" s="54">
+        <v>2014</v>
+      </c>
+      <c r="F1" s="54" t="s">
         <v>163</v>
       </c>
-      <c r="C1" s="61">
-        <v>2012</v>
-      </c>
-      <c r="D1" s="61">
-        <v>2013</v>
-      </c>
-      <c r="E1" s="61">
-        <v>2014</v>
-      </c>
-      <c r="F1" s="61" t="s">
+      <c r="G1" s="54" t="s">
         <v>164</v>
       </c>
-      <c r="G1" s="61" t="s">
+      <c r="H1" s="54" t="s">
         <v>165</v>
       </c>
-      <c r="H1" s="61" t="s">
+      <c r="I1" s="54" t="s">
         <v>166</v>
       </c>
-      <c r="I1" s="61" t="s">
+      <c r="J1" s="54" t="s">
         <v>167</v>
       </c>
-      <c r="J1" s="61" t="s">
+      <c r="K1" s="54" t="s">
         <v>168</v>
       </c>
-      <c r="K1" s="61" t="s">
+      <c r="L1" s="54" t="s">
         <v>169</v>
-      </c>
-      <c r="L1" s="61" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -3976,15 +3979,15 @@
         <f t="shared" ref="I26" si="9">SUM(I2:I25)</f>
         <v>0.99999999999999967</v>
       </c>
-      <c r="J26" s="62">
+      <c r="J26" s="55">
         <f t="shared" ref="J26" si="10">SUM(J2:J25)</f>
         <v>0.40073400270852677</v>
       </c>
-      <c r="K26" s="62">
+      <c r="K26" s="55">
         <f t="shared" ref="K26" si="11">SUM(K2:K25)</f>
         <v>0.4171276762746271</v>
       </c>
-      <c r="L26" s="62">
+      <c r="L26" s="55">
         <f t="shared" ref="L26" si="12">SUM(L2:L25)</f>
         <v>0.36706596430163779</v>
       </c>

</xml_diff>

<commit_message>
finaliza jornada QH 16-12-2014
</commit_message>
<xml_diff>
--- a/Documentacion/indicadores revisión junio 11 2014.xlsx
+++ b/Documentacion/indicadores revisión junio 11 2014.xlsx
@@ -1075,9 +1075,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.000%"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -1354,10 +1354,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1427,9 +1427,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1470,9 +1467,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1488,16 +1482,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1515,7 +1509,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1528,25 +1522,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1568,7 +1556,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -1897,10 +1887,10 @@
   <dimension ref="B1:R41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1922,10 +1912,10 @@
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="67" t="s">
+      <c r="C2" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="67"/>
+      <c r="D2" s="63"/>
       <c r="E2" s="8" t="s">
         <v>2</v>
       </c>
@@ -1941,36 +1931,36 @@
       <c r="I2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="50" t="s">
+      <c r="J2" s="48" t="s">
         <v>146</v>
       </c>
-      <c r="K2" s="50" t="s">
+      <c r="K2" s="48" t="s">
         <v>155</v>
       </c>
-      <c r="L2" s="50" t="s">
+      <c r="L2" s="48" t="s">
         <v>148</v>
       </c>
-      <c r="M2" s="50" t="s">
+      <c r="M2" s="48" t="s">
         <v>158</v>
       </c>
-      <c r="N2" s="50" t="s">
+      <c r="N2" s="48" t="s">
         <v>147</v>
       </c>
-      <c r="O2" s="50" t="s">
+      <c r="O2" s="48" t="s">
         <v>152</v>
       </c>
-      <c r="P2" s="50" t="s">
+      <c r="P2" s="48" t="s">
         <v>149</v>
       </c>
-      <c r="Q2" s="50" t="s">
+      <c r="Q2" s="48" t="s">
         <v>150</v>
       </c>
-      <c r="R2" s="50" t="s">
+      <c r="R2" s="48" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="3" spans="2:18" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="49" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="11" t="s">
@@ -1982,16 +1972,16 @@
       <c r="E3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="68" t="s">
+      <c r="F3" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="70" t="s">
+      <c r="G3" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="70" t="s">
+      <c r="H3" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="72" t="s">
+      <c r="I3" s="68" t="s">
         <v>14</v>
       </c>
       <c r="J3" s="21" t="s">
@@ -2021,7 +2011,7 @@
       <c r="R3" s="21"/>
     </row>
     <row r="4" spans="2:18" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="50" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="14" t="s">
@@ -2033,10 +2023,10 @@
       <c r="E4" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="69"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
       <c r="J4" s="21" t="s">
         <v>151</v>
       </c>
@@ -2064,7 +2054,7 @@
       <c r="R4" s="21"/>
     </row>
     <row r="5" spans="2:18" ht="104.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="51" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="14" t="s">
@@ -2079,9 +2069,9 @@
       <c r="F5" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
       <c r="J5" s="21" t="s">
         <v>151</v>
       </c>
@@ -2215,7 +2205,7 @@
       </c>
     </row>
     <row r="8" spans="2:18" ht="114" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="51" t="s">
         <v>39</v>
       </c>
       <c r="C8" s="23" t="s">
@@ -2265,59 +2255,59 @@
       </c>
       <c r="R8" s="21"/>
     </row>
-    <row r="9" spans="2:18" s="27" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:18" s="26" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="58" t="s">
+      <c r="C9" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="59" t="s">
+      <c r="D9" s="57" t="s">
         <v>157</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="33" t="s">
+      <c r="F9" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="34" t="s">
+      <c r="G9" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="34" t="s">
+      <c r="H9" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="I9" s="34" t="s">
+      <c r="I9" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="J9" s="58" t="s">
-        <v>151</v>
-      </c>
-      <c r="K9" s="58" t="s">
+      <c r="J9" s="56" t="s">
+        <v>151</v>
+      </c>
+      <c r="K9" s="56" t="s">
         <v>156</v>
       </c>
-      <c r="L9" s="58" t="s">
-        <v>151</v>
-      </c>
-      <c r="M9" s="58" t="s">
+      <c r="L9" s="56" t="s">
+        <v>151</v>
+      </c>
+      <c r="M9" s="56" t="s">
         <v>156</v>
       </c>
-      <c r="N9" s="58" t="s">
-        <v>151</v>
-      </c>
-      <c r="O9" s="58" t="s">
-        <v>151</v>
-      </c>
-      <c r="P9" s="58" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q9" s="58" t="s">
-        <v>151</v>
-      </c>
-      <c r="R9" s="58"/>
+      <c r="N9" s="56" t="s">
+        <v>151</v>
+      </c>
+      <c r="O9" s="56" t="s">
+        <v>151</v>
+      </c>
+      <c r="P9" s="56" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q9" s="56" t="s">
+        <v>151</v>
+      </c>
+      <c r="R9" s="56"/>
     </row>
     <row r="10" spans="2:18" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="50" t="s">
         <v>52</v>
       </c>
       <c r="C10" s="14" t="s">
@@ -2367,78 +2357,78 @@
       </c>
       <c r="R10" s="21"/>
     </row>
-    <row r="11" spans="2:18" s="27" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="53" t="s">
+    <row r="11" spans="2:18" s="26" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="73" t="s">
+      <c r="D11" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="66" t="s">
+      <c r="E11" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="F11" s="73" t="s">
+      <c r="F11" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="73" t="s">
+      <c r="G11" s="69" t="s">
         <v>64</v>
       </c>
-      <c r="H11" s="66" t="s">
+      <c r="H11" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="I11" s="66" t="s">
+      <c r="I11" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="J11" s="27" t="s">
+      <c r="J11" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="K11" s="27">
+      <c r="K11" s="26">
         <v>15</v>
       </c>
-      <c r="L11" s="27">
+      <c r="L11" s="26">
         <v>20</v>
       </c>
-      <c r="M11" s="27">
+      <c r="M11" s="26">
         <f>L11*L12</f>
         <v>500000000</v>
       </c>
     </row>
-    <row r="12" spans="2:18" s="27" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="53" t="s">
+    <row r="12" spans="2:18" s="26" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="73"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="73"/>
-      <c r="H12" s="66"/>
-      <c r="I12" s="66"/>
-      <c r="J12" s="27" t="s">
+      <c r="D12" s="69"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="62"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="K12" s="27">
+      <c r="K12" s="26">
         <v>1500000</v>
       </c>
-      <c r="L12" s="27">
+      <c r="L12" s="26">
         <v>25000000</v>
       </c>
-      <c r="M12" s="27">
+      <c r="M12" s="26">
         <f>K12*K11</f>
         <v>22500000</v>
       </c>
-      <c r="N12" s="27">
+      <c r="N12" s="26">
         <f>M12-M11</f>
         <v>-477500000</v>
       </c>
     </row>
     <row r="13" spans="2:18" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="52" t="s">
+      <c r="B13" s="50" t="s">
         <v>67</v>
       </c>
       <c r="C13" s="14" t="s">
@@ -2447,7 +2437,7 @@
       <c r="D13" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="28" t="s">
+      <c r="E13" s="27" t="s">
         <v>70</v>
       </c>
       <c r="F13" s="16" t="s">
@@ -2464,7 +2454,7 @@
       </c>
     </row>
     <row r="14" spans="2:18" ht="144" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="52" t="s">
+      <c r="B14" s="50" t="s">
         <v>73</v>
       </c>
       <c r="C14" s="14" t="s">
@@ -2488,12 +2478,12 @@
       <c r="I14" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="J14" s="56" t="s">
+      <c r="J14" s="54" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="15" spans="2:18" ht="144" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="53" t="s">
+      <c r="B15" s="51" t="s">
         <v>80</v>
       </c>
       <c r="C15" s="14" t="s">
@@ -2522,10 +2512,10 @@
       </c>
     </row>
     <row r="16" spans="2:18" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="B16" s="53" t="s">
+      <c r="B16" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="28" t="s">
         <v>86</v>
       </c>
       <c r="D16" s="14" t="s">
@@ -2548,13 +2538,13 @@
       </c>
     </row>
     <row r="17" spans="2:9" ht="153" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="52" t="s">
+      <c r="B17" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="29" t="s">
         <v>93</v>
       </c>
       <c r="E17" s="16" t="s">
@@ -2573,78 +2563,78 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="2:9" s="27" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="25" t="s">
+    <row r="18" spans="2:9" s="26" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="D18" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="F18" s="33" t="s">
+      <c r="F18" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="G18" s="34" t="s">
+      <c r="G18" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="H18" s="34" t="s">
+      <c r="H18" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="I18" s="34" t="s">
+      <c r="I18" s="33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="2:9" s="27" customFormat="1" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="35" t="s">
+    <row r="19" spans="2:9" s="26" customFormat="1" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="D19" s="35" t="s">
+      <c r="D19" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="E19" s="35" t="s">
+      <c r="E19" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="F19" s="32" t="s">
+      <c r="F19" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="G19" s="34" t="s">
+      <c r="G19" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="33" t="s">
         <v>108</v>
       </c>
       <c r="I19" s="24" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="2:9" s="27" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="35" t="s">
+    <row r="20" spans="2:9" s="26" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="C20" s="35" t="s">
+      <c r="C20" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="D20" s="35" t="s">
+      <c r="D20" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="E20" s="35" t="s">
+      <c r="E20" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="F20" s="35" t="s">
+      <c r="F20" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="G20" s="34" t="s">
+      <c r="G20" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="H20" s="34" t="s">
+      <c r="H20" s="33" t="s">
         <v>108</v>
       </c>
       <c r="I20" s="24" t="s">
@@ -2652,19 +2642,19 @@
       </c>
     </row>
     <row r="21" spans="2:9" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="35" t="s">
+      <c r="B21" s="70" t="s">
         <v>114</v>
       </c>
-      <c r="C21" s="36" t="s">
+      <c r="C21" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="D21" s="37" t="s">
+      <c r="D21" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="E21" s="38" t="s">
+      <c r="E21" s="37" t="s">
         <v>117</v>
       </c>
-      <c r="F21" s="39" t="s">
+      <c r="F21" s="38" t="s">
         <v>118</v>
       </c>
       <c r="G21" s="22" t="s">
@@ -2677,104 +2667,104 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="2:9" s="27" customFormat="1" ht="137.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="40" t="s">
+    <row r="22" spans="2:9" s="26" customFormat="1" ht="137.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="60" t="s">
         <v>119</v>
       </c>
-      <c r="C22" s="30" t="s">
+      <c r="C22" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="D22" s="41" t="s">
+      <c r="D22" s="39" t="s">
         <v>121</v>
       </c>
-      <c r="E22" s="38" t="s">
+      <c r="E22" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="F22" s="35" t="s">
+      <c r="F22" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="G22" s="34" t="s">
+      <c r="G22" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="H22" s="30" t="s">
+      <c r="H22" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="I22" s="41" t="s">
+      <c r="I22" s="39" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="2:9" s="65" customFormat="1" ht="137.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="60" t="s">
+    <row r="23" spans="2:9" s="26" customFormat="1" ht="137.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="61" t="s">
         <v>172</v>
       </c>
-      <c r="C23" s="61" t="s">
+      <c r="C23" s="58" t="s">
         <v>124</v>
       </c>
-      <c r="D23" s="62" t="s">
+      <c r="D23" s="39" t="s">
         <v>125</v>
       </c>
-      <c r="E23" s="62" t="s">
+      <c r="E23" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="F23" s="63" t="s">
+      <c r="F23" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="G23" s="64" t="s">
+      <c r="G23" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="H23" s="61" t="s">
+      <c r="H23" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="I23" s="62" t="s">
+      <c r="I23" s="39" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="2:9" s="27" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="42" t="s">
+    <row r="24" spans="2:9" s="26" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="40" t="s">
         <v>128</v>
       </c>
-      <c r="C24" s="30" t="s">
+      <c r="C24" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="D24" s="34" t="s">
+      <c r="D24" s="33" t="s">
         <v>130</v>
       </c>
-      <c r="E24" s="33" t="s">
+      <c r="E24" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="F24" s="33" t="s">
+      <c r="F24" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="G24" s="34" t="s">
+      <c r="G24" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="H24" s="34" t="s">
+      <c r="H24" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="I24" s="34" t="s">
+      <c r="I24" s="33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="2:9" s="27" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:9" s="26" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="C25" s="30" t="s">
+      <c r="C25" s="29" t="s">
         <v>135</v>
       </c>
       <c r="D25" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="E25" s="34" t="s">
+      <c r="E25" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="F25" s="33" t="s">
+      <c r="F25" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="G25" s="34" t="s">
+      <c r="G25" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="H25" s="34" t="s">
+      <c r="H25" s="33" t="s">
         <v>139</v>
       </c>
       <c r="I25" s="22" t="s">
@@ -2782,52 +2772,52 @@
       </c>
     </row>
     <row r="26" spans="2:9" ht="102.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="57" t="s">
+      <c r="B26" s="55" t="s">
         <v>140</v>
       </c>
-      <c r="C26" s="43" t="s">
+      <c r="C26" s="41" t="s">
         <v>141</v>
       </c>
       <c r="D26" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="E26" s="41" t="s">
+      <c r="E26" s="39" t="s">
         <v>143</v>
       </c>
-      <c r="F26" s="44" t="s">
+      <c r="F26" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="G26" s="45" t="s">
+      <c r="G26" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="H26" s="45" t="s">
+      <c r="H26" s="43" t="s">
         <v>145</v>
       </c>
-      <c r="I26" s="45" t="s">
+      <c r="I26" s="43" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F34" s="46"/>
+      <c r="F34" s="44"/>
     </row>
     <row r="35" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D35" s="47"/>
-      <c r="F35" s="46"/>
+      <c r="D35" s="45"/>
+      <c r="F35" s="44"/>
     </row>
     <row r="36" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F36" s="46"/>
+      <c r="F36" s="44"/>
     </row>
     <row r="37" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F37" s="46"/>
+      <c r="F37" s="44"/>
     </row>
     <row r="38" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F38" s="48"/>
+      <c r="F38" s="46"/>
     </row>
     <row r="40" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F40" s="49"/>
+      <c r="F40" s="47"/>
     </row>
     <row r="41" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F41" s="48"/>
+      <c r="F41" s="46"/>
     </row>
   </sheetData>
   <autoFilter ref="B2:I26">
@@ -2869,40 +2859,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="52" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="52" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="54">
+      <c r="C1" s="52">
         <v>2012</v>
       </c>
-      <c r="D1" s="54">
+      <c r="D1" s="52">
         <v>2013</v>
       </c>
-      <c r="E1" s="54">
+      <c r="E1" s="52">
         <v>2014</v>
       </c>
-      <c r="F1" s="54" t="s">
+      <c r="F1" s="52" t="s">
         <v>163</v>
       </c>
-      <c r="G1" s="54" t="s">
+      <c r="G1" s="52" t="s">
         <v>164</v>
       </c>
-      <c r="H1" s="54" t="s">
+      <c r="H1" s="52" t="s">
         <v>165</v>
       </c>
-      <c r="I1" s="54" t="s">
+      <c r="I1" s="52" t="s">
         <v>166</v>
       </c>
-      <c r="J1" s="54" t="s">
+      <c r="J1" s="52" t="s">
         <v>167</v>
       </c>
-      <c r="K1" s="54" t="s">
+      <c r="K1" s="52" t="s">
         <v>168</v>
       </c>
-      <c r="L1" s="54" t="s">
+      <c r="L1" s="52" t="s">
         <v>169</v>
       </c>
     </row>
@@ -3995,27 +3985,27 @@
         <f t="shared" ref="I26" si="9">SUM(I2:I25)</f>
         <v>0.99999999999999967</v>
       </c>
-      <c r="J26" s="55">
+      <c r="J26" s="53">
         <f t="shared" ref="J26" si="10">SUM(J2:J25)</f>
         <v>0.40073400270852677</v>
       </c>
-      <c r="K26" s="55">
+      <c r="K26" s="53">
         <f t="shared" ref="K26" si="11">SUM(K2:K25)</f>
         <v>0.4171276762746271</v>
       </c>
-      <c r="L26" s="55">
+      <c r="L26" s="53">
         <f t="shared" ref="L26" si="12">SUM(L2:L25)</f>
         <v>0.36706596430163779</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="54" t="s">
+      <c r="A30" s="52" t="s">
         <v>173</v>
       </c>
-      <c r="B30" s="54" t="s">
+      <c r="B30" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="C30" s="54" t="s">
+      <c r="C30" s="52" t="s">
         <v>175</v>
       </c>
       <c r="H30" t="s">
@@ -4035,7 +4025,7 @@
       <c r="B31">
         <v>575</v>
       </c>
-      <c r="C31" s="74">
+      <c r="C31" s="59">
         <f>A31/$A$35</f>
         <v>0.4</v>
       </c>
@@ -4051,7 +4041,7 @@
       <c r="B32">
         <v>585</v>
       </c>
-      <c r="C32" s="74">
+      <c r="C32" s="59">
         <f t="shared" ref="C32:C34" si="13">A32/$A$35</f>
         <v>0.35</v>
       </c>
@@ -4076,7 +4066,7 @@
       <c r="B33">
         <v>595</v>
       </c>
-      <c r="C33" s="74">
+      <c r="C33" s="59">
         <f t="shared" si="13"/>
         <v>0.2</v>
       </c>
@@ -4092,7 +4082,7 @@
       <c r="B34">
         <v>600</v>
       </c>
-      <c r="C34" s="74">
+      <c r="C34" s="59">
         <f t="shared" si="13"/>
         <v>0.05</v>
       </c>

</xml_diff>

<commit_message>
finaliza jornada QH 19-12-2014
</commit_message>
<xml_diff>
--- a/Documentacion/indicadores revisión junio 11 2014.xlsx
+++ b/Documentacion/indicadores revisión junio 11 2014.xlsx
@@ -1532,6 +1532,9 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1555,9 +1558,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1887,10 +1887,10 @@
   <dimension ref="B1:R41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1912,10 +1912,10 @@
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="63"/>
+      <c r="D2" s="64"/>
       <c r="E2" s="8" t="s">
         <v>2</v>
       </c>
@@ -1972,16 +1972,16 @@
       <c r="E3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="64" t="s">
+      <c r="F3" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="66" t="s">
+      <c r="G3" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="66" t="s">
+      <c r="H3" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="68" t="s">
+      <c r="I3" s="69" t="s">
         <v>14</v>
       </c>
       <c r="J3" s="21" t="s">
@@ -2023,10 +2023,10 @@
       <c r="E4" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="65"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
       <c r="J4" s="21" t="s">
         <v>151</v>
       </c>
@@ -2069,9 +2069,9 @@
       <c r="F5" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="67"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
       <c r="J5" s="21" t="s">
         <v>151</v>
       </c>
@@ -2364,22 +2364,22 @@
       <c r="C11" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="69" t="s">
+      <c r="D11" s="70" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="62" t="s">
+      <c r="E11" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="F11" s="69" t="s">
+      <c r="F11" s="70" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="69" t="s">
+      <c r="G11" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="H11" s="62" t="s">
+      <c r="H11" s="63" t="s">
         <v>45</v>
       </c>
-      <c r="I11" s="62" t="s">
+      <c r="I11" s="63" t="s">
         <v>31</v>
       </c>
       <c r="J11" s="26" t="s">
@@ -2403,12 +2403,12 @@
       <c r="C12" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="69"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="69"/>
-      <c r="H12" s="62"/>
-      <c r="I12" s="62"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="70"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="63"/>
       <c r="J12" s="26" t="s">
         <v>160</v>
       </c>
@@ -2642,7 +2642,7 @@
       </c>
     </row>
     <row r="21" spans="2:9" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="70" t="s">
+      <c r="B21" s="62" t="s">
         <v>114</v>
       </c>
       <c r="C21" s="35" t="s">

</xml_diff>

<commit_message>
finaliza jornada QH 22-12-2014
</commit_message>
<xml_diff>
--- a/Documentacion/indicadores revisión junio 11 2014.xlsx
+++ b/Documentacion/indicadores revisión junio 11 2014.xlsx
@@ -9,17 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Ajustes" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ajustes!$B$2:$I$26</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Ajustes!$B$1:$I$26</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
+  <pivotCaches>
+    <pivotCache cacheId="30" r:id="rId4"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="238">
   <si>
     <t>NOMBRE INDICADOR</t>
   </si>
@@ -1069,15 +1073,195 @@
   <si>
     <t>año fin</t>
   </si>
+  <si>
+    <t>partida</t>
+  </si>
+  <si>
+    <t>Etiquetas de fila</t>
+  </si>
+  <si>
+    <t>Total general</t>
+  </si>
+  <si>
+    <t>(en blanco)</t>
+  </si>
+  <si>
+    <t>0803001100 - Bananas o plátanos frescos del tipo "plantain" (plátano para cocción).</t>
+  </si>
+  <si>
+    <t>0803001300 - Bocadillo (manzanito, orito) (Musa acuminata), frescos.</t>
+  </si>
+  <si>
+    <t>0803001900 - Los demás bananos o plátanos frescos.</t>
+  </si>
+  <si>
+    <t>0803002000 - Bananos o plátanos secos.</t>
+  </si>
+  <si>
+    <t>0803101000 - "PLATANOS ""PLANTAINS"" FRESCOS."</t>
+  </si>
+  <si>
+    <t>0803102000 - "PLATANOS ""PLANTAINS"" SECOS."</t>
+  </si>
+  <si>
+    <t>0803901200 - Bananas bocadillo (manzanito, orito) (Musa acuminata), frescas</t>
+  </si>
+  <si>
+    <t>0803901900 - Los demás bananos o plátanos frescos.</t>
+  </si>
+  <si>
+    <t>0803902000 - Los demás bananos secos</t>
+  </si>
+  <si>
+    <t>0701100000 - Papas (patatas) frescas o refrigeradas para la siembra.</t>
+  </si>
+  <si>
+    <t>0701900000 - Las demás papas (patatas), frescas o refrigeradas.</t>
+  </si>
+  <si>
+    <t>0710100000 - Papas (patatas) aunque estén cocidas en agua o vapor, congeladas.</t>
+  </si>
+  <si>
+    <t>1105100000 - Harina, sémola y polvo de papa (patata).</t>
+  </si>
+  <si>
+    <t>1105200000 - Copos, gránulos y "pellets" de papa (patata).</t>
+  </si>
+  <si>
+    <t>2004100000 - Papas (patatas) preparadas o conservadas (excepto en vinagre o en ácido acético), congeladas.</t>
+  </si>
+  <si>
+    <t>2005200000 - Papas (patatas), preparadas o conservadas (excepto en vinagre o en ácido acético), sin congelar.</t>
+  </si>
+  <si>
+    <t>0714100000 - Raíces de mandioca (yuca), frescas, refrigerados, congeladas o secos, incluso troceadas  o en "pellets".</t>
+  </si>
+  <si>
+    <t>0714201000 - Camote (batatas, boniatos) fresco, para la siembra.</t>
+  </si>
+  <si>
+    <t>0714209000 - Los demás camotes (batatas, boniatos) frescos, refrigerados, congeladas o secos, incluso troceadas  o en "pellets".</t>
+  </si>
+  <si>
+    <t>0714300000 - Ñame (Dioscorea spp) frescos, refrigerados, congelados o secos, incluso troceados o en pellet</t>
+  </si>
+  <si>
+    <t>0714500000 - Yautía (Malanga) (Xanthosoma spp) frescos, refrige</t>
+  </si>
+  <si>
+    <t>0714909000 - Las demás raíces de arruruz o salep, aguaturmas (patacas), y raíces y tubérculos similares ricos en fécula o inulina, frescas, refrigeradas, congeladas o secas, incluso troceadas o en "pellets"; médula de sagu.</t>
+  </si>
+  <si>
+    <t>1903000000 - Tapioca y sus sucedáneos preparados con fécula, en copos, grumos, granos perlados, cerniduras o formas similares.</t>
+  </si>
+  <si>
+    <t>1512210000</t>
+  </si>
+  <si>
+    <t>1512290000</t>
+  </si>
+  <si>
+    <t>1515210000</t>
+  </si>
+  <si>
+    <t>1515290000</t>
+  </si>
+  <si>
+    <t>1508100000</t>
+  </si>
+  <si>
+    <t>1508900000</t>
+  </si>
+  <si>
+    <t>1509100000</t>
+  </si>
+  <si>
+    <t>1509900000</t>
+  </si>
+  <si>
+    <t>1510000000</t>
+  </si>
+  <si>
+    <t>1511100000</t>
+  </si>
+  <si>
+    <t>1511900000</t>
+  </si>
+  <si>
+    <t>1515500000</t>
+  </si>
+  <si>
+    <t>1507100000</t>
+  </si>
+  <si>
+    <t>1507901000</t>
+  </si>
+  <si>
+    <t>1507909000</t>
+  </si>
+  <si>
+    <t>1506001000</t>
+  </si>
+  <si>
+    <t>1506009000</t>
+  </si>
+  <si>
+    <t>1513211000</t>
+  </si>
+  <si>
+    <t>1513291000</t>
+  </si>
+  <si>
+    <t>1513110000</t>
+  </si>
+  <si>
+    <t>1513190000</t>
+  </si>
+  <si>
+    <t>1512111000</t>
+  </si>
+  <si>
+    <t>1512112000</t>
+  </si>
+  <si>
+    <t>1512191000</t>
+  </si>
+  <si>
+    <t>1206001000</t>
+  </si>
+  <si>
+    <t>1206009000</t>
+  </si>
+  <si>
+    <t>1207401000</t>
+  </si>
+  <si>
+    <t>1207409000</t>
+  </si>
+  <si>
+    <t>1201001000</t>
+  </si>
+  <si>
+    <t>1201009000</t>
+  </si>
+  <si>
+    <t>1201100000</t>
+  </si>
+  <si>
+    <t>1201900000</t>
+  </si>
+  <si>
+    <t>1208100000</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.000%"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -1272,7 +1456,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1351,13 +1535,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1482,16 +1677,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1509,7 +1704,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1559,6 +1754,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -1619,6 +1821,1398 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="fsiatama" refreshedDate="41995.611134375002" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="176">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:A177" sheet="Hoja2"/>
+  </cacheSource>
+  <cacheFields count="1">
+    <cacheField name="partida" numFmtId="0">
+      <sharedItems containsBlank="1" count="354">
+        <s v="1512210000"/>
+        <s v="1512290000"/>
+        <s v="1515210000"/>
+        <s v="1515290000"/>
+        <s v="1508100000"/>
+        <s v="1508900000"/>
+        <s v="1509100000"/>
+        <s v="1509900000"/>
+        <s v="1510000000"/>
+        <s v="1511100000"/>
+        <s v="1511900000"/>
+        <s v="1515500000"/>
+        <s v="1507100000"/>
+        <s v="1507901000"/>
+        <s v="1507909000"/>
+        <s v="1506001000"/>
+        <s v="1506009000"/>
+        <s v="1513211000"/>
+        <s v="1513291000"/>
+        <s v="1513110000"/>
+        <s v="1513190000"/>
+        <s v="1512111000"/>
+        <s v="1512112000"/>
+        <s v="1512191000"/>
+        <s v="1206001000"/>
+        <s v="1206009000"/>
+        <s v="1207401000"/>
+        <s v="1207409000"/>
+        <s v="1201001000"/>
+        <s v="1201009000"/>
+        <s v="1201100000"/>
+        <s v="1201900000"/>
+        <s v="1208100000"/>
+        <m/>
+        <s v="" u="1"/>
+        <s v="190420" u="1"/>
+        <s v="0704200000" u="1"/>
+        <s v="1003900090" u="1"/>
+        <s v="1106301000" u="1"/>
+        <s v="1107200000" u="1"/>
+        <s v="1701130000" u="1"/>
+        <s v="1109" u="1"/>
+        <s v="110220" u="1"/>
+        <s v="0802121000" u="1"/>
+        <s v="2005590000" u="1"/>
+        <s v="2103" u="1"/>
+        <s v="190230" u="1"/>
+        <s v="0809200000" u="1"/>
+        <s v="1008909900" u="1"/>
+        <s v="190510" u="1"/>
+        <s v="0803002000" u="1"/>
+        <s v="1701140000" u="1"/>
+        <s v="1702909000" u="1"/>
+        <s v="0811101000" u="1"/>
+        <s v="1905400000" u="1"/>
+        <s v="0713311000" u="1"/>
+        <s v="0809210000" u="1"/>
+        <s v="0811909100" u="1"/>
+        <s v="1701991000" u="1"/>
+        <s v="1904900010" u="1"/>
+        <s v="1003" u="1"/>
+        <s v="0713399900" u="1"/>
+        <s v="0714201000" u="1"/>
+        <s v="1212930000" u="1"/>
+        <s v="100620" u="1"/>
+        <s v="0810100000" u="1"/>
+        <s v="0904201000" u="1"/>
+        <s v="1005909000" u="1"/>
+        <s v="1108110000" u="1"/>
+        <s v="2005200000" u="1"/>
+        <s v="1108" u="1"/>
+        <s v="100590" u="1"/>
+        <s v="110311" u="1"/>
+        <s v="0710400000" u="1"/>
+        <s v="0713321000" u="1"/>
+        <s v="1001991010" u="1"/>
+        <s v="1006300010" u="1"/>
+        <s v="1109000000" u="1"/>
+        <s v="100119" u="1"/>
+        <s v="190410" u="1"/>
+        <s v="0904211000" u="1"/>
+        <s v="1104300000" u="1"/>
+        <s v="1108120000" u="1"/>
+        <s v="2008702000" u="1"/>
+        <s v="100710" u="1"/>
+        <s v="0703201000" u="1"/>
+        <s v="0704100000" u="1"/>
+        <s v="1106201000" u="1"/>
+        <s v="1107100000" u="1"/>
+        <s v="110210" u="1"/>
+        <s v="2005800000" u="1"/>
+        <s v="190220" u="1"/>
+        <s v="210330" u="1"/>
+        <s v="0713201000" u="1"/>
+        <s v="0714100000" u="1"/>
+        <s v="0809100000" u="1"/>
+        <s v="0813500000" u="1"/>
+        <s v="0904221000" u="1"/>
+        <s v="1104299000" u="1"/>
+        <s v="1108130000" u="1"/>
+        <s v="110313" u="1"/>
+        <s v="110429" u="1"/>
+        <s v="190190" u="1"/>
+        <s v="0709400000" u="1"/>
+        <s v="0712901000" u="1"/>
+        <s v="0803901200" u="1"/>
+        <s v="1105200000" u="1"/>
+        <s v="1902190000" u="1"/>
+        <s v="1107" u="1"/>
+        <s v="0701900000" u="1"/>
+        <s v="0713339200" u="1"/>
+        <s v="0803001900" u="1"/>
+        <s v="0804400000" u="1"/>
+        <s v="0712200000" u="1"/>
+        <s v="1108140000" u="1"/>
+        <s v="1003001000" u="1"/>
+        <s v="1006109000" u="1"/>
+        <s v="2008601000" u="1"/>
+        <s v="2103909000" u="1"/>
+        <s v="100610" u="1"/>
+        <s v="0703100000" u="1"/>
+        <s v="0712902000" u="1"/>
+        <s v="1005901200" u="1"/>
+        <s v="1106100000" u="1"/>
+        <s v="1905310000" u="1"/>
+        <s v="0710300000" u="1"/>
+        <s v="1006400000" u="1"/>
+        <s v="1001" u="1"/>
+        <s v="100829" u="1"/>
+        <s v="0705290000" u="1"/>
+        <s v="0811909500" u="1"/>
+        <s v="1007009000" u="1"/>
+        <s v="1905320000" u="1"/>
+        <s v="1106" u="1"/>
+        <s v="2005" u="1"/>
+        <s v="100390" u="1"/>
+        <s v="100700" u="1"/>
+        <s v="1001902090" u="1"/>
+        <s v="1904300000" u="1"/>
+        <s v="070999" u="1"/>
+        <s v="0711200000" u="1"/>
+        <s v="0713409000" u="1"/>
+        <s v="2005700000" u="1"/>
+        <s v="0713101000" u="1"/>
+        <s v="0805900000" u="1"/>
+        <s v="0813400000" u="1"/>
+        <s v="1208900000" u="1"/>
+        <s v="1905901000" u="1"/>
+        <s v="2008500000" u="1"/>
+        <s v="100510" u="1"/>
+        <s v="110419" u="1"/>
+        <s v="0709300000" u="1"/>
+        <s v="0801190000" u="1"/>
+        <s v="1008901000" u="1"/>
+        <s v="1105100000" u="1"/>
+        <s v="2004100000" u="1"/>
+        <s v="0810909000" u="1"/>
+        <s v="0814009000" u="1"/>
+        <s v="1905200000" u="1"/>
+        <s v="190211" u="1"/>
+        <s v="0713331900" u="1"/>
+        <s v="1003009010" u="1"/>
+        <s v="1904900000" u="1"/>
+        <s v="0803001300" u="1"/>
+        <s v="0803901100" u="1"/>
+        <s v="1007900000" u="1"/>
+        <s v="1704901000" u="1"/>
+        <s v="0713339100" u="1"/>
+        <s v="0713391000" u="1"/>
+        <s v="0809290000" u="1"/>
+        <s v="1102900000" u="1"/>
+        <s v="110100" u="1"/>
+        <s v="1104230000" u="1"/>
+        <s v="1302310000" u="1"/>
+        <s v="1701119000" u="1"/>
+        <s v="0712" u="1"/>
+        <s v="1108190000" u="1"/>
+        <s v="1703900000" u="1"/>
+        <s v="110319" u="1"/>
+        <s v="0701100000" u="1"/>
+        <s v="0714909000" u="1"/>
+        <s v="1005901100" u="1"/>
+        <s v="1106309000" u="1"/>
+        <s v="110630" u="1"/>
+        <s v="0710210000" u="1"/>
+        <s v="0713399200" u="1"/>
+        <s v="0802129000" u="1"/>
+        <s v="1102901000" u="1"/>
+        <s v="1904200000" u="1"/>
+        <s v="2001901000" u="1"/>
+        <s v="0709901000" u="1"/>
+        <s v="0811909400" u="1"/>
+        <s v="1001992000" u="1"/>
+        <s v="1003900010" u="1"/>
+        <s v="2005600000" u="1"/>
+        <s v="0811909900" u="1"/>
+        <s v="1102200000" u="1"/>
+        <s v="1104" u="1"/>
+        <s v="100190" u="1"/>
+        <s v="0709200000" u="1"/>
+        <s v="0710220000" u="1"/>
+        <s v="0811109000" u="1"/>
+        <s v="1902300000" u="1"/>
+        <s v="110720" u="1"/>
+        <s v="0713319000" u="1"/>
+        <s v="0801119000" u="1"/>
+        <s v="1701999000" u="1"/>
+        <s v="1905100000" u="1"/>
+        <s v="0714209000" u="1"/>
+        <s v="2008709000" u="1"/>
+        <s v="0710801000" u="1"/>
+        <s v="0904209000" u="1"/>
+        <s v="0713329000" u="1"/>
+        <s v="0714500000" u="1"/>
+        <s v="1905" u="1"/>
+        <s v="190540" u="1"/>
+        <s v="0710100000" u="1"/>
+        <s v="0810909090" u="1"/>
+        <s v="1006200000" u="1"/>
+        <s v="1008" u="1"/>
+        <s v="0803001200" u="1"/>
+        <s v="0904219000" u="1"/>
+        <s v="1103110000" u="1"/>
+        <s v="1904900090" u="1"/>
+        <s v="1103" u="1"/>
+        <s v="0703209000" u="1"/>
+        <s v="0708200000" u="1"/>
+        <s v="1001190000" u="1"/>
+        <s v="1106209000" u="1"/>
+        <s v="110620" u="1"/>
+        <s v="110811" u="1"/>
+        <s v="1702200000" u="1"/>
+        <s v="1904100000" u="1"/>
+        <s v="0710" u="1"/>
+        <s v="1208" u="1"/>
+        <s v="071040" u="1"/>
+        <s v="110900" u="1"/>
+        <s v="0713209000" u="1"/>
+        <s v="0810400000" u="1"/>
+        <s v="0904229000" u="1"/>
+        <s v="1001991090" u="1"/>
+        <s v="1006300090" u="1"/>
+        <s v="1007100000" u="1"/>
+        <s v="0803902000" u="1"/>
+        <s v="0813200000" u="1"/>
+        <s v="1102100000" u="1"/>
+        <s v="1702902000" u="1"/>
+        <s v="2008300000" u="1"/>
+        <s v="071290" u="1"/>
+        <s v="110430" u="1"/>
+        <s v="110812" u="1"/>
+        <s v="1902200000" u="1"/>
+        <s v="1904" u="1"/>
+        <s v="110710" u="1"/>
+        <s v="0804100000" u="1"/>
+        <s v="0810901040" u="1"/>
+        <s v="0811909300" u="1"/>
+        <s v="1103130000" u="1"/>
+        <s v="1701910000" u="1"/>
+        <s v="1703100000" u="1"/>
+        <s v="2005510000" u="1"/>
+        <s v="1007" u="1"/>
+        <s v="200580" u="1"/>
+        <s v="0713359000" u="1"/>
+        <s v="2008609000" u="1"/>
+        <s v="1102" u="1"/>
+        <s v="100300" u="1"/>
+        <s v="110813" u="1"/>
+        <s v="1005902000" u="1"/>
+        <s v="1702903000" u="1"/>
+        <s v="0709" u="1"/>
+        <s v="190219" u="1"/>
+        <s v="0809400000" u="1"/>
+        <s v="2103301000" u="1"/>
+        <s v="0709700000" u="1"/>
+        <s v="1001109000" u="1"/>
+        <s v="1104291000" u="1"/>
+        <s v="1901901000" u="1"/>
+        <s v="100110" u="1"/>
+        <s v="110814" u="1"/>
+        <s v="0810909020" u="1"/>
+        <s v="0708100000" u="1"/>
+        <s v="0802210000" u="1"/>
+        <s v="1005903000" u="1"/>
+        <s v="1008290000" u="1"/>
+        <s v="1702904000" u="1"/>
+        <s v="110610" u="1"/>
+        <s v="190531" u="1"/>
+        <s v="0812902000" u="1"/>
+        <s v="1006" u="1"/>
+        <s v="100640" u="1"/>
+        <s v="0713109000" u="1"/>
+        <s v="0803001100" u="1"/>
+        <s v="1001902010" u="1"/>
+        <s v="1006101000" u="1"/>
+        <s v="1901902000" u="1"/>
+        <s v="1905909000" u="1"/>
+        <s v="2005400000" u="1"/>
+        <s v="1101" u="1"/>
+        <s v="190590" u="1"/>
+        <s v="0802220000" u="1"/>
+        <s v="0813100000" u="1"/>
+        <s v="1008909000" u="1"/>
+        <s v="100890" u="1"/>
+        <s v="190532" u="1"/>
+        <s v="0803901900" u="1"/>
+        <s v="0811901000" u="1"/>
+        <s v="1005904000" u="1"/>
+        <s v="190430" u="1"/>
+        <s v="0713339900" u="1"/>
+        <s v="0803101000" u="1"/>
+        <s v="1005100000" u="1"/>
+        <s v="1104190000" u="1"/>
+        <s v="1404901000" u="1"/>
+        <s v="0811200000" u="1"/>
+        <s v="1007001000" u="1"/>
+        <s v="1704909000" u="1"/>
+        <s v="2103902000" u="1"/>
+        <s v="120890" u="1"/>
+        <s v="0709991000" u="1"/>
+        <s v="1902110000" u="1"/>
+        <s v="1902" u="1"/>
+        <s v="0714300000" u="1"/>
+        <s v="0809300000" u="1"/>
+        <s v="1903000000" u="1"/>
+        <s v="2008800000" u="1"/>
+        <s v="1005" u="1"/>
+        <s v="100199" u="1"/>
+        <s v="190520" u="1"/>
+        <s v="0709600000" u="1"/>
+        <s v="0803102000" u="1"/>
+        <s v="1008209000" u="1"/>
+        <s v="100820" u="1"/>
+        <s v="190490" u="1"/>
+        <s v="0812100000" u="1"/>
+        <s v="1003009090" u="1"/>
+        <s v="1101000000" u="1"/>
+        <s v="100790" u="1"/>
+        <s v="0704900000" u="1"/>
+        <s v="0802110000" u="1"/>
+        <s v="1102909000" u="1"/>
+        <s v="110290" u="1"/>
+        <s v="1103190000" u="1"/>
+        <s v="070990" u="1"/>
+        <s v="100630" u="1"/>
+        <s v="110423" u="1"/>
+        <s v="0705210000" u="1"/>
+        <s v="0810200000" u="1"/>
+        <s v="110819" u="1"/>
+        <s v="0713331100" u="1"/>
+        <s v="1701120000" u="1"/>
+        <s v="1901" u="1"/>
+        <s v="0810902000" u="1"/>
+        <s v="1701111000" u="1"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="176">
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="10"/>
+  </r>
+  <r>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="10"/>
+  </r>
+  <r>
+    <x v="11"/>
+  </r>
+  <r>
+    <x v="11"/>
+  </r>
+  <r>
+    <x v="12"/>
+  </r>
+  <r>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="14"/>
+  </r>
+  <r>
+    <x v="12"/>
+  </r>
+  <r>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="14"/>
+  </r>
+  <r>
+    <x v="15"/>
+  </r>
+  <r>
+    <x v="16"/>
+  </r>
+  <r>
+    <x v="15"/>
+  </r>
+  <r>
+    <x v="16"/>
+  </r>
+  <r>
+    <x v="17"/>
+  </r>
+  <r>
+    <x v="18"/>
+  </r>
+  <r>
+    <x v="17"/>
+  </r>
+  <r>
+    <x v="18"/>
+  </r>
+  <r>
+    <x v="19"/>
+  </r>
+  <r>
+    <x v="20"/>
+  </r>
+  <r>
+    <x v="19"/>
+  </r>
+  <r>
+    <x v="20"/>
+  </r>
+  <r>
+    <x v="21"/>
+  </r>
+  <r>
+    <x v="22"/>
+  </r>
+  <r>
+    <x v="23"/>
+  </r>
+  <r>
+    <x v="21"/>
+  </r>
+  <r>
+    <x v="22"/>
+  </r>
+  <r>
+    <x v="23"/>
+  </r>
+  <r>
+    <x v="24"/>
+  </r>
+  <r>
+    <x v="25"/>
+  </r>
+  <r>
+    <x v="24"/>
+  </r>
+  <r>
+    <x v="25"/>
+  </r>
+  <r>
+    <x v="26"/>
+  </r>
+  <r>
+    <x v="27"/>
+  </r>
+  <r>
+    <x v="26"/>
+  </r>
+  <r>
+    <x v="27"/>
+  </r>
+  <r>
+    <x v="28"/>
+  </r>
+  <r>
+    <x v="29"/>
+  </r>
+  <r>
+    <x v="30"/>
+  </r>
+  <r>
+    <x v="31"/>
+  </r>
+  <r>
+    <x v="32"/>
+  </r>
+  <r>
+    <x v="28"/>
+  </r>
+  <r>
+    <x v="29"/>
+  </r>
+  <r>
+    <x v="30"/>
+  </r>
+  <r>
+    <x v="31"/>
+  </r>
+  <r>
+    <x v="32"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="33"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B2:B37" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="1">
+    <pivotField axis="axisRow" showAll="0" sortType="ascending">
+      <items count="355">
+        <item m="1" x="34"/>
+        <item m="1" x="179"/>
+        <item m="1" x="109"/>
+        <item m="1" x="120"/>
+        <item m="1" x="85"/>
+        <item m="1" x="225"/>
+        <item m="1" x="86"/>
+        <item m="1" x="36"/>
+        <item m="1" x="338"/>
+        <item m="1" x="346"/>
+        <item m="1" x="129"/>
+        <item m="1" x="281"/>
+        <item m="1" x="226"/>
+        <item m="1" x="270"/>
+        <item m="1" x="199"/>
+        <item m="1" x="151"/>
+        <item m="1" x="103"/>
+        <item m="1" x="329"/>
+        <item m="1" x="274"/>
+        <item m="1" x="343"/>
+        <item m="1" x="190"/>
+        <item m="1" x="139"/>
+        <item m="1" x="319"/>
+        <item m="1" x="233"/>
+        <item m="1" x="216"/>
+        <item m="1" x="184"/>
+        <item m="1" x="200"/>
+        <item m="1" x="125"/>
+        <item m="1" x="235"/>
+        <item m="1" x="73"/>
+        <item m="1" x="210"/>
+        <item m="1" x="140"/>
+        <item m="1" x="175"/>
+        <item m="1" x="113"/>
+        <item m="1" x="248"/>
+        <item m="1" x="104"/>
+        <item m="1" x="121"/>
+        <item m="1" x="143"/>
+        <item m="1" x="291"/>
+        <item m="1" x="93"/>
+        <item m="1" x="237"/>
+        <item m="1" x="55"/>
+        <item m="1" x="204"/>
+        <item m="1" x="74"/>
+        <item m="1" x="212"/>
+        <item m="1" x="349"/>
+        <item m="1" x="160"/>
+        <item m="1" x="167"/>
+        <item m="1" x="110"/>
+        <item m="1" x="309"/>
+        <item m="1" x="263"/>
+        <item m="1" x="168"/>
+        <item m="1" x="185"/>
+        <item m="1" x="61"/>
+        <item m="1" x="141"/>
+        <item m="1" x="94"/>
+        <item m="1" x="62"/>
+        <item m="1" x="208"/>
+        <item m="1" x="322"/>
+        <item m="1" x="213"/>
+        <item m="1" x="180"/>
+        <item m="1" x="205"/>
+        <item m="1" x="152"/>
+        <item m="1" x="339"/>
+        <item m="1" x="43"/>
+        <item m="1" x="186"/>
+        <item m="1" x="282"/>
+        <item m="1" x="300"/>
+        <item m="1" x="292"/>
+        <item m="1" x="220"/>
+        <item m="1" x="163"/>
+        <item m="1" x="111"/>
+        <item m="1" x="50"/>
+        <item m="1" x="310"/>
+        <item m="1" x="330"/>
+        <item m="1" x="164"/>
+        <item m="1" x="105"/>
+        <item m="1" x="305"/>
+        <item m="1" x="243"/>
+        <item m="1" x="254"/>
+        <item m="1" x="112"/>
+        <item m="1" x="144"/>
+        <item m="1" x="95"/>
+        <item m="1" x="47"/>
+        <item m="1" x="56"/>
+        <item m="1" x="169"/>
+        <item m="1" x="323"/>
+        <item m="1" x="272"/>
+        <item m="1" x="65"/>
+        <item m="1" x="347"/>
+        <item m="1" x="238"/>
+        <item m="1" x="255"/>
+        <item m="1" x="352"/>
+        <item m="1" x="156"/>
+        <item m="1" x="280"/>
+        <item m="1" x="217"/>
+        <item m="1" x="53"/>
+        <item m="1" x="201"/>
+        <item m="1" x="314"/>
+        <item m="1" x="306"/>
+        <item m="1" x="57"/>
+        <item m="1" x="256"/>
+        <item m="1" x="191"/>
+        <item m="1" x="130"/>
+        <item m="1" x="195"/>
+        <item m="1" x="334"/>
+        <item m="1" x="288"/>
+        <item m="1" x="301"/>
+        <item m="1" x="244"/>
+        <item m="1" x="145"/>
+        <item m="1" x="96"/>
+        <item m="1" x="157"/>
+        <item m="1" x="66"/>
+        <item m="1" x="211"/>
+        <item m="1" x="80"/>
+        <item m="1" x="221"/>
+        <item m="1" x="97"/>
+        <item m="1" x="239"/>
+        <item m="1" x="127"/>
+        <item m="1" x="278"/>
+        <item m="1" x="275"/>
+        <item m="1" x="78"/>
+        <item m="1" x="227"/>
+        <item m="1" x="198"/>
+        <item m="1" x="293"/>
+        <item m="1" x="137"/>
+        <item m="1" x="327"/>
+        <item m="1" x="75"/>
+        <item m="1" x="240"/>
+        <item m="1" x="192"/>
+        <item m="1" x="60"/>
+        <item m="1" x="266"/>
+        <item m="1" x="115"/>
+        <item m="1" x="161"/>
+        <item m="1" x="335"/>
+        <item m="1" x="135"/>
+        <item m="1" x="193"/>
+        <item m="1" x="37"/>
+        <item m="1" x="326"/>
+        <item m="1" x="149"/>
+        <item m="1" x="311"/>
+        <item m="1" x="71"/>
+        <item m="1" x="181"/>
+        <item m="1" x="122"/>
+        <item m="1" x="268"/>
+        <item m="1" x="283"/>
+        <item m="1" x="307"/>
+        <item m="1" x="67"/>
+        <item m="1" x="289"/>
+        <item m="1" x="119"/>
+        <item m="1" x="294"/>
+        <item m="1" x="116"/>
+        <item m="1" x="64"/>
+        <item m="1" x="218"/>
+        <item m="1" x="344"/>
+        <item m="1" x="76"/>
+        <item m="1" x="241"/>
+        <item m="1" x="290"/>
+        <item m="1" x="126"/>
+        <item m="1" x="261"/>
+        <item m="1" x="136"/>
+        <item m="1" x="315"/>
+        <item m="1" x="131"/>
+        <item m="1" x="84"/>
+        <item m="1" x="242"/>
+        <item m="1" x="337"/>
+        <item m="1" x="165"/>
+        <item m="1" x="219"/>
+        <item m="1" x="332"/>
+        <item m="1" x="331"/>
+        <item m="1" x="128"/>
+        <item m="1" x="284"/>
+        <item m="1" x="303"/>
+        <item m="1" x="153"/>
+        <item m="1" x="302"/>
+        <item m="1" x="48"/>
+        <item m="1" x="298"/>
+        <item m="1" x="171"/>
+        <item m="1" x="336"/>
+        <item m="1" x="265"/>
+        <item m="1" x="89"/>
+        <item m="1" x="245"/>
+        <item m="1" x="42"/>
+        <item m="1" x="196"/>
+        <item m="1" x="341"/>
+        <item m="1" x="170"/>
+        <item m="1" x="187"/>
+        <item m="1" x="340"/>
+        <item m="1" x="224"/>
+        <item m="1" x="72"/>
+        <item m="1" x="222"/>
+        <item m="1" x="100"/>
+        <item m="1" x="257"/>
+        <item m="1" x="178"/>
+        <item m="1" x="342"/>
+        <item m="1" x="197"/>
+        <item m="1" x="150"/>
+        <item m="1" x="312"/>
+        <item m="1" x="345"/>
+        <item m="1" x="172"/>
+        <item m="1" x="101"/>
+        <item m="1" x="276"/>
+        <item m="1" x="98"/>
+        <item m="1" x="249"/>
+        <item m="1" x="81"/>
+        <item m="1" x="154"/>
+        <item m="1" x="106"/>
+        <item m="1" x="133"/>
+        <item m="1" x="286"/>
+        <item m="1" x="123"/>
+        <item m="1" x="229"/>
+        <item m="1" x="87"/>
+        <item m="1" x="228"/>
+        <item m="1" x="183"/>
+        <item m="1" x="38"/>
+        <item m="1" x="182"/>
+        <item m="1" x="108"/>
+        <item m="1" x="253"/>
+        <item m="1" x="88"/>
+        <item m="1" x="203"/>
+        <item m="1" x="39"/>
+        <item m="1" x="70"/>
+        <item m="1" x="230"/>
+        <item m="1" x="68"/>
+        <item m="1" x="250"/>
+        <item m="1" x="82"/>
+        <item m="1" x="267"/>
+        <item m="1" x="99"/>
+        <item m="1" x="279"/>
+        <item m="1" x="114"/>
+        <item m="1" x="348"/>
+        <item m="1" x="176"/>
+        <item m="1" x="41"/>
+        <item m="1" x="236"/>
+        <item m="1" x="77"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item m="1" x="234"/>
+        <item x="32"/>
+        <item m="1" x="318"/>
+        <item m="1" x="146"/>
+        <item m="1" x="63"/>
+        <item m="1" x="173"/>
+        <item m="1" x="313"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="11"/>
+        <item m="1" x="353"/>
+        <item m="1" x="174"/>
+        <item m="1" x="350"/>
+        <item m="1" x="40"/>
+        <item m="1" x="51"/>
+        <item m="1" x="258"/>
+        <item m="1" x="58"/>
+        <item m="1" x="206"/>
+        <item m="1" x="231"/>
+        <item m="1" x="246"/>
+        <item m="1" x="269"/>
+        <item m="1" x="285"/>
+        <item m="1" x="52"/>
+        <item m="1" x="259"/>
+        <item m="1" x="177"/>
+        <item m="1" x="166"/>
+        <item m="1" x="316"/>
+        <item m="1" x="351"/>
+        <item m="1" x="102"/>
+        <item m="1" x="277"/>
+        <item m="1" x="295"/>
+        <item m="1" x="321"/>
+        <item m="1" x="159"/>
+        <item m="1" x="320"/>
+        <item m="1" x="271"/>
+        <item m="1" x="107"/>
+        <item m="1" x="91"/>
+        <item m="1" x="251"/>
+        <item m="1" x="46"/>
+        <item m="1" x="202"/>
+        <item m="1" x="324"/>
+        <item m="1" x="252"/>
+        <item m="1" x="79"/>
+        <item m="1" x="232"/>
+        <item m="1" x="35"/>
+        <item m="1" x="188"/>
+        <item m="1" x="308"/>
+        <item m="1" x="138"/>
+        <item m="1" x="333"/>
+        <item m="1" x="162"/>
+        <item m="1" x="59"/>
+        <item m="1" x="223"/>
+        <item m="1" x="214"/>
+        <item m="1" x="49"/>
+        <item m="1" x="207"/>
+        <item m="1" x="328"/>
+        <item m="1" x="158"/>
+        <item m="1" x="287"/>
+        <item m="1" x="124"/>
+        <item m="1" x="304"/>
+        <item m="1" x="132"/>
+        <item m="1" x="215"/>
+        <item m="1" x="54"/>
+        <item m="1" x="299"/>
+        <item m="1" x="147"/>
+        <item m="1" x="296"/>
+        <item m="1" x="189"/>
+        <item m="1" x="155"/>
+        <item m="1" x="134"/>
+        <item m="1" x="69"/>
+        <item m="1" x="297"/>
+        <item m="1" x="260"/>
+        <item m="1" x="44"/>
+        <item m="1" x="194"/>
+        <item m="1" x="142"/>
+        <item m="1" x="262"/>
+        <item m="1" x="90"/>
+        <item m="1" x="247"/>
+        <item m="1" x="148"/>
+        <item m="1" x="117"/>
+        <item m="1" x="264"/>
+        <item m="1" x="83"/>
+        <item m="1" x="209"/>
+        <item m="1" x="325"/>
+        <item m="1" x="45"/>
+        <item m="1" x="92"/>
+        <item m="1" x="273"/>
+        <item m="1" x="317"/>
+        <item m="1" x="118"/>
+        <item x="33"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="35">
+    <i>
+      <x v="235"/>
+    </i>
+    <i>
+      <x v="236"/>
+    </i>
+    <i>
+      <x v="237"/>
+    </i>
+    <i>
+      <x v="238"/>
+    </i>
+    <i>
+      <x v="239"/>
+    </i>
+    <i>
+      <x v="240"/>
+    </i>
+    <i>
+      <x v="241"/>
+    </i>
+    <i>
+      <x v="242"/>
+    </i>
+    <i>
+      <x v="244"/>
+    </i>
+    <i>
+      <x v="250"/>
+    </i>
+    <i>
+      <x v="251"/>
+    </i>
+    <i>
+      <x v="252"/>
+    </i>
+    <i>
+      <x v="253"/>
+    </i>
+    <i>
+      <x v="254"/>
+    </i>
+    <i>
+      <x v="255"/>
+    </i>
+    <i>
+      <x v="256"/>
+    </i>
+    <i>
+      <x v="257"/>
+    </i>
+    <i>
+      <x v="258"/>
+    </i>
+    <i>
+      <x v="259"/>
+    </i>
+    <i>
+      <x v="260"/>
+    </i>
+    <i>
+      <x v="261"/>
+    </i>
+    <i>
+      <x v="262"/>
+    </i>
+    <i>
+      <x v="263"/>
+    </i>
+    <i>
+      <x v="264"/>
+    </i>
+    <i>
+      <x v="265"/>
+    </i>
+    <i>
+      <x v="266"/>
+    </i>
+    <i>
+      <x v="267"/>
+    </i>
+    <i>
+      <x v="268"/>
+    </i>
+    <i>
+      <x v="269"/>
+    </i>
+    <i>
+      <x v="270"/>
+    </i>
+    <i>
+      <x v="271"/>
+    </i>
+    <i>
+      <x v="272"/>
+    </i>
+    <i>
+      <x v="273"/>
+    </i>
+    <i>
+      <x v="353"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1886,11 +3480,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A19" sqref="A19"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2590,7 +4184,7 @@
       </c>
     </row>
     <row r="19" spans="2:9" s="26" customFormat="1" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="62" t="s">
         <v>102</v>
       </c>
       <c r="C19" s="34" t="s">
@@ -2616,7 +4210,7 @@
       </c>
     </row>
     <row r="20" spans="2:9" s="26" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="62" t="s">
         <v>109</v>
       </c>
       <c r="C20" s="34" t="s">
@@ -4109,4 +5703,2410 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M471"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13:I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="74" t="s">
+        <v>205</v>
+      </c>
+      <c r="B2" s="71" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="74" t="s">
+        <v>206</v>
+      </c>
+      <c r="B3" s="72" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="74" t="s">
+        <v>205</v>
+      </c>
+      <c r="B4" s="72" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="74" t="s">
+        <v>206</v>
+      </c>
+      <c r="B5" s="72" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="74" t="s">
+        <v>207</v>
+      </c>
+      <c r="B6" s="72" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="74" t="s">
+        <v>208</v>
+      </c>
+      <c r="B7" s="72" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="74" t="s">
+        <v>207</v>
+      </c>
+      <c r="B8" s="72" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="74" t="s">
+        <v>208</v>
+      </c>
+      <c r="B9" s="72" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="74" t="s">
+        <v>209</v>
+      </c>
+      <c r="B10" s="72" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="74" t="s">
+        <v>210</v>
+      </c>
+      <c r="B11" s="72" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="74" t="s">
+        <v>209</v>
+      </c>
+      <c r="B12" s="72" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="74" t="s">
+        <v>210</v>
+      </c>
+      <c r="B13" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="H13">
+        <v>2010</v>
+      </c>
+      <c r="I13" s="75">
+        <v>845027.64130188676</v>
+      </c>
+      <c r="K13">
+        <v>261704.6</v>
+      </c>
+      <c r="M13">
+        <v>4737783</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="74" t="s">
+        <v>211</v>
+      </c>
+      <c r="B14" s="72" t="s">
+        <v>217</v>
+      </c>
+      <c r="H14">
+        <v>2011</v>
+      </c>
+      <c r="I14" s="75">
+        <v>1057657.9879999999</v>
+      </c>
+      <c r="K14">
+        <v>265455.5</v>
+      </c>
+      <c r="M14">
+        <v>4897031.7999999989</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="74" t="s">
+        <v>212</v>
+      </c>
+      <c r="B15" s="72" t="s">
+        <v>218</v>
+      </c>
+      <c r="H15">
+        <v>2012</v>
+      </c>
+      <c r="I15" s="75">
+        <v>1095752.9345</v>
+      </c>
+      <c r="K15">
+        <v>318215.58862780791</v>
+      </c>
+      <c r="M15">
+        <v>5293919.9873215118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="74" t="s">
+        <v>213</v>
+      </c>
+      <c r="B16" s="72" t="s">
+        <v>219</v>
+      </c>
+      <c r="H16">
+        <v>2013</v>
+      </c>
+      <c r="I16" s="75">
+        <v>1151586.4650000001</v>
+      </c>
+      <c r="K16">
+        <v>352234.97062846157</v>
+      </c>
+      <c r="M16">
+        <v>5901980.1473486982</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="74" t="s">
+        <v>211</v>
+      </c>
+      <c r="B17" s="72" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="74" t="s">
+        <v>212</v>
+      </c>
+      <c r="B18" s="72" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="74" t="s">
+        <v>213</v>
+      </c>
+      <c r="B19" s="72" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="74" t="s">
+        <v>214</v>
+      </c>
+      <c r="B20" s="72" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="74" t="s">
+        <v>215</v>
+      </c>
+      <c r="B21" s="72" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="74" t="s">
+        <v>214</v>
+      </c>
+      <c r="B22" s="72" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="74" t="s">
+        <v>215</v>
+      </c>
+      <c r="B23" s="72" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="74" t="s">
+        <v>216</v>
+      </c>
+      <c r="B24" s="72" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="74" t="s">
+        <v>216</v>
+      </c>
+      <c r="B25" s="72" t="s">
+        <v>227</v>
+      </c>
+      <c r="H25" t="s">
+        <v>182</v>
+      </c>
+      <c r="I25">
+        <f>FIND("-",H25)</f>
+        <v>12</v>
+      </c>
+      <c r="J25" t="str">
+        <f>LEFT(H25,I25-1)</f>
+        <v xml:space="preserve">0803001100 </v>
+      </c>
+      <c r="K25" t="str">
+        <f>IFERROR(TRIM(J25),"")</f>
+        <v>0803001100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="74" t="s">
+        <v>217</v>
+      </c>
+      <c r="B26" s="72" t="s">
+        <v>228</v>
+      </c>
+      <c r="I26" t="e">
+        <f t="shared" ref="I26:I75" si="0">FIND("-",H26)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J26" t="e">
+        <f t="shared" ref="J26:J75" si="1">LEFT(H26,I26-1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" ref="K26:K75" si="2">IFERROR(TRIM(J26),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="74" t="s">
+        <v>218</v>
+      </c>
+      <c r="B27" s="72" t="s">
+        <v>205</v>
+      </c>
+      <c r="H27" t="s">
+        <v>183</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J27" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">0803001300 </v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="2"/>
+        <v>0803001300</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="74" t="s">
+        <v>219</v>
+      </c>
+      <c r="B28" s="72" t="s">
+        <v>206</v>
+      </c>
+      <c r="I28" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J28" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="74" t="s">
+        <v>217</v>
+      </c>
+      <c r="B29" s="72" t="s">
+        <v>224</v>
+      </c>
+      <c r="H29" t="s">
+        <v>184</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J29" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">0803001900 </v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="2"/>
+        <v>0803001900</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="74" t="s">
+        <v>218</v>
+      </c>
+      <c r="B30" s="72" t="s">
+        <v>225</v>
+      </c>
+      <c r="I30" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J30" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="74" t="s">
+        <v>219</v>
+      </c>
+      <c r="B31" s="72" t="s">
+        <v>222</v>
+      </c>
+      <c r="H31" t="s">
+        <v>185</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J31" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">0803002000 </v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="2"/>
+        <v>0803002000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="74" t="s">
+        <v>220</v>
+      </c>
+      <c r="B32" s="72" t="s">
+        <v>223</v>
+      </c>
+      <c r="I32" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J32" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="74" t="s">
+        <v>221</v>
+      </c>
+      <c r="B33" s="72" t="s">
+        <v>207</v>
+      </c>
+      <c r="H33" t="s">
+        <v>186</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J33" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">0803101000 </v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="2"/>
+        <v>0803101000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="74" t="s">
+        <v>220</v>
+      </c>
+      <c r="B34" s="72" t="s">
+        <v>208</v>
+      </c>
+      <c r="I34" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J34" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K34" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="74" t="s">
+        <v>221</v>
+      </c>
+      <c r="B35" s="72" t="s">
+        <v>216</v>
+      </c>
+      <c r="H35" t="s">
+        <v>187</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J35" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">0803102000 </v>
+      </c>
+      <c r="K35" t="str">
+        <f t="shared" si="2"/>
+        <v>0803102000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="74" t="s">
+        <v>222</v>
+      </c>
+      <c r="B36" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="I36" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J36" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K36" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="74" t="s">
+        <v>223</v>
+      </c>
+      <c r="B37" s="72" t="s">
+        <v>180</v>
+      </c>
+      <c r="H37" t="s">
+        <v>188</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J37" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">0803901200 </v>
+      </c>
+      <c r="K37" t="str">
+        <f t="shared" si="2"/>
+        <v>0803901200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="74" t="s">
+        <v>222</v>
+      </c>
+      <c r="I38" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J38" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K38" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="74" t="s">
+        <v>223</v>
+      </c>
+      <c r="H39" t="s">
+        <v>189</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J39" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">0803901900 </v>
+      </c>
+      <c r="K39" t="str">
+        <f t="shared" si="2"/>
+        <v>0803901900</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="74" t="s">
+        <v>224</v>
+      </c>
+      <c r="I40" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J40" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K40" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="H41" t="s">
+        <v>190</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J41" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">0803902000 </v>
+      </c>
+      <c r="K41" t="str">
+        <f t="shared" si="2"/>
+        <v>0803902000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="74" t="s">
+        <v>224</v>
+      </c>
+      <c r="I42" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J42" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K42" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="74" t="s">
+        <v>225</v>
+      </c>
+      <c r="I43" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J43" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K43" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="74" t="s">
+        <v>226</v>
+      </c>
+      <c r="I44" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J44" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K44" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="H45" t="s">
+        <v>191</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J45" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">0701100000 </v>
+      </c>
+      <c r="K45" t="str">
+        <f t="shared" si="2"/>
+        <v>0701100000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="74" t="s">
+        <v>228</v>
+      </c>
+      <c r="I46" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J46" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K46" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="74" t="s">
+        <v>226</v>
+      </c>
+      <c r="H47" t="s">
+        <v>192</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J47" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">0701900000 </v>
+      </c>
+      <c r="K47" t="str">
+        <f t="shared" si="2"/>
+        <v>0701900000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="I48" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J48" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K48" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="74" t="s">
+        <v>228</v>
+      </c>
+      <c r="H49" t="s">
+        <v>193</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J49" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">0710100000 </v>
+      </c>
+      <c r="K49" t="str">
+        <f t="shared" si="2"/>
+        <v>0710100000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="74" t="s">
+        <v>229</v>
+      </c>
+      <c r="I50" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J50" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K50" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="74" t="s">
+        <v>230</v>
+      </c>
+      <c r="H51" t="s">
+        <v>194</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J51" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">1105100000 </v>
+      </c>
+      <c r="K51" t="str">
+        <f t="shared" si="2"/>
+        <v>1105100000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="74" t="s">
+        <v>229</v>
+      </c>
+      <c r="I52" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J52" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K52" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="74" t="s">
+        <v>230</v>
+      </c>
+      <c r="H53" t="s">
+        <v>195</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J53" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">1105200000 </v>
+      </c>
+      <c r="K53" t="str">
+        <f t="shared" si="2"/>
+        <v>1105200000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="74" t="s">
+        <v>231</v>
+      </c>
+      <c r="I54" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J54" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K54" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="74" t="s">
+        <v>232</v>
+      </c>
+      <c r="H55" t="s">
+        <v>196</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J55" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">2004100000 </v>
+      </c>
+      <c r="K55" t="str">
+        <f t="shared" si="2"/>
+        <v>2004100000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="74" t="s">
+        <v>231</v>
+      </c>
+      <c r="I56" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J56" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K56" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="74" t="s">
+        <v>232</v>
+      </c>
+      <c r="H57" t="s">
+        <v>197</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J57" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">2005200000 </v>
+      </c>
+      <c r="K57" t="str">
+        <f t="shared" si="2"/>
+        <v>2005200000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="74" t="s">
+        <v>233</v>
+      </c>
+      <c r="I58" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J58" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K58" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="74" t="s">
+        <v>234</v>
+      </c>
+      <c r="I59" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J59" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K59" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="74" t="s">
+        <v>235</v>
+      </c>
+      <c r="I60" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J60" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K60" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="74" t="s">
+        <v>236</v>
+      </c>
+      <c r="H61" t="s">
+        <v>198</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J61" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">0714100000 </v>
+      </c>
+      <c r="K61" t="str">
+        <f t="shared" si="2"/>
+        <v>0714100000</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="74" t="s">
+        <v>237</v>
+      </c>
+      <c r="I62" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J62" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K62" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="74" t="s">
+        <v>233</v>
+      </c>
+      <c r="H63" t="s">
+        <v>199</v>
+      </c>
+      <c r="I63">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J63" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">0714201000 </v>
+      </c>
+      <c r="K63" t="str">
+        <f t="shared" si="2"/>
+        <v>0714201000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="74" t="s">
+        <v>234</v>
+      </c>
+      <c r="I64" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J64" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K64" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" s="74" t="s">
+        <v>235</v>
+      </c>
+      <c r="H65" t="s">
+        <v>200</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J65" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">0714209000 </v>
+      </c>
+      <c r="K65" t="str">
+        <f t="shared" si="2"/>
+        <v>0714209000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" s="74" t="s">
+        <v>236</v>
+      </c>
+      <c r="I66" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J66" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K66" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" s="74" t="s">
+        <v>237</v>
+      </c>
+      <c r="H67" t="s">
+        <v>201</v>
+      </c>
+      <c r="I67">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J67" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">0714300000 </v>
+      </c>
+      <c r="K67" t="str">
+        <f t="shared" si="2"/>
+        <v>0714300000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" s="73"/>
+      <c r="I68" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J68" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K68" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" s="73"/>
+      <c r="H69" t="s">
+        <v>202</v>
+      </c>
+      <c r="I69">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J69" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">0714500000 </v>
+      </c>
+      <c r="K69" t="str">
+        <f t="shared" si="2"/>
+        <v>0714500000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" s="73"/>
+      <c r="I70" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J70" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K70" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" s="73"/>
+      <c r="H71" t="s">
+        <v>203</v>
+      </c>
+      <c r="I71">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J71" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">0714909000 </v>
+      </c>
+      <c r="K71" t="str">
+        <f t="shared" si="2"/>
+        <v>0714909000</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" s="73"/>
+      <c r="I72" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J72" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K72" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" s="73"/>
+      <c r="I73" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J73" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K73" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74" s="73"/>
+      <c r="I74" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J74" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K74" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75" s="73"/>
+      <c r="H75" t="s">
+        <v>204</v>
+      </c>
+      <c r="I75">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J75" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">1903000000 </v>
+      </c>
+      <c r="K75" t="str">
+        <f t="shared" si="2"/>
+        <v>1903000000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" s="73"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" s="73"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78" s="73"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79" s="73"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" s="73"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="73"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="73"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="73"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="73"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="73"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="73"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="73"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="73"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="73"/>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="73"/>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="73"/>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="73"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="73"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="73"/>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="73"/>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="73"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="73"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="73"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="73"/>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="73"/>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="73"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="73"/>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="73"/>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="73"/>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="73"/>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="73"/>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="73"/>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="73"/>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="73"/>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="73"/>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="73"/>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="73"/>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="73"/>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="73"/>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="73"/>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="73"/>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="73"/>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="73"/>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="73"/>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="73"/>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="73"/>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="73"/>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="73"/>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="73"/>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="73"/>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="73"/>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="73"/>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="73"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="73"/>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="73"/>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="73"/>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="73"/>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="73"/>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="73"/>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="73"/>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="73"/>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="73"/>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="73"/>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="73"/>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="73"/>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="73"/>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="73"/>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="73"/>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="73"/>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="73"/>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="73"/>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="73"/>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="73"/>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="73"/>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="73"/>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="73"/>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="73"/>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="73"/>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="73"/>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="73"/>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="73"/>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="73"/>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="73"/>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="73"/>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="73"/>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="73"/>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="73"/>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="73"/>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="73"/>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="73"/>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="73"/>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="73"/>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="73"/>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="73"/>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="73"/>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="73"/>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="73"/>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="73"/>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="73"/>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="73"/>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="73"/>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="73"/>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="73"/>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="73"/>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="73"/>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="73"/>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="73"/>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="73"/>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="73"/>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="73"/>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="73"/>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="73"/>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="73"/>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="73"/>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="73"/>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="73"/>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="73"/>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" s="73"/>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="73"/>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="73"/>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" s="73"/>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="73"/>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" s="73"/>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" s="73"/>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" s="73"/>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" s="73"/>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" s="73"/>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" s="73"/>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" s="73"/>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" s="73"/>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" s="73"/>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" s="73"/>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" s="73"/>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" s="73"/>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" s="73"/>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" s="73"/>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" s="73"/>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" s="73"/>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" s="73"/>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" s="73"/>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" s="73"/>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" s="73"/>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" s="73"/>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219" s="73"/>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" s="73"/>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" s="73"/>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" s="73"/>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223" s="73"/>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" s="73"/>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" s="73"/>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" s="73"/>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" s="73"/>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" s="73"/>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" s="73"/>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" s="73"/>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" s="73"/>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" s="73"/>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" s="73"/>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" s="73"/>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" s="73"/>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" s="73"/>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" s="73"/>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238" s="73"/>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239" s="73"/>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240" s="73"/>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241" s="73"/>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242" s="73"/>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243" s="73"/>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244" s="73"/>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245" s="73"/>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246" s="73"/>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247" s="73"/>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248" s="73"/>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249" s="73"/>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250" s="73"/>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251" s="73"/>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252" s="73"/>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A253" s="73"/>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A254" s="73"/>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255" s="73"/>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A256" s="73"/>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257" s="73"/>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258" s="73"/>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259" s="73"/>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A260" s="73"/>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261" s="73"/>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262" s="73"/>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A263" s="73"/>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264" s="73"/>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A265" s="73"/>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A266" s="73"/>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A267" s="73"/>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A268" s="73"/>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A269" s="73"/>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A270" s="73"/>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A271" s="73"/>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A272" s="73"/>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A273" s="73"/>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A274" s="73"/>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A275" s="73"/>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A276" s="73"/>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A277" s="73"/>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A278" s="73"/>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A279" s="73"/>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A280" s="73"/>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A281" s="73"/>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A282" s="73"/>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A283" s="73"/>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A284" s="73"/>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A285" s="73"/>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A286" s="73"/>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A287" s="73"/>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A288" s="73"/>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A289" s="73"/>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A290" s="73"/>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A291" s="73"/>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A292" s="73"/>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A293" s="73"/>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A294" s="73"/>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A295" s="73"/>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A296" s="73"/>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A297" s="73"/>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A298" s="73"/>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A299" s="73"/>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A300" s="73"/>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A301" s="73"/>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A302" s="73"/>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A303" s="73"/>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A304" s="73"/>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A305" s="73"/>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A306" s="73"/>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A307" s="73"/>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A308" s="73"/>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A309" s="73"/>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A310" s="73"/>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A311" s="73"/>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A312" s="73"/>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A313" s="73"/>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A314" s="73"/>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A315" s="73"/>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A316" s="73"/>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A317" s="73"/>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A318" s="73"/>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A319" s="73"/>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A320" s="73"/>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A321" s="73"/>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A322" s="73"/>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A323" s="73"/>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A324" s="73"/>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A325" s="73"/>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A326" s="73"/>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A327" s="73"/>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A328" s="73"/>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A329" s="73"/>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A330" s="73"/>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A331" s="73"/>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A332" s="73"/>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A333" s="73"/>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A334" s="73"/>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A335" s="73"/>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A336" s="73"/>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A337" s="73"/>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A338" s="73"/>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A339" s="73"/>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A340" s="73"/>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A341" s="73"/>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A342" s="73"/>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A343" s="73"/>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A344" s="73"/>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A345" s="73"/>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A346" s="73"/>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A347" s="73"/>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A348" s="73"/>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A349" s="73"/>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A350" s="73"/>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A351" s="73"/>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A352" s="73"/>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A353" s="73"/>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A354" s="73"/>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A355" s="73"/>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A356" s="73"/>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A357" s="73"/>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A358" s="73"/>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A359" s="73"/>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A360" s="73"/>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A361" s="73"/>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A362" s="73"/>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A363" s="73"/>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A364" s="73"/>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A365" s="73"/>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A366" s="73"/>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A367" s="73"/>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A368" s="73"/>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A369" s="73"/>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A370" s="73"/>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A371" s="73"/>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A372" s="73"/>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A373" s="73"/>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A374" s="73"/>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A375" s="73"/>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A376" s="73"/>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A377" s="73"/>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A378" s="73"/>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A379" s="73"/>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A380" s="73"/>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A381" s="73"/>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A382" s="73"/>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A383" s="73"/>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A384" s="73"/>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A385" s="73"/>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A386" s="73"/>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A387" s="73"/>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A388" s="73"/>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A389" s="73"/>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A390" s="73"/>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A391" s="73"/>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A392" s="73"/>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A393" s="73"/>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A394" s="73"/>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A395" s="73"/>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A396" s="73"/>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A397" s="73"/>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A398" s="73"/>
+    </row>
+    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A399" s="73"/>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A400" s="73"/>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A401" s="73"/>
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A402" s="73"/>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A403" s="73"/>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A404" s="73"/>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A405" s="73"/>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A406" s="73"/>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A407" s="73"/>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A408" s="73"/>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A409" s="73"/>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A410" s="73"/>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A411" s="73"/>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A412" s="73"/>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A413" s="73"/>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A414" s="73"/>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A415" s="73"/>
+    </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A416" s="73"/>
+    </row>
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A417" s="73"/>
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A418" s="73"/>
+    </row>
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A419" s="73"/>
+    </row>
+    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A420" s="73"/>
+    </row>
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A421" s="73"/>
+    </row>
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A422" s="73"/>
+    </row>
+    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A423" s="73"/>
+    </row>
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A424" s="73"/>
+    </row>
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A425" s="73"/>
+    </row>
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A426" s="73"/>
+    </row>
+    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A427" s="73"/>
+    </row>
+    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A428" s="73"/>
+    </row>
+    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A429" s="73"/>
+    </row>
+    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A430" s="73"/>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A431" s="73"/>
+    </row>
+    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A432" s="73"/>
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A433" s="73"/>
+    </row>
+    <row r="434" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A434" s="73"/>
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A435" s="73"/>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A436" s="73"/>
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A437" s="73"/>
+    </row>
+    <row r="438" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A438" s="73"/>
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A439" s="73"/>
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A440" s="73"/>
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A441" s="73"/>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A442" s="73"/>
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A443" s="73"/>
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A444" s="73"/>
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A445" s="73"/>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A446" s="73"/>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A447" s="73"/>
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A448" s="73"/>
+    </row>
+    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A449" s="73"/>
+    </row>
+    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A450" s="73"/>
+    </row>
+    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A451" s="73"/>
+    </row>
+    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A452" s="73"/>
+    </row>
+    <row r="453" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A453" s="73"/>
+    </row>
+    <row r="454" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A454" s="73"/>
+    </row>
+    <row r="455" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A455" s="73"/>
+    </row>
+    <row r="456" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A456" s="73"/>
+    </row>
+    <row r="457" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A457" s="73"/>
+    </row>
+    <row r="458" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A458" s="73"/>
+    </row>
+    <row r="459" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A459" s="73"/>
+    </row>
+    <row r="460" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A460" s="73"/>
+    </row>
+    <row r="461" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A461" s="73"/>
+    </row>
+    <row r="462" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A462" s="73"/>
+    </row>
+    <row r="463" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A463" s="73"/>
+    </row>
+    <row r="464" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A464" s="73"/>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A465" s="73"/>
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A466" s="73"/>
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A467" s="73"/>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A468" s="73"/>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A469" s="73"/>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A470" s="73"/>
+    </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A471" s="73"/>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finaliza jornada QH 23-12-2014
</commit_message>
<xml_diff>
--- a/Documentacion/indicadores revisión junio 11 2014.xlsx
+++ b/Documentacion/indicadores revisión junio 11 2014.xlsx
@@ -217,33 +217,6 @@
   </si>
   <si>
     <t>AE=    X / (P+M-X)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Donde M= importaciones, P = producción y X= exportaciones.               </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Las variables se deben calcular con respecto a VOL. (Cantidades) NO valores en $</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.  Fuente: EVA</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">   
@@ -1253,15 +1226,42 @@
   <si>
     <t>1208100000</t>
   </si>
+  <si>
+    <r>
+      <t>Donde M= importaciones, P = producción y X= exportaciones.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Las variables se deben calcular con respecto a VOL. (Cantidades) NO valores en $</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.  Fuente: EVA</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.000%"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -1549,7 +1549,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="76">
@@ -1677,16 +1677,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1704,7 +1704,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1734,7 +1734,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3481,10 +3481,10 @@
   <dimension ref="B1:R41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3526,31 +3526,31 @@
         <v>6</v>
       </c>
       <c r="J2" s="48" t="s">
+        <v>145</v>
+      </c>
+      <c r="K2" s="48" t="s">
+        <v>154</v>
+      </c>
+      <c r="L2" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="M2" s="48" t="s">
+        <v>157</v>
+      </c>
+      <c r="N2" s="48" t="s">
         <v>146</v>
       </c>
-      <c r="K2" s="48" t="s">
-        <v>155</v>
-      </c>
-      <c r="L2" s="48" t="s">
+      <c r="O2" s="48" t="s">
+        <v>151</v>
+      </c>
+      <c r="P2" s="48" t="s">
         <v>148</v>
       </c>
-      <c r="M2" s="48" t="s">
-        <v>158</v>
-      </c>
-      <c r="N2" s="48" t="s">
-        <v>147</v>
-      </c>
-      <c r="O2" s="48" t="s">
+      <c r="Q2" s="48" t="s">
+        <v>149</v>
+      </c>
+      <c r="R2" s="48" t="s">
         <v>152</v>
-      </c>
-      <c r="P2" s="48" t="s">
-        <v>149</v>
-      </c>
-      <c r="Q2" s="48" t="s">
-        <v>150</v>
-      </c>
-      <c r="R2" s="48" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="3" spans="2:18" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3579,28 +3579,28 @@
         <v>14</v>
       </c>
       <c r="J3" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K3" s="21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L3" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M3" s="21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N3" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O3" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P3" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Q3" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R3" s="21"/>
     </row>
@@ -3622,28 +3622,28 @@
       <c r="H4" s="73"/>
       <c r="I4" s="73"/>
       <c r="J4" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K4" s="21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L4" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M4" s="21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N4" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O4" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P4" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Q4" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R4" s="21"/>
     </row>
@@ -3667,28 +3667,28 @@
       <c r="H5" s="73"/>
       <c r="I5" s="73"/>
       <c r="J5" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K5" s="21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L5" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M5" s="21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N5" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O5" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P5" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Q5" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R5" s="21"/>
     </row>
@@ -3718,266 +3718,266 @@
         <v>31</v>
       </c>
       <c r="J6" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K6" s="21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L6" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M6" s="21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N6" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O6" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P6" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Q6" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R6" s="21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="2:18" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="50" t="s">
         <v>32</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>33</v>
       </c>
       <c r="D7" s="22" t="s">
+        <v>237</v>
+      </c>
+      <c r="E7" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="F7" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="G7" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="H7" s="22" t="s">
         <v>37</v>
-      </c>
-      <c r="H7" s="22" t="s">
-        <v>38</v>
       </c>
       <c r="I7" s="22" t="s">
         <v>31</v>
       </c>
       <c r="J7" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K7" s="21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L7" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M7" s="21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N7" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O7" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P7" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Q7" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R7" s="21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="2:18" ht="114" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="D8" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="E8" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="F8" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="G8" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="H8" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="I8" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="I8" s="22" t="s">
-        <v>46</v>
-      </c>
       <c r="J8" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K8" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L8" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M8" s="21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N8" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O8" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P8" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Q8" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R8" s="21"/>
     </row>
     <row r="9" spans="2:18" s="26" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="56" t="s">
+      <c r="D9" s="57" t="s">
+        <v>156</v>
+      </c>
+      <c r="E9" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="57" t="s">
-        <v>157</v>
-      </c>
-      <c r="E9" s="32" t="s">
+      <c r="F9" s="32" t="s">
         <v>49</v>
-      </c>
-      <c r="F9" s="32" t="s">
-        <v>50</v>
       </c>
       <c r="G9" s="33" t="s">
         <v>12</v>
       </c>
       <c r="H9" s="33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I9" s="33" t="s">
         <v>31</v>
       </c>
       <c r="J9" s="56" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K9" s="56" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L9" s="56" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M9" s="56" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N9" s="56" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O9" s="56" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P9" s="56" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Q9" s="56" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R9" s="56"/>
     </row>
     <row r="10" spans="2:18" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="D10" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="E10" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="F10" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="G10" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="G10" s="22" t="s">
+      <c r="H10" s="14" t="s">
         <v>57</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>58</v>
       </c>
       <c r="I10" s="24" t="s">
         <v>31</v>
       </c>
       <c r="J10" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K10" s="21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L10" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M10" s="21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N10" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O10" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P10" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Q10" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R10" s="21"/>
     </row>
     <row r="11" spans="2:18" s="26" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="D11" s="75" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="75" t="s">
+      <c r="E11" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="68" t="s">
+      <c r="F11" s="75" t="s">
         <v>62</v>
       </c>
-      <c r="F11" s="75" t="s">
+      <c r="G11" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="75" t="s">
-        <v>64</v>
-      </c>
       <c r="H11" s="68" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I11" s="68" t="s">
         <v>31</v>
       </c>
       <c r="J11" s="26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K11" s="26">
         <v>15</v>
@@ -3992,10 +3992,10 @@
     </row>
     <row r="12" spans="2:18" s="26" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="51" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="25" t="s">
         <v>65</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>66</v>
       </c>
       <c r="D12" s="75"/>
       <c r="E12" s="68"/>
@@ -4004,7 +4004,7 @@
       <c r="H12" s="68"/>
       <c r="I12" s="68"/>
       <c r="J12" s="26" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K12" s="26">
         <v>1500000</v>
@@ -4023,109 +4023,109 @@
     </row>
     <row r="13" spans="2:18" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="D13" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="E13" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="F13" s="16" t="s">
         <v>70</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>71</v>
       </c>
       <c r="G13" s="22" t="s">
         <v>29</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I13" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="2:18" ht="144" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="50" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="D14" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="E14" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="F14" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="G14" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="G14" s="22" t="s">
+      <c r="H14" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="H14" s="22" t="s">
-        <v>79</v>
-      </c>
       <c r="I14" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J14" s="54" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="2:18" ht="144" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="D15" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="E15" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="F15" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F15" s="18" t="s">
-        <v>84</v>
-      </c>
       <c r="G15" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I15" s="24" t="s">
         <v>31</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="2:18" ht="89.25" x14ac:dyDescent="0.2">
       <c r="B16" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="D16" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="E16" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="F16" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="F16" s="16" t="s">
+      <c r="G16" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="G16" s="24" t="s">
-        <v>90</v>
-      </c>
       <c r="H16" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I16" s="22" t="s">
         <v>31</v>
@@ -4133,25 +4133,25 @@
     </row>
     <row r="17" spans="2:9" ht="153" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="D17" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="E17" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="F17" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="G17" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="G17" s="22" t="s">
-        <v>96</v>
-      </c>
       <c r="H17" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I17" s="22" t="s">
         <v>31</v>
@@ -4159,25 +4159,25 @@
     </row>
     <row r="18" spans="2:9" s="26" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="D18" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="D18" s="30" t="s">
+      <c r="E18" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="F18" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="F18" s="32" t="s">
-        <v>101</v>
-      </c>
       <c r="G18" s="33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H18" s="33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I18" s="33" t="s">
         <v>31</v>
@@ -4185,25 +4185,25 @@
     </row>
     <row r="19" spans="2:9" s="26" customFormat="1" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="62" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="D19" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="D19" s="34" t="s">
+      <c r="E19" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="E19" s="34" t="s">
+      <c r="F19" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="F19" s="31" t="s">
+      <c r="G19" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="G19" s="33" t="s">
+      <c r="H19" s="33" t="s">
         <v>107</v>
-      </c>
-      <c r="H19" s="33" t="s">
-        <v>108</v>
       </c>
       <c r="I19" s="24" t="s">
         <v>31</v>
@@ -4211,25 +4211,25 @@
     </row>
     <row r="20" spans="2:9" s="26" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="62" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="D20" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="E20" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="E20" s="34" t="s">
+      <c r="F20" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="F20" s="34" t="s">
-        <v>113</v>
-      </c>
       <c r="G20" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="H20" s="33" t="s">
         <v>107</v>
-      </c>
-      <c r="H20" s="33" t="s">
-        <v>108</v>
       </c>
       <c r="I20" s="24" t="s">
         <v>31</v>
@@ -4237,25 +4237,25 @@
     </row>
     <row r="21" spans="2:9" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="62" t="s">
+        <v>113</v>
+      </c>
+      <c r="C21" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="C21" s="35" t="s">
+      <c r="D21" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="D21" s="36" t="s">
+      <c r="E21" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="E21" s="37" t="s">
+      <c r="F21" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="F21" s="38" t="s">
-        <v>118</v>
-      </c>
       <c r="G21" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="H21" s="14" t="s">
         <v>57</v>
-      </c>
-      <c r="H21" s="14" t="s">
-        <v>58</v>
       </c>
       <c r="I21" s="24" t="s">
         <v>31</v>
@@ -4263,25 +4263,25 @@
     </row>
     <row r="22" spans="2:9" s="26" customFormat="1" ht="137.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="60" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="D22" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="D22" s="39" t="s">
+      <c r="E22" s="37" t="s">
         <v>121</v>
       </c>
-      <c r="E22" s="37" t="s">
+      <c r="F22" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="F22" s="34" t="s">
-        <v>123</v>
-      </c>
       <c r="G22" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="H22" s="29" t="s">
         <v>57</v>
-      </c>
-      <c r="H22" s="29" t="s">
-        <v>58</v>
       </c>
       <c r="I22" s="39" t="s">
         <v>31</v>
@@ -4289,25 +4289,25 @@
     </row>
     <row r="23" spans="2:9" s="26" customFormat="1" ht="137.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="61" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C23" s="58" t="s">
+        <v>123</v>
+      </c>
+      <c r="D23" s="39" t="s">
         <v>124</v>
       </c>
-      <c r="D23" s="39" t="s">
+      <c r="E23" s="39" t="s">
         <v>125</v>
       </c>
-      <c r="E23" s="39" t="s">
+      <c r="F23" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="F23" s="32" t="s">
-        <v>127</v>
-      </c>
       <c r="G23" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="H23" s="58" t="s">
         <v>57</v>
-      </c>
-      <c r="H23" s="58" t="s">
-        <v>58</v>
       </c>
       <c r="I23" s="39" t="s">
         <v>31</v>
@@ -4315,25 +4315,25 @@
     </row>
     <row r="24" spans="2:9" s="26" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="D24" s="33" t="s">
         <v>129</v>
       </c>
-      <c r="D24" s="33" t="s">
+      <c r="E24" s="32" t="s">
         <v>130</v>
       </c>
-      <c r="E24" s="32" t="s">
+      <c r="F24" s="32" t="s">
         <v>131</v>
-      </c>
-      <c r="F24" s="32" t="s">
-        <v>132</v>
       </c>
       <c r="G24" s="33" t="s">
         <v>12</v>
       </c>
       <c r="H24" s="33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I24" s="33" t="s">
         <v>31</v>
@@ -4341,51 +4341,51 @@
     </row>
     <row r="25" spans="2:9" s="26" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="C25" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="C25" s="29" t="s">
+      <c r="D25" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="D25" s="24" t="s">
+      <c r="E25" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="E25" s="33" t="s">
+      <c r="F25" s="32" t="s">
         <v>137</v>
-      </c>
-      <c r="F25" s="32" t="s">
-        <v>138</v>
       </c>
       <c r="G25" s="33" t="s">
         <v>12</v>
       </c>
       <c r="H25" s="33" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I25" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="2:9" ht="102.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="55" t="s">
+        <v>139</v>
+      </c>
+      <c r="C26" s="41" t="s">
         <v>140</v>
       </c>
-      <c r="C26" s="41" t="s">
+      <c r="D26" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="D26" s="24" t="s">
+      <c r="E26" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="E26" s="39" t="s">
+      <c r="F26" s="42" t="s">
         <v>143</v>
       </c>
-      <c r="F26" s="42" t="s">
+      <c r="G26" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="H26" s="43" t="s">
         <v>144</v>
-      </c>
-      <c r="G26" s="43" t="s">
-        <v>78</v>
-      </c>
-      <c r="H26" s="43" t="s">
-        <v>145</v>
       </c>
       <c r="I26" s="43" t="s">
         <v>31</v>
@@ -4454,10 +4454,10 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="52" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="52" t="s">
         <v>161</v>
-      </c>
-      <c r="B1" s="52" t="s">
-        <v>162</v>
       </c>
       <c r="C1" s="52">
         <v>2012</v>
@@ -4469,25 +4469,25 @@
         <v>2014</v>
       </c>
       <c r="F1" s="52" t="s">
+        <v>162</v>
+      </c>
+      <c r="G1" s="52" t="s">
         <v>163</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="H1" s="52" t="s">
         <v>164</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="I1" s="52" t="s">
         <v>165</v>
       </c>
-      <c r="I1" s="52" t="s">
+      <c r="J1" s="52" t="s">
         <v>166</v>
       </c>
-      <c r="J1" s="52" t="s">
+      <c r="K1" s="52" t="s">
         <v>167</v>
       </c>
-      <c r="K1" s="52" t="s">
+      <c r="L1" s="52" t="s">
         <v>168</v>
-      </c>
-      <c r="L1" s="52" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -5594,22 +5594,22 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="52" t="s">
+        <v>172</v>
+      </c>
+      <c r="B30" s="52" t="s">
         <v>173</v>
       </c>
-      <c r="B30" s="52" t="s">
+      <c r="C30" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="C30" s="52" t="s">
+      <c r="H30" t="s">
+        <v>148</v>
+      </c>
+      <c r="I30" t="s">
         <v>175</v>
       </c>
-      <c r="H30" t="s">
-        <v>149</v>
-      </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>176</v>
-      </c>
-      <c r="J30" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -5644,13 +5644,13 @@
         <v>204.75</v>
       </c>
       <c r="H32" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I32" t="s">
+        <v>175</v>
+      </c>
+      <c r="J32" t="s">
         <v>176</v>
-      </c>
-      <c r="J32" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -5722,103 +5722,103 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="66" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B2" s="63" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B3" s="64" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="66" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B4" s="64" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="66" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B5" s="64" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="66" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B6" s="64" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="66" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B7" s="64" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="66" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B8" s="64" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="66" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B9" s="64" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="66" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B10" s="64" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="66" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B11" s="64" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="66" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B12" s="64" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="66" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B13" s="64" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H13">
         <v>2010</v>
@@ -5835,10 +5835,10 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="66" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B14" s="64" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H14">
         <v>2011</v>
@@ -5855,10 +5855,10 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="66" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B15" s="64" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H15">
         <v>2012</v>
@@ -5875,10 +5875,10 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="66" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B16" s="64" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H16">
         <v>2013</v>
@@ -5895,77 +5895,77 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="66" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B17" s="64" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="66" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B18" s="64" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="66" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B19" s="64" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="66" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B20" s="64" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="66" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B21" s="64" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="66" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B22" s="64" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="66" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B23" s="64" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="66" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B24" s="64" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="66" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B25" s="64" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I25">
         <f>FIND("-",H25)</f>
@@ -5982,10 +5982,10 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="66" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B26" s="64" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I26" t="e">
         <f t="shared" ref="I26:I75" si="0">FIND("-",H26)</f>
@@ -6002,13 +6002,13 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="66" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B27" s="64" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H27" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I27">
         <f t="shared" si="0"/>
@@ -6025,10 +6025,10 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="66" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B28" s="64" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I28" t="e">
         <f t="shared" si="0"/>
@@ -6045,13 +6045,13 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="66" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B29" s="64" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H29" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I29">
         <f t="shared" si="0"/>
@@ -6068,10 +6068,10 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="66" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B30" s="64" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I30" t="e">
         <f t="shared" si="0"/>
@@ -6088,13 +6088,13 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="66" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B31" s="64" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H31" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I31">
         <f t="shared" si="0"/>
@@ -6111,10 +6111,10 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="66" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B32" s="64" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I32" t="e">
         <f t="shared" si="0"/>
@@ -6131,13 +6131,13 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="66" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B33" s="64" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I33">
         <f t="shared" si="0"/>
@@ -6154,10 +6154,10 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="66" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B34" s="64" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I34" t="e">
         <f t="shared" si="0"/>
@@ -6174,13 +6174,13 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="66" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B35" s="64" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H35" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I35">
         <f t="shared" si="0"/>
@@ -6197,10 +6197,10 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="66" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B36" s="64" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I36" t="e">
         <f t="shared" si="0"/>
@@ -6217,13 +6217,13 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="66" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B37" s="64" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H37" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I37">
         <f t="shared" si="0"/>
@@ -6240,7 +6240,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="66" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I38" t="e">
         <f t="shared" si="0"/>
@@ -6257,10 +6257,10 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="66" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H39" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I39">
         <f t="shared" si="0"/>
@@ -6277,7 +6277,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="66" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I40" t="e">
         <f t="shared" si="0"/>
@@ -6294,10 +6294,10 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="66" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H41" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I41">
         <f t="shared" si="0"/>
@@ -6314,7 +6314,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="66" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I42" t="e">
         <f t="shared" si="0"/>
@@ -6331,7 +6331,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="66" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I43" t="e">
         <f t="shared" si="0"/>
@@ -6348,7 +6348,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="66" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I44" t="e">
         <f t="shared" si="0"/>
@@ -6365,10 +6365,10 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="66" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H45" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I45">
         <f t="shared" si="0"/>
@@ -6385,7 +6385,7 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="66" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I46" t="e">
         <f t="shared" si="0"/>
@@ -6402,10 +6402,10 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="66" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H47" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I47">
         <f t="shared" si="0"/>
@@ -6422,7 +6422,7 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="66" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I48" t="e">
         <f t="shared" si="0"/>
@@ -6439,10 +6439,10 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="66" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H49" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I49">
         <f t="shared" si="0"/>
@@ -6459,7 +6459,7 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="66" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I50" t="e">
         <f t="shared" si="0"/>
@@ -6476,10 +6476,10 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="66" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H51" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I51">
         <f t="shared" si="0"/>
@@ -6496,7 +6496,7 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="66" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I52" t="e">
         <f t="shared" si="0"/>
@@ -6513,10 +6513,10 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="66" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H53" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I53">
         <f t="shared" si="0"/>
@@ -6533,7 +6533,7 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="66" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I54" t="e">
         <f t="shared" si="0"/>
@@ -6550,10 +6550,10 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="66" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H55" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I55">
         <f t="shared" si="0"/>
@@ -6570,7 +6570,7 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="66" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I56" t="e">
         <f t="shared" si="0"/>
@@ -6587,10 +6587,10 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="66" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H57" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I57">
         <f t="shared" si="0"/>
@@ -6607,7 +6607,7 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="66" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I58" t="e">
         <f t="shared" si="0"/>
@@ -6624,7 +6624,7 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="66" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I59" t="e">
         <f t="shared" si="0"/>
@@ -6641,7 +6641,7 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="66" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I60" t="e">
         <f t="shared" si="0"/>
@@ -6658,10 +6658,10 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="66" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H61" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I61">
         <f t="shared" si="0"/>
@@ -6678,7 +6678,7 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="66" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I62" t="e">
         <f t="shared" si="0"/>
@@ -6695,10 +6695,10 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="66" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H63" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I63">
         <f t="shared" si="0"/>
@@ -6715,7 +6715,7 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="66" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I64" t="e">
         <f t="shared" si="0"/>
@@ -6732,10 +6732,10 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="66" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H65" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I65">
         <f t="shared" si="0"/>
@@ -6752,7 +6752,7 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="66" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I66" t="e">
         <f t="shared" si="0"/>
@@ -6769,10 +6769,10 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="66" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H67" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I67">
         <f t="shared" si="0"/>
@@ -6805,7 +6805,7 @@
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="65"/>
       <c r="H69" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I69">
         <f t="shared" si="0"/>
@@ -6838,7 +6838,7 @@
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="65"/>
       <c r="H71" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I71">
         <f t="shared" si="0"/>
@@ -6901,7 +6901,7 @@
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="65"/>
       <c r="H75" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I75">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
finaliza jornada QH 29-12-2014
</commit_message>
<xml_diff>
--- a/Documentacion/indicadores revisión junio 11 2014.xlsx
+++ b/Documentacion/indicadores revisión junio 11 2014.xlsx
@@ -3481,10 +3481,10 @@
   <dimension ref="B1:R41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
finaliza jornada QH 30-12-2014
</commit_message>
<xml_diff>
--- a/Documentacion/indicadores revisión junio 11 2014.xlsx
+++ b/Documentacion/indicadores revisión junio 11 2014.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Hoja2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ajustes!$B$2:$I$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ajustes!$A$2:$R$26</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Ajustes!$B$1:$I$26</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="239">
   <si>
     <t>NOMBRE INDICADOR</t>
   </si>
@@ -1252,6 +1252,9 @@
       </rPr>
       <t>.  Fuente: EVA</t>
     </r>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -1552,7 +1555,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1665,9 +1668,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1760,6 +1760,15 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3478,13 +3487,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:R41"/>
+  <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3501,15 +3510,18 @@
     <col min="10" max="16384" width="11.42578125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:18" s="10" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:18" s="10" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>238</v>
+      </c>
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="69" t="s">
+      <c r="C2" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="69"/>
+      <c r="D2" s="68"/>
       <c r="E2" s="8" t="s">
         <v>2</v>
       </c>
@@ -3525,36 +3537,39 @@
       <c r="I2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="48" t="s">
+      <c r="J2" s="47" t="s">
         <v>145</v>
       </c>
-      <c r="K2" s="48" t="s">
+      <c r="K2" s="47" t="s">
         <v>154</v>
       </c>
-      <c r="L2" s="48" t="s">
+      <c r="L2" s="47" t="s">
         <v>147</v>
       </c>
-      <c r="M2" s="48" t="s">
+      <c r="M2" s="47" t="s">
         <v>157</v>
       </c>
-      <c r="N2" s="48" t="s">
+      <c r="N2" s="47" t="s">
         <v>146</v>
       </c>
-      <c r="O2" s="48" t="s">
+      <c r="O2" s="47" t="s">
         <v>151</v>
       </c>
-      <c r="P2" s="48" t="s">
+      <c r="P2" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="Q2" s="48" t="s">
+      <c r="Q2" s="47" t="s">
         <v>149</v>
       </c>
-      <c r="R2" s="48" t="s">
+      <c r="R2" s="47" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="2:18" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="49" t="s">
+    <row r="3" spans="1:18" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="76">
+        <v>1</v>
+      </c>
+      <c r="B3" s="48" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="11" t="s">
@@ -3566,16 +3581,16 @@
       <c r="E3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="70" t="s">
+      <c r="F3" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="72" t="s">
+      <c r="G3" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="72" t="s">
+      <c r="H3" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="74" t="s">
+      <c r="I3" s="73" t="s">
         <v>14</v>
       </c>
       <c r="J3" s="21" t="s">
@@ -3604,8 +3619,11 @@
       </c>
       <c r="R3" s="21"/>
     </row>
-    <row r="4" spans="2:18" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="50" t="s">
+    <row r="4" spans="1:18" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="76">
+        <v>2</v>
+      </c>
+      <c r="B4" s="49" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="14" t="s">
@@ -3617,10 +3635,10 @@
       <c r="E4" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="71"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="72"/>
       <c r="J4" s="21" t="s">
         <v>150</v>
       </c>
@@ -3647,8 +3665,11 @@
       </c>
       <c r="R4" s="21"/>
     </row>
-    <row r="5" spans="2:18" ht="104.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="51" t="s">
+    <row r="5" spans="1:18" ht="104.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="76">
+        <v>3</v>
+      </c>
+      <c r="B5" s="50" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="14" t="s">
@@ -3663,9 +3684,9 @@
       <c r="F5" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="72"/>
       <c r="J5" s="21" t="s">
         <v>150</v>
       </c>
@@ -3692,8 +3713,11 @@
       </c>
       <c r="R5" s="21"/>
     </row>
-    <row r="6" spans="2:18" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="50" t="s">
+    <row r="6" spans="1:18" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="76">
+        <v>18</v>
+      </c>
+      <c r="B6" s="49" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="21" t="s">
@@ -3745,8 +3769,11 @@
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="2:18" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="50" t="s">
+    <row r="7" spans="1:18" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="76">
+        <v>19</v>
+      </c>
+      <c r="B7" s="49" t="s">
         <v>32</v>
       </c>
       <c r="C7" s="14" t="s">
@@ -3798,8 +3825,11 @@
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="2:18" ht="114" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="51" t="s">
+    <row r="8" spans="1:18" ht="114" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="76">
+        <v>8</v>
+      </c>
+      <c r="B8" s="50" t="s">
         <v>38</v>
       </c>
       <c r="C8" s="23" t="s">
@@ -3849,14 +3879,15 @@
       </c>
       <c r="R8" s="21"/>
     </row>
-    <row r="9" spans="2:18" s="26" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" s="26" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="77"/>
       <c r="B9" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="56" t="s">
+      <c r="C9" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="57" t="s">
+      <c r="D9" s="56" t="s">
         <v>156</v>
       </c>
       <c r="E9" s="32" t="s">
@@ -3874,34 +3905,37 @@
       <c r="I9" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="J9" s="56" t="s">
+      <c r="J9" s="55" t="s">
         <v>150</v>
       </c>
-      <c r="K9" s="56" t="s">
+      <c r="K9" s="55" t="s">
         <v>155</v>
       </c>
-      <c r="L9" s="56" t="s">
+      <c r="L9" s="55" t="s">
         <v>150</v>
       </c>
-      <c r="M9" s="56" t="s">
+      <c r="M9" s="55" t="s">
         <v>155</v>
       </c>
-      <c r="N9" s="56" t="s">
+      <c r="N9" s="55" t="s">
         <v>150</v>
       </c>
-      <c r="O9" s="56" t="s">
+      <c r="O9" s="55" t="s">
         <v>150</v>
       </c>
-      <c r="P9" s="56" t="s">
+      <c r="P9" s="55" t="s">
         <v>150</v>
       </c>
-      <c r="Q9" s="56" t="s">
+      <c r="Q9" s="55" t="s">
         <v>150</v>
       </c>
-      <c r="R9" s="56"/>
-    </row>
-    <row r="10" spans="2:18" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="50" t="s">
+      <c r="R9" s="55"/>
+    </row>
+    <row r="10" spans="1:18" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="76">
+        <v>4</v>
+      </c>
+      <c r="B10" s="49" t="s">
         <v>51</v>
       </c>
       <c r="C10" s="14" t="s">
@@ -3951,29 +3985,32 @@
       </c>
       <c r="R10" s="21"/>
     </row>
-    <row r="11" spans="2:18" s="26" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="51" t="s">
+    <row r="11" spans="1:18" s="26" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="77">
+        <v>5</v>
+      </c>
+      <c r="B11" s="50" t="s">
         <v>58</v>
       </c>
       <c r="C11" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="75" t="s">
+      <c r="D11" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="68" t="s">
+      <c r="E11" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="F11" s="75" t="s">
+      <c r="F11" s="74" t="s">
         <v>62</v>
       </c>
-      <c r="G11" s="75" t="s">
+      <c r="G11" s="74" t="s">
         <v>63</v>
       </c>
-      <c r="H11" s="68" t="s">
+      <c r="H11" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="I11" s="68" t="s">
+      <c r="I11" s="67" t="s">
         <v>31</v>
       </c>
       <c r="J11" s="26" t="s">
@@ -3990,19 +4027,22 @@
         <v>500000000</v>
       </c>
     </row>
-    <row r="12" spans="2:18" s="26" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="51" t="s">
+    <row r="12" spans="1:18" s="26" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="77">
+        <v>6</v>
+      </c>
+      <c r="B12" s="50" t="s">
         <v>64</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="75"/>
-      <c r="E12" s="68"/>
-      <c r="F12" s="75"/>
-      <c r="G12" s="75"/>
-      <c r="H12" s="68"/>
-      <c r="I12" s="68"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="74"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="67"/>
       <c r="J12" s="26" t="s">
         <v>159</v>
       </c>
@@ -4021,8 +4061,11 @@
         <v>-477500000</v>
       </c>
     </row>
-    <row r="13" spans="2:18" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="50" t="s">
+    <row r="13" spans="1:18" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="76">
+        <v>7</v>
+      </c>
+      <c r="B13" s="49" t="s">
         <v>66</v>
       </c>
       <c r="C13" s="14" t="s">
@@ -4047,8 +4090,11 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="2:18" ht="144" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="50" t="s">
+    <row r="14" spans="1:18" ht="144" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="76">
+        <v>9</v>
+      </c>
+      <c r="B14" s="49" t="s">
         <v>72</v>
       </c>
       <c r="C14" s="14" t="s">
@@ -4072,12 +4118,15 @@
       <c r="I14" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="J14" s="54" t="s">
+      <c r="J14" s="53" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="15" spans="2:18" ht="144" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="51" t="s">
+    <row r="15" spans="1:18" ht="144" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="76">
+        <v>10</v>
+      </c>
+      <c r="B15" s="50" t="s">
         <v>79</v>
       </c>
       <c r="C15" s="14" t="s">
@@ -4105,8 +4154,11 @@
         <v>170</v>
       </c>
     </row>
-    <row r="16" spans="2:18" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="B16" s="51" t="s">
+    <row r="16" spans="1:18" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="76">
+        <v>11</v>
+      </c>
+      <c r="B16" s="50" t="s">
         <v>84</v>
       </c>
       <c r="C16" s="28" t="s">
@@ -4131,8 +4183,11 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="153" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="50" t="s">
+    <row r="17" spans="1:9" ht="153" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="77">
+        <v>12</v>
+      </c>
+      <c r="B17" s="49" t="s">
         <v>90</v>
       </c>
       <c r="C17" s="29" t="s">
@@ -4157,8 +4212,11 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="2:9" s="26" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="51" t="s">
+    <row r="18" spans="1:9" s="26" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="77">
+        <v>13</v>
+      </c>
+      <c r="B18" s="50" t="s">
         <v>96</v>
       </c>
       <c r="C18" s="29" t="s">
@@ -4183,8 +4241,11 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="2:9" s="26" customFormat="1" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="62" t="s">
+    <row r="19" spans="1:9" s="26" customFormat="1" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="77">
+        <v>16</v>
+      </c>
+      <c r="B19" s="61" t="s">
         <v>101</v>
       </c>
       <c r="C19" s="34" t="s">
@@ -4209,8 +4270,11 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="2:9" s="26" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="62" t="s">
+    <row r="20" spans="1:9" s="26" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="77">
+        <v>17</v>
+      </c>
+      <c r="B20" s="61" t="s">
         <v>108</v>
       </c>
       <c r="C20" s="34" t="s">
@@ -4235,8 +4299,11 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="62" t="s">
+    <row r="21" spans="1:9" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="76">
+        <v>15</v>
+      </c>
+      <c r="B21" s="61" t="s">
         <v>113</v>
       </c>
       <c r="C21" s="35" t="s">
@@ -4261,8 +4328,11 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="2:9" s="26" customFormat="1" ht="137.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="60" t="s">
+    <row r="22" spans="1:9" s="26" customFormat="1" ht="137.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="77">
+        <v>14</v>
+      </c>
+      <c r="B22" s="59" t="s">
         <v>118</v>
       </c>
       <c r="C22" s="29" t="s">
@@ -4287,11 +4357,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="2:9" s="26" customFormat="1" ht="137.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="61" t="s">
+    <row r="23" spans="1:9" s="26" customFormat="1" ht="137.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="77">
+        <v>20</v>
+      </c>
+      <c r="B23" s="60" t="s">
         <v>171</v>
       </c>
-      <c r="C23" s="58" t="s">
+      <c r="C23" s="57" t="s">
         <v>123</v>
       </c>
       <c r="D23" s="39" t="s">
@@ -4306,15 +4379,18 @@
       <c r="G23" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="H23" s="58" t="s">
+      <c r="H23" s="57" t="s">
         <v>57</v>
       </c>
       <c r="I23" s="39" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="2:9" s="26" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="40" t="s">
+    <row r="24" spans="1:9" s="26" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="77">
+        <v>21</v>
+      </c>
+      <c r="B24" s="75" t="s">
         <v>127</v>
       </c>
       <c r="C24" s="29" t="s">
@@ -4339,8 +4415,11 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="2:9" s="26" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="20" t="s">
+    <row r="25" spans="1:9" s="26" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="77">
+        <v>21</v>
+      </c>
+      <c r="B25" s="49" t="s">
         <v>133</v>
       </c>
       <c r="C25" s="29" t="s">
@@ -4365,11 +4444,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="2:9" ht="102.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="55" t="s">
+    <row r="26" spans="1:9" ht="102.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="76"/>
+      <c r="B26" s="54" t="s">
         <v>139</v>
       </c>
-      <c r="C26" s="41" t="s">
+      <c r="C26" s="40" t="s">
         <v>140</v>
       </c>
       <c r="D26" s="24" t="s">
@@ -4378,44 +4458,44 @@
       <c r="E26" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="F26" s="42" t="s">
+      <c r="F26" s="41" t="s">
         <v>143</v>
       </c>
-      <c r="G26" s="43" t="s">
+      <c r="G26" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="H26" s="43" t="s">
+      <c r="H26" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="I26" s="43" t="s">
+      <c r="I26" s="42" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F34" s="44"/>
+      <c r="F34" s="43"/>
     </row>
     <row r="35" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D35" s="45"/>
-      <c r="F35" s="44"/>
+      <c r="D35" s="44"/>
+      <c r="F35" s="43"/>
     </row>
     <row r="36" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F36" s="44"/>
+      <c r="F36" s="43"/>
     </row>
     <row r="37" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F37" s="44"/>
+      <c r="F37" s="43"/>
     </row>
     <row r="38" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F38" s="46"/>
+      <c r="F38" s="45"/>
     </row>
     <row r="40" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F40" s="47"/>
+      <c r="F40" s="46"/>
     </row>
     <row r="41" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F41" s="46"/>
+      <c r="F41" s="45"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:I26">
-    <filterColumn colId="1" showButton="0"/>
+  <autoFilter ref="A2:R26">
+    <filterColumn colId="2" showButton="0"/>
   </autoFilter>
   <mergeCells count="11">
     <mergeCell ref="I11:I12"/>
@@ -4453,40 +4533,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="51" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="51" t="s">
         <v>161</v>
       </c>
-      <c r="C1" s="52">
+      <c r="C1" s="51">
         <v>2012</v>
       </c>
-      <c r="D1" s="52">
+      <c r="D1" s="51">
         <v>2013</v>
       </c>
-      <c r="E1" s="52">
+      <c r="E1" s="51">
         <v>2014</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="51" t="s">
         <v>162</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="G1" s="51" t="s">
         <v>163</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="51" t="s">
         <v>164</v>
       </c>
-      <c r="I1" s="52" t="s">
+      <c r="I1" s="51" t="s">
         <v>165</v>
       </c>
-      <c r="J1" s="52" t="s">
+      <c r="J1" s="51" t="s">
         <v>166</v>
       </c>
-      <c r="K1" s="52" t="s">
+      <c r="K1" s="51" t="s">
         <v>167</v>
       </c>
-      <c r="L1" s="52" t="s">
+      <c r="L1" s="51" t="s">
         <v>168</v>
       </c>
     </row>
@@ -5579,27 +5659,27 @@
         <f t="shared" ref="I26" si="9">SUM(I2:I25)</f>
         <v>0.99999999999999967</v>
       </c>
-      <c r="J26" s="53">
+      <c r="J26" s="52">
         <f t="shared" ref="J26" si="10">SUM(J2:J25)</f>
         <v>0.40073400270852677</v>
       </c>
-      <c r="K26" s="53">
+      <c r="K26" s="52">
         <f t="shared" ref="K26" si="11">SUM(K2:K25)</f>
         <v>0.4171276762746271</v>
       </c>
-      <c r="L26" s="53">
+      <c r="L26" s="52">
         <f t="shared" ref="L26" si="12">SUM(L2:L25)</f>
         <v>0.36706596430163779</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="52" t="s">
+      <c r="A30" s="51" t="s">
         <v>172</v>
       </c>
-      <c r="B30" s="52" t="s">
+      <c r="B30" s="51" t="s">
         <v>173</v>
       </c>
-      <c r="C30" s="52" t="s">
+      <c r="C30" s="51" t="s">
         <v>174</v>
       </c>
       <c r="H30" t="s">
@@ -5619,7 +5699,7 @@
       <c r="B31">
         <v>575</v>
       </c>
-      <c r="C31" s="59">
+      <c r="C31" s="58">
         <f>A31/$A$35</f>
         <v>0.4</v>
       </c>
@@ -5635,7 +5715,7 @@
       <c r="B32">
         <v>585</v>
       </c>
-      <c r="C32" s="59">
+      <c r="C32" s="58">
         <f t="shared" ref="C32:C34" si="13">A32/$A$35</f>
         <v>0.35</v>
       </c>
@@ -5660,7 +5740,7 @@
       <c r="B33">
         <v>595</v>
       </c>
-      <c r="C33" s="59">
+      <c r="C33" s="58">
         <f t="shared" si="13"/>
         <v>0.2</v>
       </c>
@@ -5676,7 +5756,7 @@
       <c r="B34">
         <v>600</v>
       </c>
-      <c r="C34" s="59">
+      <c r="C34" s="58">
         <f t="shared" si="13"/>
         <v>0.05</v>
       </c>
@@ -5726,104 +5806,104 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="62" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="65" t="s">
         <v>205</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="63" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="66" t="s">
+      <c r="A4" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="63" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="66" t="s">
+      <c r="A5" s="65" t="s">
         <v>205</v>
       </c>
-      <c r="B5" s="64" t="s">
+      <c r="B5" s="63" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="66" t="s">
+      <c r="A6" s="65" t="s">
         <v>206</v>
       </c>
-      <c r="B6" s="64" t="s">
+      <c r="B6" s="63" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="66" t="s">
+      <c r="A7" s="65" t="s">
         <v>207</v>
       </c>
-      <c r="B7" s="64" t="s">
+      <c r="B7" s="63" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="66" t="s">
+      <c r="A8" s="65" t="s">
         <v>206</v>
       </c>
-      <c r="B8" s="64" t="s">
+      <c r="B8" s="63" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="66" t="s">
+      <c r="A9" s="65" t="s">
         <v>207</v>
       </c>
-      <c r="B9" s="64" t="s">
+      <c r="B9" s="63" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="66" t="s">
+      <c r="A10" s="65" t="s">
         <v>208</v>
       </c>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="63" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="66" t="s">
+      <c r="A11" s="65" t="s">
         <v>209</v>
       </c>
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="63" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="66" t="s">
+      <c r="A12" s="65" t="s">
         <v>208</v>
       </c>
-      <c r="B12" s="64" t="s">
+      <c r="B12" s="63" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="66" t="s">
+      <c r="A13" s="65" t="s">
         <v>209</v>
       </c>
-      <c r="B13" s="64" t="s">
+      <c r="B13" s="63" t="s">
         <v>220</v>
       </c>
       <c r="H13">
         <v>2010</v>
       </c>
-      <c r="I13" s="67">
+      <c r="I13" s="66">
         <v>845027.64130188676</v>
       </c>
       <c r="K13">
@@ -5834,16 +5914,16 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="66" t="s">
+      <c r="A14" s="65" t="s">
         <v>210</v>
       </c>
-      <c r="B14" s="64" t="s">
+      <c r="B14" s="63" t="s">
         <v>216</v>
       </c>
       <c r="H14">
         <v>2011</v>
       </c>
-      <c r="I14" s="67">
+      <c r="I14" s="66">
         <v>1057657.9879999999</v>
       </c>
       <c r="K14">
@@ -5854,16 +5934,16 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="66" t="s">
+      <c r="A15" s="65" t="s">
         <v>211</v>
       </c>
-      <c r="B15" s="64" t="s">
+      <c r="B15" s="63" t="s">
         <v>217</v>
       </c>
       <c r="H15">
         <v>2012</v>
       </c>
-      <c r="I15" s="67">
+      <c r="I15" s="66">
         <v>1095752.9345</v>
       </c>
       <c r="K15">
@@ -5874,16 +5954,16 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="66" t="s">
+      <c r="A16" s="65" t="s">
         <v>212</v>
       </c>
-      <c r="B16" s="64" t="s">
+      <c r="B16" s="63" t="s">
         <v>218</v>
       </c>
       <c r="H16">
         <v>2013</v>
       </c>
-      <c r="I16" s="67">
+      <c r="I16" s="66">
         <v>1151586.4650000001</v>
       </c>
       <c r="K16">
@@ -5894,74 +5974,74 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="66" t="s">
+      <c r="A17" s="65" t="s">
         <v>210</v>
       </c>
-      <c r="B17" s="64" t="s">
+      <c r="B17" s="63" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="66" t="s">
+      <c r="A18" s="65" t="s">
         <v>211</v>
       </c>
-      <c r="B18" s="64" t="s">
+      <c r="B18" s="63" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="66" t="s">
+      <c r="A19" s="65" t="s">
         <v>212</v>
       </c>
-      <c r="B19" s="64" t="s">
+      <c r="B19" s="63" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="66" t="s">
+      <c r="A20" s="65" t="s">
         <v>213</v>
       </c>
-      <c r="B20" s="64" t="s">
+      <c r="B20" s="63" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="66" t="s">
+      <c r="A21" s="65" t="s">
         <v>214</v>
       </c>
-      <c r="B21" s="64" t="s">
+      <c r="B21" s="63" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="66" t="s">
+      <c r="A22" s="65" t="s">
         <v>213</v>
       </c>
-      <c r="B22" s="64" t="s">
+      <c r="B22" s="63" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="66" t="s">
+      <c r="A23" s="65" t="s">
         <v>214</v>
       </c>
-      <c r="B23" s="64" t="s">
+      <c r="B23" s="63" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="66" t="s">
+      <c r="A24" s="65" t="s">
         <v>215</v>
       </c>
-      <c r="B24" s="64" t="s">
+      <c r="B24" s="63" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="66" t="s">
+      <c r="A25" s="65" t="s">
         <v>215</v>
       </c>
-      <c r="B25" s="64" t="s">
+      <c r="B25" s="63" t="s">
         <v>226</v>
       </c>
       <c r="H25" t="s">
@@ -5981,10 +6061,10 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="66" t="s">
+      <c r="A26" s="65" t="s">
         <v>216</v>
       </c>
-      <c r="B26" s="64" t="s">
+      <c r="B26" s="63" t="s">
         <v>227</v>
       </c>
       <c r="I26" t="e">
@@ -6001,10 +6081,10 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="66" t="s">
+      <c r="A27" s="65" t="s">
         <v>217</v>
       </c>
-      <c r="B27" s="64" t="s">
+      <c r="B27" s="63" t="s">
         <v>204</v>
       </c>
       <c r="H27" t="s">
@@ -6024,10 +6104,10 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="66" t="s">
+      <c r="A28" s="65" t="s">
         <v>218</v>
       </c>
-      <c r="B28" s="64" t="s">
+      <c r="B28" s="63" t="s">
         <v>205</v>
       </c>
       <c r="I28" t="e">
@@ -6044,10 +6124,10 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="66" t="s">
+      <c r="A29" s="65" t="s">
         <v>216</v>
       </c>
-      <c r="B29" s="64" t="s">
+      <c r="B29" s="63" t="s">
         <v>223</v>
       </c>
       <c r="H29" t="s">
@@ -6067,10 +6147,10 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="66" t="s">
+      <c r="A30" s="65" t="s">
         <v>217</v>
       </c>
-      <c r="B30" s="64" t="s">
+      <c r="B30" s="63" t="s">
         <v>224</v>
       </c>
       <c r="I30" t="e">
@@ -6087,10 +6167,10 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="66" t="s">
+      <c r="A31" s="65" t="s">
         <v>218</v>
       </c>
-      <c r="B31" s="64" t="s">
+      <c r="B31" s="63" t="s">
         <v>221</v>
       </c>
       <c r="H31" t="s">
@@ -6110,10 +6190,10 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="66" t="s">
+      <c r="A32" s="65" t="s">
         <v>219</v>
       </c>
-      <c r="B32" s="64" t="s">
+      <c r="B32" s="63" t="s">
         <v>222</v>
       </c>
       <c r="I32" t="e">
@@ -6130,10 +6210,10 @@
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="66" t="s">
+      <c r="A33" s="65" t="s">
         <v>220</v>
       </c>
-      <c r="B33" s="64" t="s">
+      <c r="B33" s="63" t="s">
         <v>206</v>
       </c>
       <c r="H33" t="s">
@@ -6153,10 +6233,10 @@
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="66" t="s">
+      <c r="A34" s="65" t="s">
         <v>219</v>
       </c>
-      <c r="B34" s="64" t="s">
+      <c r="B34" s="63" t="s">
         <v>207</v>
       </c>
       <c r="I34" t="e">
@@ -6173,10 +6253,10 @@
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="66" t="s">
+      <c r="A35" s="65" t="s">
         <v>220</v>
       </c>
-      <c r="B35" s="64" t="s">
+      <c r="B35" s="63" t="s">
         <v>215</v>
       </c>
       <c r="H35" t="s">
@@ -6196,10 +6276,10 @@
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="66" t="s">
+      <c r="A36" s="65" t="s">
         <v>221</v>
       </c>
-      <c r="B36" s="64" t="s">
+      <c r="B36" s="63" t="s">
         <v>180</v>
       </c>
       <c r="I36" t="e">
@@ -6216,10 +6296,10 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="66" t="s">
+      <c r="A37" s="65" t="s">
         <v>222</v>
       </c>
-      <c r="B37" s="64" t="s">
+      <c r="B37" s="63" t="s">
         <v>179</v>
       </c>
       <c r="H37" t="s">
@@ -6239,7 +6319,7 @@
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="66" t="s">
+      <c r="A38" s="65" t="s">
         <v>221</v>
       </c>
       <c r="I38" t="e">
@@ -6256,7 +6336,7 @@
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="66" t="s">
+      <c r="A39" s="65" t="s">
         <v>222</v>
       </c>
       <c r="H39" t="s">
@@ -6276,7 +6356,7 @@
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="66" t="s">
+      <c r="A40" s="65" t="s">
         <v>223</v>
       </c>
       <c r="I40" t="e">
@@ -6293,7 +6373,7 @@
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="66" t="s">
+      <c r="A41" s="65" t="s">
         <v>224</v>
       </c>
       <c r="H41" t="s">
@@ -6313,7 +6393,7 @@
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="66" t="s">
+      <c r="A42" s="65" t="s">
         <v>223</v>
       </c>
       <c r="I42" t="e">
@@ -6330,7 +6410,7 @@
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="66" t="s">
+      <c r="A43" s="65" t="s">
         <v>224</v>
       </c>
       <c r="I43" t="e">
@@ -6347,7 +6427,7 @@
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="66" t="s">
+      <c r="A44" s="65" t="s">
         <v>225</v>
       </c>
       <c r="I44" t="e">
@@ -6364,7 +6444,7 @@
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="66" t="s">
+      <c r="A45" s="65" t="s">
         <v>226</v>
       </c>
       <c r="H45" t="s">
@@ -6384,7 +6464,7 @@
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="66" t="s">
+      <c r="A46" s="65" t="s">
         <v>227</v>
       </c>
       <c r="I46" t="e">
@@ -6401,7 +6481,7 @@
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="66" t="s">
+      <c r="A47" s="65" t="s">
         <v>225</v>
       </c>
       <c r="H47" t="s">
@@ -6421,7 +6501,7 @@
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="66" t="s">
+      <c r="A48" s="65" t="s">
         <v>226</v>
       </c>
       <c r="I48" t="e">
@@ -6438,7 +6518,7 @@
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="66" t="s">
+      <c r="A49" s="65" t="s">
         <v>227</v>
       </c>
       <c r="H49" t="s">
@@ -6458,7 +6538,7 @@
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="66" t="s">
+      <c r="A50" s="65" t="s">
         <v>228</v>
       </c>
       <c r="I50" t="e">
@@ -6475,7 +6555,7 @@
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="66" t="s">
+      <c r="A51" s="65" t="s">
         <v>229</v>
       </c>
       <c r="H51" t="s">
@@ -6495,7 +6575,7 @@
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="66" t="s">
+      <c r="A52" s="65" t="s">
         <v>228</v>
       </c>
       <c r="I52" t="e">
@@ -6512,7 +6592,7 @@
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="66" t="s">
+      <c r="A53" s="65" t="s">
         <v>229</v>
       </c>
       <c r="H53" t="s">
@@ -6532,7 +6612,7 @@
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="66" t="s">
+      <c r="A54" s="65" t="s">
         <v>230</v>
       </c>
       <c r="I54" t="e">
@@ -6549,7 +6629,7 @@
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="66" t="s">
+      <c r="A55" s="65" t="s">
         <v>231</v>
       </c>
       <c r="H55" t="s">
@@ -6569,7 +6649,7 @@
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="66" t="s">
+      <c r="A56" s="65" t="s">
         <v>230</v>
       </c>
       <c r="I56" t="e">
@@ -6586,7 +6666,7 @@
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="66" t="s">
+      <c r="A57" s="65" t="s">
         <v>231</v>
       </c>
       <c r="H57" t="s">
@@ -6606,7 +6686,7 @@
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="66" t="s">
+      <c r="A58" s="65" t="s">
         <v>232</v>
       </c>
       <c r="I58" t="e">
@@ -6623,7 +6703,7 @@
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="66" t="s">
+      <c r="A59" s="65" t="s">
         <v>233</v>
       </c>
       <c r="I59" t="e">
@@ -6640,7 +6720,7 @@
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="66" t="s">
+      <c r="A60" s="65" t="s">
         <v>234</v>
       </c>
       <c r="I60" t="e">
@@ -6657,7 +6737,7 @@
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="66" t="s">
+      <c r="A61" s="65" t="s">
         <v>235</v>
       </c>
       <c r="H61" t="s">
@@ -6677,7 +6757,7 @@
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="66" t="s">
+      <c r="A62" s="65" t="s">
         <v>236</v>
       </c>
       <c r="I62" t="e">
@@ -6694,7 +6774,7 @@
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="66" t="s">
+      <c r="A63" s="65" t="s">
         <v>232</v>
       </c>
       <c r="H63" t="s">
@@ -6714,7 +6794,7 @@
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="66" t="s">
+      <c r="A64" s="65" t="s">
         <v>233</v>
       </c>
       <c r="I64" t="e">
@@ -6731,7 +6811,7 @@
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="66" t="s">
+      <c r="A65" s="65" t="s">
         <v>234</v>
       </c>
       <c r="H65" t="s">
@@ -6751,7 +6831,7 @@
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="66" t="s">
+      <c r="A66" s="65" t="s">
         <v>235</v>
       </c>
       <c r="I66" t="e">
@@ -6768,7 +6848,7 @@
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="66" t="s">
+      <c r="A67" s="65" t="s">
         <v>236</v>
       </c>
       <c r="H67" t="s">
@@ -6788,7 +6868,7 @@
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="65"/>
+      <c r="A68" s="64"/>
       <c r="I68" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
@@ -6803,7 +6883,7 @@
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A69" s="65"/>
+      <c r="A69" s="64"/>
       <c r="H69" t="s">
         <v>201</v>
       </c>
@@ -6821,7 +6901,7 @@
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A70" s="65"/>
+      <c r="A70" s="64"/>
       <c r="I70" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
@@ -6836,7 +6916,7 @@
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="65"/>
+      <c r="A71" s="64"/>
       <c r="H71" t="s">
         <v>202</v>
       </c>
@@ -6854,7 +6934,7 @@
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72" s="65"/>
+      <c r="A72" s="64"/>
       <c r="I72" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
@@ -6869,7 +6949,7 @@
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A73" s="65"/>
+      <c r="A73" s="64"/>
       <c r="I73" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
@@ -6884,7 +6964,7 @@
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A74" s="65"/>
+      <c r="A74" s="64"/>
       <c r="I74" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
@@ -6899,7 +6979,7 @@
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A75" s="65"/>
+      <c r="A75" s="64"/>
       <c r="H75" t="s">
         <v>203</v>
       </c>
@@ -6917,1192 +6997,1192 @@
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A76" s="65"/>
+      <c r="A76" s="64"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A77" s="65"/>
+      <c r="A77" s="64"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A78" s="65"/>
+      <c r="A78" s="64"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A79" s="65"/>
+      <c r="A79" s="64"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A80" s="65"/>
+      <c r="A80" s="64"/>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="65"/>
+      <c r="A81" s="64"/>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="65"/>
+      <c r="A82" s="64"/>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="65"/>
+      <c r="A83" s="64"/>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="65"/>
+      <c r="A84" s="64"/>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="65"/>
+      <c r="A85" s="64"/>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="65"/>
+      <c r="A86" s="64"/>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="65"/>
+      <c r="A87" s="64"/>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="65"/>
+      <c r="A88" s="64"/>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="65"/>
+      <c r="A89" s="64"/>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="65"/>
+      <c r="A90" s="64"/>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="65"/>
+      <c r="A91" s="64"/>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="65"/>
+      <c r="A92" s="64"/>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="65"/>
+      <c r="A93" s="64"/>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="65"/>
+      <c r="A94" s="64"/>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="65"/>
+      <c r="A95" s="64"/>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="65"/>
+      <c r="A96" s="64"/>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="65"/>
+      <c r="A97" s="64"/>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="65"/>
+      <c r="A98" s="64"/>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="65"/>
+      <c r="A99" s="64"/>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="65"/>
+      <c r="A100" s="64"/>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="65"/>
+      <c r="A101" s="64"/>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="65"/>
+      <c r="A102" s="64"/>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="65"/>
+      <c r="A103" s="64"/>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="65"/>
+      <c r="A104" s="64"/>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" s="65"/>
+      <c r="A105" s="64"/>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="65"/>
+      <c r="A106" s="64"/>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" s="65"/>
+      <c r="A107" s="64"/>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="65"/>
+      <c r="A108" s="64"/>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="65"/>
+      <c r="A109" s="64"/>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="65"/>
+      <c r="A110" s="64"/>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" s="65"/>
+      <c r="A111" s="64"/>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" s="65"/>
+      <c r="A112" s="64"/>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="65"/>
+      <c r="A113" s="64"/>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="65"/>
+      <c r="A114" s="64"/>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="65"/>
+      <c r="A115" s="64"/>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="65"/>
+      <c r="A116" s="64"/>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" s="65"/>
+      <c r="A117" s="64"/>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" s="65"/>
+      <c r="A118" s="64"/>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" s="65"/>
+      <c r="A119" s="64"/>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="65"/>
+      <c r="A120" s="64"/>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" s="65"/>
+      <c r="A121" s="64"/>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" s="65"/>
+      <c r="A122" s="64"/>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" s="65"/>
+      <c r="A123" s="64"/>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" s="65"/>
+      <c r="A124" s="64"/>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" s="65"/>
+      <c r="A125" s="64"/>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" s="65"/>
+      <c r="A126" s="64"/>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" s="65"/>
+      <c r="A127" s="64"/>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" s="65"/>
+      <c r="A128" s="64"/>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="65"/>
+      <c r="A129" s="64"/>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="65"/>
+      <c r="A130" s="64"/>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="65"/>
+      <c r="A131" s="64"/>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="65"/>
+      <c r="A132" s="64"/>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="65"/>
+      <c r="A133" s="64"/>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" s="65"/>
+      <c r="A134" s="64"/>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="65"/>
+      <c r="A135" s="64"/>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" s="65"/>
+      <c r="A136" s="64"/>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="65"/>
+      <c r="A137" s="64"/>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" s="65"/>
+      <c r="A138" s="64"/>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="65"/>
+      <c r="A139" s="64"/>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="65"/>
+      <c r="A140" s="64"/>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" s="65"/>
+      <c r="A141" s="64"/>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" s="65"/>
+      <c r="A142" s="64"/>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="65"/>
+      <c r="A143" s="64"/>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" s="65"/>
+      <c r="A144" s="64"/>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" s="65"/>
+      <c r="A145" s="64"/>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="65"/>
+      <c r="A146" s="64"/>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="65"/>
+      <c r="A147" s="64"/>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" s="65"/>
+      <c r="A148" s="64"/>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" s="65"/>
+      <c r="A149" s="64"/>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="65"/>
+      <c r="A150" s="64"/>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" s="65"/>
+      <c r="A151" s="64"/>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" s="65"/>
+      <c r="A152" s="64"/>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="65"/>
+      <c r="A153" s="64"/>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" s="65"/>
+      <c r="A154" s="64"/>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" s="65"/>
+      <c r="A155" s="64"/>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" s="65"/>
+      <c r="A156" s="64"/>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" s="65"/>
+      <c r="A157" s="64"/>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" s="65"/>
+      <c r="A158" s="64"/>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" s="65"/>
+      <c r="A159" s="64"/>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" s="65"/>
+      <c r="A160" s="64"/>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" s="65"/>
+      <c r="A161" s="64"/>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" s="65"/>
+      <c r="A162" s="64"/>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163" s="65"/>
+      <c r="A163" s="64"/>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" s="65"/>
+      <c r="A164" s="64"/>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" s="65"/>
+      <c r="A165" s="64"/>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166" s="65"/>
+      <c r="A166" s="64"/>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" s="65"/>
+      <c r="A167" s="64"/>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168" s="65"/>
+      <c r="A168" s="64"/>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169" s="65"/>
+      <c r="A169" s="64"/>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A170" s="65"/>
+      <c r="A170" s="64"/>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" s="65"/>
+      <c r="A171" s="64"/>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172" s="65"/>
+      <c r="A172" s="64"/>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A173" s="65"/>
+      <c r="A173" s="64"/>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174" s="65"/>
+      <c r="A174" s="64"/>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" s="65"/>
+      <c r="A175" s="64"/>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176" s="65"/>
+      <c r="A176" s="64"/>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" s="65"/>
+      <c r="A177" s="64"/>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178" s="65"/>
+      <c r="A178" s="64"/>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A179" s="65"/>
+      <c r="A179" s="64"/>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" s="65"/>
+      <c r="A180" s="64"/>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181" s="65"/>
+      <c r="A181" s="64"/>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A182" s="65"/>
+      <c r="A182" s="64"/>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" s="65"/>
+      <c r="A183" s="64"/>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A184" s="65"/>
+      <c r="A184" s="64"/>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185" s="65"/>
+      <c r="A185" s="64"/>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186" s="65"/>
+      <c r="A186" s="64"/>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A187" s="65"/>
+      <c r="A187" s="64"/>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A188" s="65"/>
+      <c r="A188" s="64"/>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189" s="65"/>
+      <c r="A189" s="64"/>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A190" s="65"/>
+      <c r="A190" s="64"/>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A191" s="65"/>
+      <c r="A191" s="64"/>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A192" s="65"/>
+      <c r="A192" s="64"/>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A193" s="65"/>
+      <c r="A193" s="64"/>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A194" s="65"/>
+      <c r="A194" s="64"/>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A195" s="65"/>
+      <c r="A195" s="64"/>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A196" s="65"/>
+      <c r="A196" s="64"/>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A197" s="65"/>
+      <c r="A197" s="64"/>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A198" s="65"/>
+      <c r="A198" s="64"/>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A199" s="65"/>
+      <c r="A199" s="64"/>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A200" s="65"/>
+      <c r="A200" s="64"/>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A201" s="65"/>
+      <c r="A201" s="64"/>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A202" s="65"/>
+      <c r="A202" s="64"/>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A203" s="65"/>
+      <c r="A203" s="64"/>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A204" s="65"/>
+      <c r="A204" s="64"/>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A205" s="65"/>
+      <c r="A205" s="64"/>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A206" s="65"/>
+      <c r="A206" s="64"/>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A207" s="65"/>
+      <c r="A207" s="64"/>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A208" s="65"/>
+      <c r="A208" s="64"/>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A209" s="65"/>
+      <c r="A209" s="64"/>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A210" s="65"/>
+      <c r="A210" s="64"/>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A211" s="65"/>
+      <c r="A211" s="64"/>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A212" s="65"/>
+      <c r="A212" s="64"/>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A213" s="65"/>
+      <c r="A213" s="64"/>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A214" s="65"/>
+      <c r="A214" s="64"/>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A215" s="65"/>
+      <c r="A215" s="64"/>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A216" s="65"/>
+      <c r="A216" s="64"/>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A217" s="65"/>
+      <c r="A217" s="64"/>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A218" s="65"/>
+      <c r="A218" s="64"/>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A219" s="65"/>
+      <c r="A219" s="64"/>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A220" s="65"/>
+      <c r="A220" s="64"/>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A221" s="65"/>
+      <c r="A221" s="64"/>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A222" s="65"/>
+      <c r="A222" s="64"/>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A223" s="65"/>
+      <c r="A223" s="64"/>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A224" s="65"/>
+      <c r="A224" s="64"/>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A225" s="65"/>
+      <c r="A225" s="64"/>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A226" s="65"/>
+      <c r="A226" s="64"/>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A227" s="65"/>
+      <c r="A227" s="64"/>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A228" s="65"/>
+      <c r="A228" s="64"/>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A229" s="65"/>
+      <c r="A229" s="64"/>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A230" s="65"/>
+      <c r="A230" s="64"/>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A231" s="65"/>
+      <c r="A231" s="64"/>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A232" s="65"/>
+      <c r="A232" s="64"/>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A233" s="65"/>
+      <c r="A233" s="64"/>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A234" s="65"/>
+      <c r="A234" s="64"/>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A235" s="65"/>
+      <c r="A235" s="64"/>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A236" s="65"/>
+      <c r="A236" s="64"/>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A237" s="65"/>
+      <c r="A237" s="64"/>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A238" s="65"/>
+      <c r="A238" s="64"/>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A239" s="65"/>
+      <c r="A239" s="64"/>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A240" s="65"/>
+      <c r="A240" s="64"/>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A241" s="65"/>
+      <c r="A241" s="64"/>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A242" s="65"/>
+      <c r="A242" s="64"/>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A243" s="65"/>
+      <c r="A243" s="64"/>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A244" s="65"/>
+      <c r="A244" s="64"/>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A245" s="65"/>
+      <c r="A245" s="64"/>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A246" s="65"/>
+      <c r="A246" s="64"/>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A247" s="65"/>
+      <c r="A247" s="64"/>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A248" s="65"/>
+      <c r="A248" s="64"/>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A249" s="65"/>
+      <c r="A249" s="64"/>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A250" s="65"/>
+      <c r="A250" s="64"/>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A251" s="65"/>
+      <c r="A251" s="64"/>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A252" s="65"/>
+      <c r="A252" s="64"/>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A253" s="65"/>
+      <c r="A253" s="64"/>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A254" s="65"/>
+      <c r="A254" s="64"/>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A255" s="65"/>
+      <c r="A255" s="64"/>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A256" s="65"/>
+      <c r="A256" s="64"/>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A257" s="65"/>
+      <c r="A257" s="64"/>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A258" s="65"/>
+      <c r="A258" s="64"/>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A259" s="65"/>
+      <c r="A259" s="64"/>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A260" s="65"/>
+      <c r="A260" s="64"/>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A261" s="65"/>
+      <c r="A261" s="64"/>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A262" s="65"/>
+      <c r="A262" s="64"/>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A263" s="65"/>
+      <c r="A263" s="64"/>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A264" s="65"/>
+      <c r="A264" s="64"/>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A265" s="65"/>
+      <c r="A265" s="64"/>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A266" s="65"/>
+      <c r="A266" s="64"/>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A267" s="65"/>
+      <c r="A267" s="64"/>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A268" s="65"/>
+      <c r="A268" s="64"/>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A269" s="65"/>
+      <c r="A269" s="64"/>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A270" s="65"/>
+      <c r="A270" s="64"/>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A271" s="65"/>
+      <c r="A271" s="64"/>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A272" s="65"/>
+      <c r="A272" s="64"/>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A273" s="65"/>
+      <c r="A273" s="64"/>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A274" s="65"/>
+      <c r="A274" s="64"/>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A275" s="65"/>
+      <c r="A275" s="64"/>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A276" s="65"/>
+      <c r="A276" s="64"/>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A277" s="65"/>
+      <c r="A277" s="64"/>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A278" s="65"/>
+      <c r="A278" s="64"/>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A279" s="65"/>
+      <c r="A279" s="64"/>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A280" s="65"/>
+      <c r="A280" s="64"/>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A281" s="65"/>
+      <c r="A281" s="64"/>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A282" s="65"/>
+      <c r="A282" s="64"/>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A283" s="65"/>
+      <c r="A283" s="64"/>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A284" s="65"/>
+      <c r="A284" s="64"/>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A285" s="65"/>
+      <c r="A285" s="64"/>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A286" s="65"/>
+      <c r="A286" s="64"/>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A287" s="65"/>
+      <c r="A287" s="64"/>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A288" s="65"/>
+      <c r="A288" s="64"/>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A289" s="65"/>
+      <c r="A289" s="64"/>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A290" s="65"/>
+      <c r="A290" s="64"/>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A291" s="65"/>
+      <c r="A291" s="64"/>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A292" s="65"/>
+      <c r="A292" s="64"/>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A293" s="65"/>
+      <c r="A293" s="64"/>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A294" s="65"/>
+      <c r="A294" s="64"/>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A295" s="65"/>
+      <c r="A295" s="64"/>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A296" s="65"/>
+      <c r="A296" s="64"/>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A297" s="65"/>
+      <c r="A297" s="64"/>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A298" s="65"/>
+      <c r="A298" s="64"/>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A299" s="65"/>
+      <c r="A299" s="64"/>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A300" s="65"/>
+      <c r="A300" s="64"/>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A301" s="65"/>
+      <c r="A301" s="64"/>
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A302" s="65"/>
+      <c r="A302" s="64"/>
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A303" s="65"/>
+      <c r="A303" s="64"/>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A304" s="65"/>
+      <c r="A304" s="64"/>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A305" s="65"/>
+      <c r="A305" s="64"/>
     </row>
     <row r="306" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A306" s="65"/>
+      <c r="A306" s="64"/>
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A307" s="65"/>
+      <c r="A307" s="64"/>
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A308" s="65"/>
+      <c r="A308" s="64"/>
     </row>
     <row r="309" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A309" s="65"/>
+      <c r="A309" s="64"/>
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A310" s="65"/>
+      <c r="A310" s="64"/>
     </row>
     <row r="311" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A311" s="65"/>
+      <c r="A311" s="64"/>
     </row>
     <row r="312" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A312" s="65"/>
+      <c r="A312" s="64"/>
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A313" s="65"/>
+      <c r="A313" s="64"/>
     </row>
     <row r="314" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A314" s="65"/>
+      <c r="A314" s="64"/>
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A315" s="65"/>
+      <c r="A315" s="64"/>
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A316" s="65"/>
+      <c r="A316" s="64"/>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A317" s="65"/>
+      <c r="A317" s="64"/>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A318" s="65"/>
+      <c r="A318" s="64"/>
     </row>
     <row r="319" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A319" s="65"/>
+      <c r="A319" s="64"/>
     </row>
     <row r="320" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A320" s="65"/>
+      <c r="A320" s="64"/>
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A321" s="65"/>
+      <c r="A321" s="64"/>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A322" s="65"/>
+      <c r="A322" s="64"/>
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A323" s="65"/>
+      <c r="A323" s="64"/>
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A324" s="65"/>
+      <c r="A324" s="64"/>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A325" s="65"/>
+      <c r="A325" s="64"/>
     </row>
     <row r="326" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A326" s="65"/>
+      <c r="A326" s="64"/>
     </row>
     <row r="327" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A327" s="65"/>
+      <c r="A327" s="64"/>
     </row>
     <row r="328" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A328" s="65"/>
+      <c r="A328" s="64"/>
     </row>
     <row r="329" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A329" s="65"/>
+      <c r="A329" s="64"/>
     </row>
     <row r="330" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A330" s="65"/>
+      <c r="A330" s="64"/>
     </row>
     <row r="331" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A331" s="65"/>
+      <c r="A331" s="64"/>
     </row>
     <row r="332" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A332" s="65"/>
+      <c r="A332" s="64"/>
     </row>
     <row r="333" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A333" s="65"/>
+      <c r="A333" s="64"/>
     </row>
     <row r="334" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A334" s="65"/>
+      <c r="A334" s="64"/>
     </row>
     <row r="335" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A335" s="65"/>
+      <c r="A335" s="64"/>
     </row>
     <row r="336" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A336" s="65"/>
+      <c r="A336" s="64"/>
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A337" s="65"/>
+      <c r="A337" s="64"/>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A338" s="65"/>
+      <c r="A338" s="64"/>
     </row>
     <row r="339" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A339" s="65"/>
+      <c r="A339" s="64"/>
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A340" s="65"/>
+      <c r="A340" s="64"/>
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A341" s="65"/>
+      <c r="A341" s="64"/>
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A342" s="65"/>
+      <c r="A342" s="64"/>
     </row>
     <row r="343" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A343" s="65"/>
+      <c r="A343" s="64"/>
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A344" s="65"/>
+      <c r="A344" s="64"/>
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A345" s="65"/>
+      <c r="A345" s="64"/>
     </row>
     <row r="346" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A346" s="65"/>
+      <c r="A346" s="64"/>
     </row>
     <row r="347" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A347" s="65"/>
+      <c r="A347" s="64"/>
     </row>
     <row r="348" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A348" s="65"/>
+      <c r="A348" s="64"/>
     </row>
     <row r="349" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A349" s="65"/>
+      <c r="A349" s="64"/>
     </row>
     <row r="350" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A350" s="65"/>
+      <c r="A350" s="64"/>
     </row>
     <row r="351" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A351" s="65"/>
+      <c r="A351" s="64"/>
     </row>
     <row r="352" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A352" s="65"/>
+      <c r="A352" s="64"/>
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A353" s="65"/>
+      <c r="A353" s="64"/>
     </row>
     <row r="354" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A354" s="65"/>
+      <c r="A354" s="64"/>
     </row>
     <row r="355" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A355" s="65"/>
+      <c r="A355" s="64"/>
     </row>
     <row r="356" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A356" s="65"/>
+      <c r="A356" s="64"/>
     </row>
     <row r="357" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A357" s="65"/>
+      <c r="A357" s="64"/>
     </row>
     <row r="358" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A358" s="65"/>
+      <c r="A358" s="64"/>
     </row>
     <row r="359" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A359" s="65"/>
+      <c r="A359" s="64"/>
     </row>
     <row r="360" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A360" s="65"/>
+      <c r="A360" s="64"/>
     </row>
     <row r="361" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A361" s="65"/>
+      <c r="A361" s="64"/>
     </row>
     <row r="362" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A362" s="65"/>
+      <c r="A362" s="64"/>
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A363" s="65"/>
+      <c r="A363" s="64"/>
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A364" s="65"/>
+      <c r="A364" s="64"/>
     </row>
     <row r="365" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A365" s="65"/>
+      <c r="A365" s="64"/>
     </row>
     <row r="366" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A366" s="65"/>
+      <c r="A366" s="64"/>
     </row>
     <row r="367" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A367" s="65"/>
+      <c r="A367" s="64"/>
     </row>
     <row r="368" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A368" s="65"/>
+      <c r="A368" s="64"/>
     </row>
     <row r="369" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A369" s="65"/>
+      <c r="A369" s="64"/>
     </row>
     <row r="370" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A370" s="65"/>
+      <c r="A370" s="64"/>
     </row>
     <row r="371" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A371" s="65"/>
+      <c r="A371" s="64"/>
     </row>
     <row r="372" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A372" s="65"/>
+      <c r="A372" s="64"/>
     </row>
     <row r="373" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A373" s="65"/>
+      <c r="A373" s="64"/>
     </row>
     <row r="374" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A374" s="65"/>
+      <c r="A374" s="64"/>
     </row>
     <row r="375" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A375" s="65"/>
+      <c r="A375" s="64"/>
     </row>
     <row r="376" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A376" s="65"/>
+      <c r="A376" s="64"/>
     </row>
     <row r="377" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A377" s="65"/>
+      <c r="A377" s="64"/>
     </row>
     <row r="378" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A378" s="65"/>
+      <c r="A378" s="64"/>
     </row>
     <row r="379" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A379" s="65"/>
+      <c r="A379" s="64"/>
     </row>
     <row r="380" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A380" s="65"/>
+      <c r="A380" s="64"/>
     </row>
     <row r="381" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A381" s="65"/>
+      <c r="A381" s="64"/>
     </row>
     <row r="382" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A382" s="65"/>
+      <c r="A382" s="64"/>
     </row>
     <row r="383" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A383" s="65"/>
+      <c r="A383" s="64"/>
     </row>
     <row r="384" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A384" s="65"/>
+      <c r="A384" s="64"/>
     </row>
     <row r="385" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A385" s="65"/>
+      <c r="A385" s="64"/>
     </row>
     <row r="386" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A386" s="65"/>
+      <c r="A386" s="64"/>
     </row>
     <row r="387" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A387" s="65"/>
+      <c r="A387" s="64"/>
     </row>
     <row r="388" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A388" s="65"/>
+      <c r="A388" s="64"/>
     </row>
     <row r="389" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A389" s="65"/>
+      <c r="A389" s="64"/>
     </row>
     <row r="390" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A390" s="65"/>
+      <c r="A390" s="64"/>
     </row>
     <row r="391" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A391" s="65"/>
+      <c r="A391" s="64"/>
     </row>
     <row r="392" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A392" s="65"/>
+      <c r="A392" s="64"/>
     </row>
     <row r="393" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A393" s="65"/>
+      <c r="A393" s="64"/>
     </row>
     <row r="394" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A394" s="65"/>
+      <c r="A394" s="64"/>
     </row>
     <row r="395" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A395" s="65"/>
+      <c r="A395" s="64"/>
     </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A396" s="65"/>
+      <c r="A396" s="64"/>
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A397" s="65"/>
+      <c r="A397" s="64"/>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A398" s="65"/>
+      <c r="A398" s="64"/>
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A399" s="65"/>
+      <c r="A399" s="64"/>
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A400" s="65"/>
+      <c r="A400" s="64"/>
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A401" s="65"/>
+      <c r="A401" s="64"/>
     </row>
     <row r="402" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A402" s="65"/>
+      <c r="A402" s="64"/>
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A403" s="65"/>
+      <c r="A403" s="64"/>
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A404" s="65"/>
+      <c r="A404" s="64"/>
     </row>
     <row r="405" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A405" s="65"/>
+      <c r="A405" s="64"/>
     </row>
     <row r="406" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A406" s="65"/>
+      <c r="A406" s="64"/>
     </row>
     <row r="407" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A407" s="65"/>
+      <c r="A407" s="64"/>
     </row>
     <row r="408" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A408" s="65"/>
+      <c r="A408" s="64"/>
     </row>
     <row r="409" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A409" s="65"/>
+      <c r="A409" s="64"/>
     </row>
     <row r="410" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A410" s="65"/>
+      <c r="A410" s="64"/>
     </row>
     <row r="411" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A411" s="65"/>
+      <c r="A411" s="64"/>
     </row>
     <row r="412" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A412" s="65"/>
+      <c r="A412" s="64"/>
     </row>
     <row r="413" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A413" s="65"/>
+      <c r="A413" s="64"/>
     </row>
     <row r="414" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A414" s="65"/>
+      <c r="A414" s="64"/>
     </row>
     <row r="415" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A415" s="65"/>
+      <c r="A415" s="64"/>
     </row>
     <row r="416" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A416" s="65"/>
+      <c r="A416" s="64"/>
     </row>
     <row r="417" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A417" s="65"/>
+      <c r="A417" s="64"/>
     </row>
     <row r="418" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A418" s="65"/>
+      <c r="A418" s="64"/>
     </row>
     <row r="419" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A419" s="65"/>
+      <c r="A419" s="64"/>
     </row>
     <row r="420" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A420" s="65"/>
+      <c r="A420" s="64"/>
     </row>
     <row r="421" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A421" s="65"/>
+      <c r="A421" s="64"/>
     </row>
     <row r="422" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A422" s="65"/>
+      <c r="A422" s="64"/>
     </row>
     <row r="423" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A423" s="65"/>
+      <c r="A423" s="64"/>
     </row>
     <row r="424" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A424" s="65"/>
+      <c r="A424" s="64"/>
     </row>
     <row r="425" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A425" s="65"/>
+      <c r="A425" s="64"/>
     </row>
     <row r="426" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A426" s="65"/>
+      <c r="A426" s="64"/>
     </row>
     <row r="427" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A427" s="65"/>
+      <c r="A427" s="64"/>
     </row>
     <row r="428" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A428" s="65"/>
+      <c r="A428" s="64"/>
     </row>
     <row r="429" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A429" s="65"/>
+      <c r="A429" s="64"/>
     </row>
     <row r="430" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A430" s="65"/>
+      <c r="A430" s="64"/>
     </row>
     <row r="431" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A431" s="65"/>
+      <c r="A431" s="64"/>
     </row>
     <row r="432" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A432" s="65"/>
+      <c r="A432" s="64"/>
     </row>
     <row r="433" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A433" s="65"/>
+      <c r="A433" s="64"/>
     </row>
     <row r="434" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A434" s="65"/>
+      <c r="A434" s="64"/>
     </row>
     <row r="435" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A435" s="65"/>
+      <c r="A435" s="64"/>
     </row>
     <row r="436" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A436" s="65"/>
+      <c r="A436" s="64"/>
     </row>
     <row r="437" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A437" s="65"/>
+      <c r="A437" s="64"/>
     </row>
     <row r="438" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A438" s="65"/>
+      <c r="A438" s="64"/>
     </row>
     <row r="439" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A439" s="65"/>
+      <c r="A439" s="64"/>
     </row>
     <row r="440" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A440" s="65"/>
+      <c r="A440" s="64"/>
     </row>
     <row r="441" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A441" s="65"/>
+      <c r="A441" s="64"/>
     </row>
     <row r="442" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A442" s="65"/>
+      <c r="A442" s="64"/>
     </row>
     <row r="443" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A443" s="65"/>
+      <c r="A443" s="64"/>
     </row>
     <row r="444" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A444" s="65"/>
+      <c r="A444" s="64"/>
     </row>
     <row r="445" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A445" s="65"/>
+      <c r="A445" s="64"/>
     </row>
     <row r="446" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A446" s="65"/>
+      <c r="A446" s="64"/>
     </row>
     <row r="447" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A447" s="65"/>
+      <c r="A447" s="64"/>
     </row>
     <row r="448" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A448" s="65"/>
+      <c r="A448" s="64"/>
     </row>
     <row r="449" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A449" s="65"/>
+      <c r="A449" s="64"/>
     </row>
     <row r="450" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A450" s="65"/>
+      <c r="A450" s="64"/>
     </row>
     <row r="451" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A451" s="65"/>
+      <c r="A451" s="64"/>
     </row>
     <row r="452" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A452" s="65"/>
+      <c r="A452" s="64"/>
     </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A453" s="65"/>
+      <c r="A453" s="64"/>
     </row>
     <row r="454" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A454" s="65"/>
+      <c r="A454" s="64"/>
     </row>
     <row r="455" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A455" s="65"/>
+      <c r="A455" s="64"/>
     </row>
     <row r="456" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A456" s="65"/>
+      <c r="A456" s="64"/>
     </row>
     <row r="457" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A457" s="65"/>
+      <c r="A457" s="64"/>
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A458" s="65"/>
+      <c r="A458" s="64"/>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A459" s="65"/>
+      <c r="A459" s="64"/>
     </row>
     <row r="460" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A460" s="65"/>
+      <c r="A460" s="64"/>
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A461" s="65"/>
+      <c r="A461" s="64"/>
     </row>
     <row r="462" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A462" s="65"/>
+      <c r="A462" s="64"/>
     </row>
     <row r="463" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A463" s="65"/>
+      <c r="A463" s="64"/>
     </row>
     <row r="464" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A464" s="65"/>
+      <c r="A464" s="64"/>
     </row>
     <row r="465" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A465" s="65"/>
+      <c r="A465" s="64"/>
     </row>
     <row r="466" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A466" s="65"/>
+      <c r="A466" s="64"/>
     </row>
     <row r="467" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A467" s="65"/>
+      <c r="A467" s="64"/>
     </row>
     <row r="468" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A468" s="65"/>
+      <c r="A468" s="64"/>
     </row>
     <row r="469" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A469" s="65"/>
+      <c r="A469" s="64"/>
     </row>
     <row r="470" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A470" s="65"/>
+      <c r="A470" s="64"/>
     </row>
     <row r="471" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A471" s="65"/>
+      <c r="A471" s="64"/>
     </row>
   </sheetData>
   <dataConsolidate/>

</xml_diff>

<commit_message>
finaliza jornada QH 02-01-2015
</commit_message>
<xml_diff>
--- a/Documentacion/indicadores revisión junio 11 2014.xlsx
+++ b/Documentacion/indicadores revisión junio 11 2014.xlsx
@@ -1555,7 +1555,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1609,9 +1609,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1737,6 +1734,15 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1760,15 +1766,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3490,10 +3487,10 @@
   <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomRight" activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3518,10 +3515,10 @@
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="68" t="s">
+      <c r="C2" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="68"/>
+      <c r="D2" s="70"/>
       <c r="E2" s="8" t="s">
         <v>2</v>
       </c>
@@ -3537,39 +3534,39 @@
       <c r="I2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="47" t="s">
+      <c r="J2" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="K2" s="47" t="s">
+      <c r="K2" s="46" t="s">
         <v>154</v>
       </c>
-      <c r="L2" s="47" t="s">
+      <c r="L2" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="M2" s="47" t="s">
+      <c r="M2" s="46" t="s">
         <v>157</v>
       </c>
-      <c r="N2" s="47" t="s">
+      <c r="N2" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="O2" s="47" t="s">
+      <c r="O2" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="P2" s="47" t="s">
+      <c r="P2" s="46" t="s">
         <v>148</v>
       </c>
-      <c r="Q2" s="47" t="s">
+      <c r="Q2" s="46" t="s">
         <v>149</v>
       </c>
-      <c r="R2" s="47" t="s">
+      <c r="R2" s="46" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="76">
+      <c r="A3" s="67">
         <v>1</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="47" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="11" t="s">
@@ -3581,49 +3578,49 @@
       <c r="E3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="69" t="s">
+      <c r="F3" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="71" t="s">
+      <c r="G3" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="71" t="s">
+      <c r="H3" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="73" t="s">
+      <c r="I3" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="J3" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="K3" s="21" t="s">
+      <c r="K3" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="L3" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="N3" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="O3" s="21" t="s">
+      <c r="O3" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="P3" s="21" t="s">
+      <c r="P3" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="Q3" s="21" t="s">
+      <c r="Q3" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="R3" s="21"/>
+      <c r="R3" s="20"/>
     </row>
     <row r="4" spans="1:18" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="76">
+      <c r="A4" s="67">
         <v>2</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="48" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="14" t="s">
@@ -3635,41 +3632,41 @@
       <c r="E4" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="70"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="72"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="21" t="s">
+      <c r="F4" s="72"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="K4" s="21" t="s">
+      <c r="K4" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="L4" s="21" t="s">
+      <c r="L4" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="M4" s="21" t="s">
+      <c r="M4" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="N4" s="21" t="s">
+      <c r="N4" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="O4" s="21" t="s">
+      <c r="O4" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="P4" s="21" t="s">
+      <c r="P4" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="Q4" s="21" t="s">
+      <c r="Q4" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="R4" s="21"/>
+      <c r="R4" s="20"/>
     </row>
     <row r="5" spans="1:18" ht="104.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="76">
+      <c r="A5" s="67">
         <v>3</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="49" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="14" t="s">
@@ -3684,46 +3681,46 @@
       <c r="F5" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="21" t="s">
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="K5" s="21" t="s">
+      <c r="K5" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="L5" s="21" t="s">
+      <c r="L5" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="M5" s="21" t="s">
+      <c r="M5" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="N5" s="21" t="s">
+      <c r="N5" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="O5" s="21" t="s">
+      <c r="O5" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="P5" s="21" t="s">
+      <c r="P5" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="Q5" s="21" t="s">
+      <c r="Q5" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="R5" s="21"/>
+      <c r="R5" s="20"/>
     </row>
     <row r="6" spans="1:18" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="76">
+      <c r="A6" s="67">
         <v>18</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="21" t="s">
         <v>26</v>
       </c>
       <c r="E6" s="16" t="s">
@@ -3735,51 +3732,51 @@
       <c r="G6" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="22" t="s">
+      <c r="I6" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="J6" s="21" t="s">
+      <c r="J6" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="K6" s="21" t="s">
+      <c r="K6" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="L6" s="21" t="s">
+      <c r="L6" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="M6" s="21" t="s">
+      <c r="M6" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="N6" s="21" t="s">
+      <c r="N6" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="O6" s="21" t="s">
+      <c r="O6" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="P6" s="21" t="s">
+      <c r="P6" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="Q6" s="21" t="s">
+      <c r="Q6" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="R6" s="21" t="s">
+      <c r="R6" s="20" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="76">
+      <c r="A7" s="67">
         <v>19</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="48" t="s">
         <v>32</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="21" t="s">
         <v>237</v>
       </c>
       <c r="E7" s="16" t="s">
@@ -3788,54 +3785,54 @@
       <c r="F7" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="H7" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="I7" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="J7" s="21" t="s">
+      <c r="J7" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="K7" s="21" t="s">
+      <c r="K7" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="L7" s="21" t="s">
+      <c r="L7" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="M7" s="21" t="s">
+      <c r="M7" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="N7" s="21" t="s">
+      <c r="N7" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="O7" s="21" t="s">
+      <c r="O7" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="P7" s="21" t="s">
+      <c r="P7" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="Q7" s="21" t="s">
+      <c r="Q7" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="R7" s="21" t="s">
+      <c r="R7" s="20" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="114" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="76">
+      <c r="A8" s="67">
         <v>8</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="23" t="s">
         <v>40</v>
       </c>
       <c r="E8" s="16" t="s">
@@ -3844,104 +3841,104 @@
       <c r="F8" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="H8" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="I8" s="22" t="s">
+      <c r="I8" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="J8" s="21" t="s">
+      <c r="J8" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="K8" s="21" t="s">
+      <c r="K8" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="L8" s="21" t="s">
+      <c r="L8" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="M8" s="21" t="s">
+      <c r="M8" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="N8" s="21" t="s">
+      <c r="N8" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="O8" s="21" t="s">
+      <c r="O8" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="P8" s="21" t="s">
+      <c r="P8" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="Q8" s="21" t="s">
+      <c r="Q8" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="R8" s="21"/>
-    </row>
-    <row r="9" spans="1:18" s="26" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="77"/>
-      <c r="B9" s="20" t="s">
+      <c r="R8" s="20"/>
+    </row>
+    <row r="9" spans="1:18" s="25" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="68"/>
+      <c r="B9" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="55" t="s">
+      <c r="C9" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="56" t="s">
+      <c r="D9" s="55" t="s">
         <v>156</v>
       </c>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="32" t="s">
+      <c r="F9" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="33" t="s">
+      <c r="G9" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="33" t="s">
+      <c r="H9" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="I9" s="33" t="s">
+      <c r="I9" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="J9" s="55" t="s">
+      <c r="J9" s="54" t="s">
         <v>150</v>
       </c>
-      <c r="K9" s="55" t="s">
+      <c r="K9" s="54" t="s">
         <v>155</v>
       </c>
-      <c r="L9" s="55" t="s">
+      <c r="L9" s="54" t="s">
         <v>150</v>
       </c>
-      <c r="M9" s="55" t="s">
+      <c r="M9" s="54" t="s">
         <v>155</v>
       </c>
-      <c r="N9" s="55" t="s">
+      <c r="N9" s="54" t="s">
         <v>150</v>
       </c>
-      <c r="O9" s="55" t="s">
+      <c r="O9" s="54" t="s">
         <v>150</v>
       </c>
-      <c r="P9" s="55" t="s">
+      <c r="P9" s="54" t="s">
         <v>150</v>
       </c>
-      <c r="Q9" s="55" t="s">
+      <c r="Q9" s="54" t="s">
         <v>150</v>
       </c>
-      <c r="R9" s="55"/>
+      <c r="R9" s="54"/>
     </row>
     <row r="10" spans="1:18" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="76">
+      <c r="A10" s="67">
         <v>4</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="48" t="s">
         <v>51</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="23" t="s">
         <v>53</v>
       </c>
       <c r="E10" s="16" t="s">
@@ -3950,122 +3947,122 @@
       <c r="F10" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="22" t="s">
+      <c r="G10" s="21" t="s">
         <v>56</v>
       </c>
       <c r="H10" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="I10" s="24" t="s">
+      <c r="I10" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="J10" s="21" t="s">
+      <c r="J10" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="K10" s="21" t="s">
+      <c r="K10" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="L10" s="21" t="s">
+      <c r="L10" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="M10" s="21" t="s">
+      <c r="M10" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="N10" s="21" t="s">
+      <c r="N10" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="O10" s="21" t="s">
+      <c r="O10" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="P10" s="21" t="s">
+      <c r="P10" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="Q10" s="21" t="s">
+      <c r="Q10" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="R10" s="21"/>
-    </row>
-    <row r="11" spans="1:18" s="26" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="77">
+      <c r="R10" s="20"/>
+    </row>
+    <row r="11" spans="1:18" s="25" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="68">
         <v>5</v>
       </c>
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="74" t="s">
+      <c r="D11" s="76" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="67" t="s">
+      <c r="E11" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="F11" s="74" t="s">
+      <c r="F11" s="76" t="s">
         <v>62</v>
       </c>
-      <c r="G11" s="74" t="s">
+      <c r="G11" s="76" t="s">
         <v>63</v>
       </c>
-      <c r="H11" s="67" t="s">
+      <c r="H11" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="I11" s="67" t="s">
+      <c r="I11" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="J11" s="26" t="s">
+      <c r="J11" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="K11" s="26">
+      <c r="K11" s="25">
         <v>15</v>
       </c>
-      <c r="L11" s="26">
+      <c r="L11" s="25">
         <v>20</v>
       </c>
-      <c r="M11" s="26">
+      <c r="M11" s="25">
         <f>L11*L12</f>
         <v>500000000</v>
       </c>
     </row>
-    <row r="12" spans="1:18" s="26" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="77">
+    <row r="12" spans="1:18" s="25" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="68">
         <v>6</v>
       </c>
-      <c r="B12" s="50" t="s">
+      <c r="B12" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="74"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="74"/>
-      <c r="H12" s="67"/>
-      <c r="I12" s="67"/>
-      <c r="J12" s="26" t="s">
+      <c r="D12" s="76"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="69"/>
+      <c r="J12" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="K12" s="26">
+      <c r="K12" s="25">
         <v>1500000</v>
       </c>
-      <c r="L12" s="26">
+      <c r="L12" s="25">
         <v>25000000</v>
       </c>
-      <c r="M12" s="26">
+      <c r="M12" s="25">
         <f>K12*K11</f>
         <v>22500000</v>
       </c>
-      <c r="N12" s="26">
+      <c r="N12" s="25">
         <f>M12-M11</f>
         <v>-477500000</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="76">
+      <c r="A13" s="67">
         <v>7</v>
       </c>
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="48" t="s">
         <v>66</v>
       </c>
       <c r="C13" s="14" t="s">
@@ -4074,27 +4071,27 @@
       <c r="D13" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="26" t="s">
         <v>69</v>
       </c>
       <c r="F13" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="G13" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="22" t="s">
+      <c r="H13" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="I13" s="22" t="s">
+      <c r="I13" s="21" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="144" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="76">
+      <c r="A14" s="67">
         <v>9</v>
       </c>
-      <c r="B14" s="49" t="s">
+      <c r="B14" s="48" t="s">
         <v>72</v>
       </c>
       <c r="C14" s="14" t="s">
@@ -4109,24 +4106,24 @@
       <c r="F14" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="G14" s="22" t="s">
+      <c r="G14" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="H14" s="22" t="s">
+      <c r="H14" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="I14" s="22" t="s">
+      <c r="I14" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="J14" s="53" t="s">
+      <c r="J14" s="52" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="144" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="76">
+      <c r="A15" s="67">
         <v>10</v>
       </c>
-      <c r="B15" s="50" t="s">
+      <c r="B15" s="49" t="s">
         <v>79</v>
       </c>
       <c r="C15" s="14" t="s">
@@ -4141,13 +4138,13 @@
       <c r="F15" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="G15" s="22" t="s">
+      <c r="G15" s="21" t="s">
         <v>56</v>
       </c>
       <c r="H15" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="I15" s="24" t="s">
+      <c r="I15" s="23" t="s">
         <v>31</v>
       </c>
       <c r="J15" s="6" t="s">
@@ -4155,13 +4152,13 @@
       </c>
     </row>
     <row r="16" spans="1:18" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="76">
+      <c r="A16" s="67">
         <v>11</v>
       </c>
-      <c r="B16" s="50" t="s">
+      <c r="B16" s="49" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="27" t="s">
         <v>85</v>
       </c>
       <c r="D16" s="14" t="s">
@@ -4173,27 +4170,27 @@
       <c r="F16" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="G16" s="24" t="s">
+      <c r="G16" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="I16" s="22" t="s">
+      <c r="I16" s="21" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="153" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="77">
+      <c r="A17" s="68">
         <v>12</v>
       </c>
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="48" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="28" t="s">
         <v>92</v>
       </c>
       <c r="E17" s="16" t="s">
@@ -4202,296 +4199,296 @@
       <c r="F17" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="G17" s="22" t="s">
+      <c r="G17" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="H17" s="22" t="s">
+      <c r="H17" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="I17" s="22" t="s">
+      <c r="I17" s="21" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="26" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="77">
+    <row r="18" spans="1:9" s="25" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="68">
         <v>13</v>
       </c>
-      <c r="B18" s="50" t="s">
+      <c r="B18" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="C18" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="D18" s="30" t="s">
+      <c r="D18" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="E18" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="F18" s="32" t="s">
+      <c r="F18" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="G18" s="33" t="s">
+      <c r="G18" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="H18" s="33" t="s">
+      <c r="H18" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="I18" s="33" t="s">
+      <c r="I18" s="32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="26" customFormat="1" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="77">
+    <row r="19" spans="1:9" s="25" customFormat="1" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="68">
         <v>16</v>
       </c>
-      <c r="B19" s="61" t="s">
+      <c r="B19" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="D19" s="34" t="s">
+      <c r="D19" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="E19" s="34" t="s">
+      <c r="E19" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="F19" s="31" t="s">
+      <c r="F19" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="G19" s="33" t="s">
+      <c r="G19" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="H19" s="33" t="s">
+      <c r="H19" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="I19" s="24" t="s">
+      <c r="I19" s="23" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="26" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="77">
+    <row r="20" spans="1:9" s="25" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="68">
         <v>17</v>
       </c>
-      <c r="B20" s="61" t="s">
+      <c r="B20" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="C20" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="D20" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="E20" s="34" t="s">
+      <c r="E20" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="F20" s="34" t="s">
+      <c r="F20" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="G20" s="33" t="s">
+      <c r="G20" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="H20" s="33" t="s">
+      <c r="H20" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="I20" s="24" t="s">
+      <c r="I20" s="23" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="76">
+      <c r="A21" s="67">
         <v>15</v>
       </c>
-      <c r="B21" s="61" t="s">
+      <c r="B21" s="60" t="s">
         <v>113</v>
       </c>
-      <c r="C21" s="35" t="s">
+      <c r="C21" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="D21" s="36" t="s">
+      <c r="D21" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="E21" s="37" t="s">
+      <c r="E21" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="F21" s="38" t="s">
+      <c r="F21" s="37" t="s">
         <v>117</v>
       </c>
-      <c r="G21" s="22" t="s">
+      <c r="G21" s="21" t="s">
         <v>56</v>
       </c>
       <c r="H21" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="I21" s="24" t="s">
+      <c r="I21" s="23" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="26" customFormat="1" ht="137.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="77">
+    <row r="22" spans="1:9" s="25" customFormat="1" ht="137.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="68">
         <v>14</v>
       </c>
-      <c r="B22" s="59" t="s">
+      <c r="B22" s="58" t="s">
         <v>118</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C22" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="D22" s="39" t="s">
+      <c r="D22" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="E22" s="37" t="s">
+      <c r="E22" s="36" t="s">
         <v>121</v>
       </c>
-      <c r="F22" s="34" t="s">
+      <c r="F22" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="G22" s="33" t="s">
+      <c r="G22" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="H22" s="29" t="s">
+      <c r="H22" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="I22" s="39" t="s">
+      <c r="I22" s="38" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="26" customFormat="1" ht="137.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="77">
+    <row r="23" spans="1:9" s="25" customFormat="1" ht="137.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="68">
         <v>20</v>
       </c>
-      <c r="B23" s="60" t="s">
+      <c r="B23" s="59" t="s">
         <v>171</v>
       </c>
-      <c r="C23" s="57" t="s">
+      <c r="C23" s="56" t="s">
         <v>123</v>
       </c>
-      <c r="D23" s="39" t="s">
+      <c r="D23" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="E23" s="39" t="s">
+      <c r="E23" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="F23" s="32" t="s">
+      <c r="F23" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="G23" s="33" t="s">
+      <c r="G23" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="H23" s="57" t="s">
+      <c r="H23" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="I23" s="39" t="s">
+      <c r="I23" s="38" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="26" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="77">
+    <row r="24" spans="1:9" s="25" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="68">
         <v>21</v>
       </c>
-      <c r="B24" s="75" t="s">
+      <c r="B24" s="66" t="s">
         <v>127</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="C24" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="D24" s="33" t="s">
+      <c r="D24" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="E24" s="32" t="s">
+      <c r="E24" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="F24" s="32" t="s">
+      <c r="F24" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="G24" s="33" t="s">
+      <c r="G24" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="H24" s="33" t="s">
+      <c r="H24" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="I24" s="33" t="s">
+      <c r="I24" s="32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="26" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="77">
+    <row r="25" spans="1:9" s="25" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="68">
         <v>21</v>
       </c>
-      <c r="B25" s="49" t="s">
+      <c r="B25" s="48" t="s">
         <v>133</v>
       </c>
-      <c r="C25" s="29" t="s">
+      <c r="C25" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="D25" s="24" t="s">
+      <c r="D25" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="E25" s="33" t="s">
+      <c r="E25" s="32" t="s">
         <v>136</v>
       </c>
-      <c r="F25" s="32" t="s">
+      <c r="F25" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="G25" s="33" t="s">
+      <c r="G25" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="H25" s="33" t="s">
+      <c r="H25" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="I25" s="22" t="s">
+      <c r="I25" s="21" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="102.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="76"/>
-      <c r="B26" s="54" t="s">
+      <c r="A26" s="67"/>
+      <c r="B26" s="53" t="s">
         <v>139</v>
       </c>
-      <c r="C26" s="40" t="s">
+      <c r="C26" s="39" t="s">
         <v>140</v>
       </c>
-      <c r="D26" s="24" t="s">
+      <c r="D26" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="E26" s="39" t="s">
+      <c r="E26" s="38" t="s">
         <v>142</v>
       </c>
-      <c r="F26" s="41" t="s">
+      <c r="F26" s="40" t="s">
         <v>143</v>
       </c>
-      <c r="G26" s="42" t="s">
+      <c r="G26" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="H26" s="42" t="s">
+      <c r="H26" s="41" t="s">
         <v>144</v>
       </c>
-      <c r="I26" s="42" t="s">
+      <c r="I26" s="41" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F34" s="43"/>
+      <c r="F34" s="42"/>
     </row>
     <row r="35" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D35" s="44"/>
-      <c r="F35" s="43"/>
+      <c r="D35" s="43"/>
+      <c r="F35" s="42"/>
     </row>
     <row r="36" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F36" s="43"/>
+      <c r="F36" s="42"/>
     </row>
     <row r="37" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F37" s="43"/>
+      <c r="F37" s="42"/>
     </row>
     <row r="38" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F38" s="45"/>
+      <c r="F38" s="44"/>
     </row>
     <row r="40" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F40" s="46"/>
+      <c r="F40" s="45"/>
     </row>
     <row r="41" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F41" s="45"/>
+      <c r="F41" s="44"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:R26">
@@ -4533,40 +4530,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="50" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="50" t="s">
         <v>161</v>
       </c>
-      <c r="C1" s="51">
+      <c r="C1" s="50">
         <v>2012</v>
       </c>
-      <c r="D1" s="51">
+      <c r="D1" s="50">
         <v>2013</v>
       </c>
-      <c r="E1" s="51">
+      <c r="E1" s="50">
         <v>2014</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="50" t="s">
         <v>162</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="G1" s="50" t="s">
         <v>163</v>
       </c>
-      <c r="H1" s="51" t="s">
+      <c r="H1" s="50" t="s">
         <v>164</v>
       </c>
-      <c r="I1" s="51" t="s">
+      <c r="I1" s="50" t="s">
         <v>165</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="J1" s="50" t="s">
         <v>166</v>
       </c>
-      <c r="K1" s="51" t="s">
+      <c r="K1" s="50" t="s">
         <v>167</v>
       </c>
-      <c r="L1" s="51" t="s">
+      <c r="L1" s="50" t="s">
         <v>168</v>
       </c>
     </row>
@@ -5659,27 +5656,27 @@
         <f t="shared" ref="I26" si="9">SUM(I2:I25)</f>
         <v>0.99999999999999967</v>
       </c>
-      <c r="J26" s="52">
+      <c r="J26" s="51">
         <f t="shared" ref="J26" si="10">SUM(J2:J25)</f>
         <v>0.40073400270852677</v>
       </c>
-      <c r="K26" s="52">
+      <c r="K26" s="51">
         <f t="shared" ref="K26" si="11">SUM(K2:K25)</f>
         <v>0.4171276762746271</v>
       </c>
-      <c r="L26" s="52">
+      <c r="L26" s="51">
         <f t="shared" ref="L26" si="12">SUM(L2:L25)</f>
         <v>0.36706596430163779</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="51" t="s">
+      <c r="A30" s="50" t="s">
         <v>172</v>
       </c>
-      <c r="B30" s="51" t="s">
+      <c r="B30" s="50" t="s">
         <v>173</v>
       </c>
-      <c r="C30" s="51" t="s">
+      <c r="C30" s="50" t="s">
         <v>174</v>
       </c>
       <c r="H30" t="s">
@@ -5699,7 +5696,7 @@
       <c r="B31">
         <v>575</v>
       </c>
-      <c r="C31" s="58">
+      <c r="C31" s="57">
         <f>A31/$A$35</f>
         <v>0.4</v>
       </c>
@@ -5715,7 +5712,7 @@
       <c r="B32">
         <v>585</v>
       </c>
-      <c r="C32" s="58">
+      <c r="C32" s="57">
         <f t="shared" ref="C32:C34" si="13">A32/$A$35</f>
         <v>0.35</v>
       </c>
@@ -5740,7 +5737,7 @@
       <c r="B33">
         <v>595</v>
       </c>
-      <c r="C33" s="58">
+      <c r="C33" s="57">
         <f t="shared" si="13"/>
         <v>0.2</v>
       </c>
@@ -5756,7 +5753,7 @@
       <c r="B34">
         <v>600</v>
       </c>
-      <c r="C34" s="58">
+      <c r="C34" s="57">
         <f t="shared" si="13"/>
         <v>0.05</v>
       </c>
@@ -5806,104 +5803,104 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="64" t="s">
         <v>204</v>
       </c>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="61" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="64" t="s">
         <v>205</v>
       </c>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="62" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="64" t="s">
         <v>204</v>
       </c>
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="62" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="65" t="s">
+      <c r="A5" s="64" t="s">
         <v>205</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="62" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="65" t="s">
+      <c r="A6" s="64" t="s">
         <v>206</v>
       </c>
-      <c r="B6" s="63" t="s">
+      <c r="B6" s="62" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="65" t="s">
+      <c r="A7" s="64" t="s">
         <v>207</v>
       </c>
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="62" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="65" t="s">
+      <c r="A8" s="64" t="s">
         <v>206</v>
       </c>
-      <c r="B8" s="63" t="s">
+      <c r="B8" s="62" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="65" t="s">
+      <c r="A9" s="64" t="s">
         <v>207</v>
       </c>
-      <c r="B9" s="63" t="s">
+      <c r="B9" s="62" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="65" t="s">
+      <c r="A10" s="64" t="s">
         <v>208</v>
       </c>
-      <c r="B10" s="63" t="s">
+      <c r="B10" s="62" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="65" t="s">
+      <c r="A11" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="B11" s="63" t="s">
+      <c r="B11" s="62" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="65" t="s">
+      <c r="A12" s="64" t="s">
         <v>208</v>
       </c>
-      <c r="B12" s="63" t="s">
+      <c r="B12" s="62" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="65" t="s">
+      <c r="A13" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="B13" s="63" t="s">
+      <c r="B13" s="62" t="s">
         <v>220</v>
       </c>
       <c r="H13">
         <v>2010</v>
       </c>
-      <c r="I13" s="66">
+      <c r="I13" s="65">
         <v>845027.64130188676</v>
       </c>
       <c r="K13">
@@ -5914,16 +5911,16 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="65" t="s">
+      <c r="A14" s="64" t="s">
         <v>210</v>
       </c>
-      <c r="B14" s="63" t="s">
+      <c r="B14" s="62" t="s">
         <v>216</v>
       </c>
       <c r="H14">
         <v>2011</v>
       </c>
-      <c r="I14" s="66">
+      <c r="I14" s="65">
         <v>1057657.9879999999</v>
       </c>
       <c r="K14">
@@ -5934,16 +5931,16 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="65" t="s">
+      <c r="A15" s="64" t="s">
         <v>211</v>
       </c>
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="62" t="s">
         <v>217</v>
       </c>
       <c r="H15">
         <v>2012</v>
       </c>
-      <c r="I15" s="66">
+      <c r="I15" s="65">
         <v>1095752.9345</v>
       </c>
       <c r="K15">
@@ -5954,16 +5951,16 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="65" t="s">
+      <c r="A16" s="64" t="s">
         <v>212</v>
       </c>
-      <c r="B16" s="63" t="s">
+      <c r="B16" s="62" t="s">
         <v>218</v>
       </c>
       <c r="H16">
         <v>2013</v>
       </c>
-      <c r="I16" s="66">
+      <c r="I16" s="65">
         <v>1151586.4650000001</v>
       </c>
       <c r="K16">
@@ -5974,74 +5971,74 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="65" t="s">
+      <c r="A17" s="64" t="s">
         <v>210</v>
       </c>
-      <c r="B17" s="63" t="s">
+      <c r="B17" s="62" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="65" t="s">
+      <c r="A18" s="64" t="s">
         <v>211</v>
       </c>
-      <c r="B18" s="63" t="s">
+      <c r="B18" s="62" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="65" t="s">
+      <c r="A19" s="64" t="s">
         <v>212</v>
       </c>
-      <c r="B19" s="63" t="s">
+      <c r="B19" s="62" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="65" t="s">
+      <c r="A20" s="64" t="s">
         <v>213</v>
       </c>
-      <c r="B20" s="63" t="s">
+      <c r="B20" s="62" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="65" t="s">
+      <c r="A21" s="64" t="s">
         <v>214</v>
       </c>
-      <c r="B21" s="63" t="s">
+      <c r="B21" s="62" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="65" t="s">
+      <c r="A22" s="64" t="s">
         <v>213</v>
       </c>
-      <c r="B22" s="63" t="s">
+      <c r="B22" s="62" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="65" t="s">
+      <c r="A23" s="64" t="s">
         <v>214</v>
       </c>
-      <c r="B23" s="63" t="s">
+      <c r="B23" s="62" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="65" t="s">
+      <c r="A24" s="64" t="s">
         <v>215</v>
       </c>
-      <c r="B24" s="63" t="s">
+      <c r="B24" s="62" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="65" t="s">
+      <c r="A25" s="64" t="s">
         <v>215</v>
       </c>
-      <c r="B25" s="63" t="s">
+      <c r="B25" s="62" t="s">
         <v>226</v>
       </c>
       <c r="H25" t="s">
@@ -6061,10 +6058,10 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="65" t="s">
+      <c r="A26" s="64" t="s">
         <v>216</v>
       </c>
-      <c r="B26" s="63" t="s">
+      <c r="B26" s="62" t="s">
         <v>227</v>
       </c>
       <c r="I26" t="e">
@@ -6081,10 +6078,10 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="65" t="s">
+      <c r="A27" s="64" t="s">
         <v>217</v>
       </c>
-      <c r="B27" s="63" t="s">
+      <c r="B27" s="62" t="s">
         <v>204</v>
       </c>
       <c r="H27" t="s">
@@ -6104,10 +6101,10 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="65" t="s">
+      <c r="A28" s="64" t="s">
         <v>218</v>
       </c>
-      <c r="B28" s="63" t="s">
+      <c r="B28" s="62" t="s">
         <v>205</v>
       </c>
       <c r="I28" t="e">
@@ -6124,10 +6121,10 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="65" t="s">
+      <c r="A29" s="64" t="s">
         <v>216</v>
       </c>
-      <c r="B29" s="63" t="s">
+      <c r="B29" s="62" t="s">
         <v>223</v>
       </c>
       <c r="H29" t="s">
@@ -6147,10 +6144,10 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="65" t="s">
+      <c r="A30" s="64" t="s">
         <v>217</v>
       </c>
-      <c r="B30" s="63" t="s">
+      <c r="B30" s="62" t="s">
         <v>224</v>
       </c>
       <c r="I30" t="e">
@@ -6167,10 +6164,10 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="65" t="s">
+      <c r="A31" s="64" t="s">
         <v>218</v>
       </c>
-      <c r="B31" s="63" t="s">
+      <c r="B31" s="62" t="s">
         <v>221</v>
       </c>
       <c r="H31" t="s">
@@ -6190,10 +6187,10 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="65" t="s">
+      <c r="A32" s="64" t="s">
         <v>219</v>
       </c>
-      <c r="B32" s="63" t="s">
+      <c r="B32" s="62" t="s">
         <v>222</v>
       </c>
       <c r="I32" t="e">
@@ -6210,10 +6207,10 @@
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="65" t="s">
+      <c r="A33" s="64" t="s">
         <v>220</v>
       </c>
-      <c r="B33" s="63" t="s">
+      <c r="B33" s="62" t="s">
         <v>206</v>
       </c>
       <c r="H33" t="s">
@@ -6233,10 +6230,10 @@
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="65" t="s">
+      <c r="A34" s="64" t="s">
         <v>219</v>
       </c>
-      <c r="B34" s="63" t="s">
+      <c r="B34" s="62" t="s">
         <v>207</v>
       </c>
       <c r="I34" t="e">
@@ -6253,10 +6250,10 @@
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="65" t="s">
+      <c r="A35" s="64" t="s">
         <v>220</v>
       </c>
-      <c r="B35" s="63" t="s">
+      <c r="B35" s="62" t="s">
         <v>215</v>
       </c>
       <c r="H35" t="s">
@@ -6276,10 +6273,10 @@
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="65" t="s">
+      <c r="A36" s="64" t="s">
         <v>221</v>
       </c>
-      <c r="B36" s="63" t="s">
+      <c r="B36" s="62" t="s">
         <v>180</v>
       </c>
       <c r="I36" t="e">
@@ -6296,10 +6293,10 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="65" t="s">
+      <c r="A37" s="64" t="s">
         <v>222</v>
       </c>
-      <c r="B37" s="63" t="s">
+      <c r="B37" s="62" t="s">
         <v>179</v>
       </c>
       <c r="H37" t="s">
@@ -6319,7 +6316,7 @@
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="65" t="s">
+      <c r="A38" s="64" t="s">
         <v>221</v>
       </c>
       <c r="I38" t="e">
@@ -6336,7 +6333,7 @@
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="65" t="s">
+      <c r="A39" s="64" t="s">
         <v>222</v>
       </c>
       <c r="H39" t="s">
@@ -6356,7 +6353,7 @@
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="65" t="s">
+      <c r="A40" s="64" t="s">
         <v>223</v>
       </c>
       <c r="I40" t="e">
@@ -6373,7 +6370,7 @@
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="65" t="s">
+      <c r="A41" s="64" t="s">
         <v>224</v>
       </c>
       <c r="H41" t="s">
@@ -6393,7 +6390,7 @@
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="65" t="s">
+      <c r="A42" s="64" t="s">
         <v>223</v>
       </c>
       <c r="I42" t="e">
@@ -6410,7 +6407,7 @@
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="65" t="s">
+      <c r="A43" s="64" t="s">
         <v>224</v>
       </c>
       <c r="I43" t="e">
@@ -6427,7 +6424,7 @@
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="65" t="s">
+      <c r="A44" s="64" t="s">
         <v>225</v>
       </c>
       <c r="I44" t="e">
@@ -6444,7 +6441,7 @@
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="65" t="s">
+      <c r="A45" s="64" t="s">
         <v>226</v>
       </c>
       <c r="H45" t="s">
@@ -6464,7 +6461,7 @@
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="65" t="s">
+      <c r="A46" s="64" t="s">
         <v>227</v>
       </c>
       <c r="I46" t="e">
@@ -6481,7 +6478,7 @@
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="65" t="s">
+      <c r="A47" s="64" t="s">
         <v>225</v>
       </c>
       <c r="H47" t="s">
@@ -6501,7 +6498,7 @@
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="65" t="s">
+      <c r="A48" s="64" t="s">
         <v>226</v>
       </c>
       <c r="I48" t="e">
@@ -6518,7 +6515,7 @@
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="65" t="s">
+      <c r="A49" s="64" t="s">
         <v>227</v>
       </c>
       <c r="H49" t="s">
@@ -6538,7 +6535,7 @@
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="65" t="s">
+      <c r="A50" s="64" t="s">
         <v>228</v>
       </c>
       <c r="I50" t="e">
@@ -6555,7 +6552,7 @@
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="65" t="s">
+      <c r="A51" s="64" t="s">
         <v>229</v>
       </c>
       <c r="H51" t="s">
@@ -6575,7 +6572,7 @@
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="65" t="s">
+      <c r="A52" s="64" t="s">
         <v>228</v>
       </c>
       <c r="I52" t="e">
@@ -6592,7 +6589,7 @@
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="65" t="s">
+      <c r="A53" s="64" t="s">
         <v>229</v>
       </c>
       <c r="H53" t="s">
@@ -6612,7 +6609,7 @@
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="65" t="s">
+      <c r="A54" s="64" t="s">
         <v>230</v>
       </c>
       <c r="I54" t="e">
@@ -6629,7 +6626,7 @@
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="65" t="s">
+      <c r="A55" s="64" t="s">
         <v>231</v>
       </c>
       <c r="H55" t="s">
@@ -6649,7 +6646,7 @@
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="65" t="s">
+      <c r="A56" s="64" t="s">
         <v>230</v>
       </c>
       <c r="I56" t="e">
@@ -6666,7 +6663,7 @@
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="65" t="s">
+      <c r="A57" s="64" t="s">
         <v>231</v>
       </c>
       <c r="H57" t="s">
@@ -6686,7 +6683,7 @@
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="65" t="s">
+      <c r="A58" s="64" t="s">
         <v>232</v>
       </c>
       <c r="I58" t="e">
@@ -6703,7 +6700,7 @@
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="65" t="s">
+      <c r="A59" s="64" t="s">
         <v>233</v>
       </c>
       <c r="I59" t="e">
@@ -6720,7 +6717,7 @@
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="65" t="s">
+      <c r="A60" s="64" t="s">
         <v>234</v>
       </c>
       <c r="I60" t="e">
@@ -6737,7 +6734,7 @@
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="65" t="s">
+      <c r="A61" s="64" t="s">
         <v>235</v>
       </c>
       <c r="H61" t="s">
@@ -6757,7 +6754,7 @@
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="65" t="s">
+      <c r="A62" s="64" t="s">
         <v>236</v>
       </c>
       <c r="I62" t="e">
@@ -6774,7 +6771,7 @@
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="65" t="s">
+      <c r="A63" s="64" t="s">
         <v>232</v>
       </c>
       <c r="H63" t="s">
@@ -6794,7 +6791,7 @@
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="65" t="s">
+      <c r="A64" s="64" t="s">
         <v>233</v>
       </c>
       <c r="I64" t="e">
@@ -6811,7 +6808,7 @@
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="65" t="s">
+      <c r="A65" s="64" t="s">
         <v>234</v>
       </c>
       <c r="H65" t="s">
@@ -6831,7 +6828,7 @@
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="65" t="s">
+      <c r="A66" s="64" t="s">
         <v>235</v>
       </c>
       <c r="I66" t="e">
@@ -6848,7 +6845,7 @@
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="65" t="s">
+      <c r="A67" s="64" t="s">
         <v>236</v>
       </c>
       <c r="H67" t="s">
@@ -6868,7 +6865,7 @@
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="64"/>
+      <c r="A68" s="63"/>
       <c r="I68" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
@@ -6883,7 +6880,7 @@
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A69" s="64"/>
+      <c r="A69" s="63"/>
       <c r="H69" t="s">
         <v>201</v>
       </c>
@@ -6901,7 +6898,7 @@
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A70" s="64"/>
+      <c r="A70" s="63"/>
       <c r="I70" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
@@ -6916,7 +6913,7 @@
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="64"/>
+      <c r="A71" s="63"/>
       <c r="H71" t="s">
         <v>202</v>
       </c>
@@ -6934,7 +6931,7 @@
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72" s="64"/>
+      <c r="A72" s="63"/>
       <c r="I72" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
@@ -6949,7 +6946,7 @@
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A73" s="64"/>
+      <c r="A73" s="63"/>
       <c r="I73" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
@@ -6964,7 +6961,7 @@
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A74" s="64"/>
+      <c r="A74" s="63"/>
       <c r="I74" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
@@ -6979,7 +6976,7 @@
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A75" s="64"/>
+      <c r="A75" s="63"/>
       <c r="H75" t="s">
         <v>203</v>
       </c>
@@ -6997,1192 +6994,1192 @@
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A76" s="64"/>
+      <c r="A76" s="63"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A77" s="64"/>
+      <c r="A77" s="63"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A78" s="64"/>
+      <c r="A78" s="63"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A79" s="64"/>
+      <c r="A79" s="63"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A80" s="64"/>
+      <c r="A80" s="63"/>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="64"/>
+      <c r="A81" s="63"/>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="64"/>
+      <c r="A82" s="63"/>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="64"/>
+      <c r="A83" s="63"/>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="64"/>
+      <c r="A84" s="63"/>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="64"/>
+      <c r="A85" s="63"/>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="64"/>
+      <c r="A86" s="63"/>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="64"/>
+      <c r="A87" s="63"/>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="64"/>
+      <c r="A88" s="63"/>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="64"/>
+      <c r="A89" s="63"/>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="64"/>
+      <c r="A90" s="63"/>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="64"/>
+      <c r="A91" s="63"/>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="64"/>
+      <c r="A92" s="63"/>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="64"/>
+      <c r="A93" s="63"/>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="64"/>
+      <c r="A94" s="63"/>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="64"/>
+      <c r="A95" s="63"/>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="64"/>
+      <c r="A96" s="63"/>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="64"/>
+      <c r="A97" s="63"/>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="64"/>
+      <c r="A98" s="63"/>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="64"/>
+      <c r="A99" s="63"/>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="64"/>
+      <c r="A100" s="63"/>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="64"/>
+      <c r="A101" s="63"/>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="64"/>
+      <c r="A102" s="63"/>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="64"/>
+      <c r="A103" s="63"/>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="64"/>
+      <c r="A104" s="63"/>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" s="64"/>
+      <c r="A105" s="63"/>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="64"/>
+      <c r="A106" s="63"/>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" s="64"/>
+      <c r="A107" s="63"/>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="64"/>
+      <c r="A108" s="63"/>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="64"/>
+      <c r="A109" s="63"/>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="64"/>
+      <c r="A110" s="63"/>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" s="64"/>
+      <c r="A111" s="63"/>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" s="64"/>
+      <c r="A112" s="63"/>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="64"/>
+      <c r="A113" s="63"/>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="64"/>
+      <c r="A114" s="63"/>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="64"/>
+      <c r="A115" s="63"/>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="64"/>
+      <c r="A116" s="63"/>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" s="64"/>
+      <c r="A117" s="63"/>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" s="64"/>
+      <c r="A118" s="63"/>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" s="64"/>
+      <c r="A119" s="63"/>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="64"/>
+      <c r="A120" s="63"/>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" s="64"/>
+      <c r="A121" s="63"/>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" s="64"/>
+      <c r="A122" s="63"/>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" s="64"/>
+      <c r="A123" s="63"/>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" s="64"/>
+      <c r="A124" s="63"/>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" s="64"/>
+      <c r="A125" s="63"/>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" s="64"/>
+      <c r="A126" s="63"/>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" s="64"/>
+      <c r="A127" s="63"/>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" s="64"/>
+      <c r="A128" s="63"/>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="64"/>
+      <c r="A129" s="63"/>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="64"/>
+      <c r="A130" s="63"/>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="64"/>
+      <c r="A131" s="63"/>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="64"/>
+      <c r="A132" s="63"/>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="64"/>
+      <c r="A133" s="63"/>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" s="64"/>
+      <c r="A134" s="63"/>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="64"/>
+      <c r="A135" s="63"/>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" s="64"/>
+      <c r="A136" s="63"/>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="64"/>
+      <c r="A137" s="63"/>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" s="64"/>
+      <c r="A138" s="63"/>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="64"/>
+      <c r="A139" s="63"/>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="64"/>
+      <c r="A140" s="63"/>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" s="64"/>
+      <c r="A141" s="63"/>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" s="64"/>
+      <c r="A142" s="63"/>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="64"/>
+      <c r="A143" s="63"/>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" s="64"/>
+      <c r="A144" s="63"/>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" s="64"/>
+      <c r="A145" s="63"/>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="64"/>
+      <c r="A146" s="63"/>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="64"/>
+      <c r="A147" s="63"/>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" s="64"/>
+      <c r="A148" s="63"/>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" s="64"/>
+      <c r="A149" s="63"/>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="64"/>
+      <c r="A150" s="63"/>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" s="64"/>
+      <c r="A151" s="63"/>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" s="64"/>
+      <c r="A152" s="63"/>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="64"/>
+      <c r="A153" s="63"/>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" s="64"/>
+      <c r="A154" s="63"/>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" s="64"/>
+      <c r="A155" s="63"/>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" s="64"/>
+      <c r="A156" s="63"/>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" s="64"/>
+      <c r="A157" s="63"/>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" s="64"/>
+      <c r="A158" s="63"/>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" s="64"/>
+      <c r="A159" s="63"/>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" s="64"/>
+      <c r="A160" s="63"/>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" s="64"/>
+      <c r="A161" s="63"/>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" s="64"/>
+      <c r="A162" s="63"/>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163" s="64"/>
+      <c r="A163" s="63"/>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" s="64"/>
+      <c r="A164" s="63"/>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" s="64"/>
+      <c r="A165" s="63"/>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166" s="64"/>
+      <c r="A166" s="63"/>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" s="64"/>
+      <c r="A167" s="63"/>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168" s="64"/>
+      <c r="A168" s="63"/>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169" s="64"/>
+      <c r="A169" s="63"/>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A170" s="64"/>
+      <c r="A170" s="63"/>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" s="64"/>
+      <c r="A171" s="63"/>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172" s="64"/>
+      <c r="A172" s="63"/>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A173" s="64"/>
+      <c r="A173" s="63"/>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174" s="64"/>
+      <c r="A174" s="63"/>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" s="64"/>
+      <c r="A175" s="63"/>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176" s="64"/>
+      <c r="A176" s="63"/>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" s="64"/>
+      <c r="A177" s="63"/>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178" s="64"/>
+      <c r="A178" s="63"/>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A179" s="64"/>
+      <c r="A179" s="63"/>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" s="64"/>
+      <c r="A180" s="63"/>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181" s="64"/>
+      <c r="A181" s="63"/>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A182" s="64"/>
+      <c r="A182" s="63"/>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" s="64"/>
+      <c r="A183" s="63"/>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A184" s="64"/>
+      <c r="A184" s="63"/>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185" s="64"/>
+      <c r="A185" s="63"/>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186" s="64"/>
+      <c r="A186" s="63"/>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A187" s="64"/>
+      <c r="A187" s="63"/>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A188" s="64"/>
+      <c r="A188" s="63"/>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189" s="64"/>
+      <c r="A189" s="63"/>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A190" s="64"/>
+      <c r="A190" s="63"/>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A191" s="64"/>
+      <c r="A191" s="63"/>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A192" s="64"/>
+      <c r="A192" s="63"/>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A193" s="64"/>
+      <c r="A193" s="63"/>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A194" s="64"/>
+      <c r="A194" s="63"/>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A195" s="64"/>
+      <c r="A195" s="63"/>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A196" s="64"/>
+      <c r="A196" s="63"/>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A197" s="64"/>
+      <c r="A197" s="63"/>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A198" s="64"/>
+      <c r="A198" s="63"/>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A199" s="64"/>
+      <c r="A199" s="63"/>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A200" s="64"/>
+      <c r="A200" s="63"/>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A201" s="64"/>
+      <c r="A201" s="63"/>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A202" s="64"/>
+      <c r="A202" s="63"/>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A203" s="64"/>
+      <c r="A203" s="63"/>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A204" s="64"/>
+      <c r="A204" s="63"/>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A205" s="64"/>
+      <c r="A205" s="63"/>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A206" s="64"/>
+      <c r="A206" s="63"/>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A207" s="64"/>
+      <c r="A207" s="63"/>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A208" s="64"/>
+      <c r="A208" s="63"/>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A209" s="64"/>
+      <c r="A209" s="63"/>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A210" s="64"/>
+      <c r="A210" s="63"/>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A211" s="64"/>
+      <c r="A211" s="63"/>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A212" s="64"/>
+      <c r="A212" s="63"/>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A213" s="64"/>
+      <c r="A213" s="63"/>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A214" s="64"/>
+      <c r="A214" s="63"/>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A215" s="64"/>
+      <c r="A215" s="63"/>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A216" s="64"/>
+      <c r="A216" s="63"/>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A217" s="64"/>
+      <c r="A217" s="63"/>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A218" s="64"/>
+      <c r="A218" s="63"/>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A219" s="64"/>
+      <c r="A219" s="63"/>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A220" s="64"/>
+      <c r="A220" s="63"/>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A221" s="64"/>
+      <c r="A221" s="63"/>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A222" s="64"/>
+      <c r="A222" s="63"/>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A223" s="64"/>
+      <c r="A223" s="63"/>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A224" s="64"/>
+      <c r="A224" s="63"/>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A225" s="64"/>
+      <c r="A225" s="63"/>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A226" s="64"/>
+      <c r="A226" s="63"/>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A227" s="64"/>
+      <c r="A227" s="63"/>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A228" s="64"/>
+      <c r="A228" s="63"/>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A229" s="64"/>
+      <c r="A229" s="63"/>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A230" s="64"/>
+      <c r="A230" s="63"/>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A231" s="64"/>
+      <c r="A231" s="63"/>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A232" s="64"/>
+      <c r="A232" s="63"/>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A233" s="64"/>
+      <c r="A233" s="63"/>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A234" s="64"/>
+      <c r="A234" s="63"/>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A235" s="64"/>
+      <c r="A235" s="63"/>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A236" s="64"/>
+      <c r="A236" s="63"/>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A237" s="64"/>
+      <c r="A237" s="63"/>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A238" s="64"/>
+      <c r="A238" s="63"/>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A239" s="64"/>
+      <c r="A239" s="63"/>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A240" s="64"/>
+      <c r="A240" s="63"/>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A241" s="64"/>
+      <c r="A241" s="63"/>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A242" s="64"/>
+      <c r="A242" s="63"/>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A243" s="64"/>
+      <c r="A243" s="63"/>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A244" s="64"/>
+      <c r="A244" s="63"/>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A245" s="64"/>
+      <c r="A245" s="63"/>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A246" s="64"/>
+      <c r="A246" s="63"/>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A247" s="64"/>
+      <c r="A247" s="63"/>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A248" s="64"/>
+      <c r="A248" s="63"/>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A249" s="64"/>
+      <c r="A249" s="63"/>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A250" s="64"/>
+      <c r="A250" s="63"/>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A251" s="64"/>
+      <c r="A251" s="63"/>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A252" s="64"/>
+      <c r="A252" s="63"/>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A253" s="64"/>
+      <c r="A253" s="63"/>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A254" s="64"/>
+      <c r="A254" s="63"/>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A255" s="64"/>
+      <c r="A255" s="63"/>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A256" s="64"/>
+      <c r="A256" s="63"/>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A257" s="64"/>
+      <c r="A257" s="63"/>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A258" s="64"/>
+      <c r="A258" s="63"/>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A259" s="64"/>
+      <c r="A259" s="63"/>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A260" s="64"/>
+      <c r="A260" s="63"/>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A261" s="64"/>
+      <c r="A261" s="63"/>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A262" s="64"/>
+      <c r="A262" s="63"/>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A263" s="64"/>
+      <c r="A263" s="63"/>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A264" s="64"/>
+      <c r="A264" s="63"/>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A265" s="64"/>
+      <c r="A265" s="63"/>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A266" s="64"/>
+      <c r="A266" s="63"/>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A267" s="64"/>
+      <c r="A267" s="63"/>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A268" s="64"/>
+      <c r="A268" s="63"/>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A269" s="64"/>
+      <c r="A269" s="63"/>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A270" s="64"/>
+      <c r="A270" s="63"/>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A271" s="64"/>
+      <c r="A271" s="63"/>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A272" s="64"/>
+      <c r="A272" s="63"/>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A273" s="64"/>
+      <c r="A273" s="63"/>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A274" s="64"/>
+      <c r="A274" s="63"/>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A275" s="64"/>
+      <c r="A275" s="63"/>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A276" s="64"/>
+      <c r="A276" s="63"/>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A277" s="64"/>
+      <c r="A277" s="63"/>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A278" s="64"/>
+      <c r="A278" s="63"/>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A279" s="64"/>
+      <c r="A279" s="63"/>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A280" s="64"/>
+      <c r="A280" s="63"/>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A281" s="64"/>
+      <c r="A281" s="63"/>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A282" s="64"/>
+      <c r="A282" s="63"/>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A283" s="64"/>
+      <c r="A283" s="63"/>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A284" s="64"/>
+      <c r="A284" s="63"/>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A285" s="64"/>
+      <c r="A285" s="63"/>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A286" s="64"/>
+      <c r="A286" s="63"/>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A287" s="64"/>
+      <c r="A287" s="63"/>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A288" s="64"/>
+      <c r="A288" s="63"/>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A289" s="64"/>
+      <c r="A289" s="63"/>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A290" s="64"/>
+      <c r="A290" s="63"/>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A291" s="64"/>
+      <c r="A291" s="63"/>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A292" s="64"/>
+      <c r="A292" s="63"/>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A293" s="64"/>
+      <c r="A293" s="63"/>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A294" s="64"/>
+      <c r="A294" s="63"/>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A295" s="64"/>
+      <c r="A295" s="63"/>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A296" s="64"/>
+      <c r="A296" s="63"/>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A297" s="64"/>
+      <c r="A297" s="63"/>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A298" s="64"/>
+      <c r="A298" s="63"/>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A299" s="64"/>
+      <c r="A299" s="63"/>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A300" s="64"/>
+      <c r="A300" s="63"/>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A301" s="64"/>
+      <c r="A301" s="63"/>
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A302" s="64"/>
+      <c r="A302" s="63"/>
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A303" s="64"/>
+      <c r="A303" s="63"/>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A304" s="64"/>
+      <c r="A304" s="63"/>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A305" s="64"/>
+      <c r="A305" s="63"/>
     </row>
     <row r="306" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A306" s="64"/>
+      <c r="A306" s="63"/>
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A307" s="64"/>
+      <c r="A307" s="63"/>
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A308" s="64"/>
+      <c r="A308" s="63"/>
     </row>
     <row r="309" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A309" s="64"/>
+      <c r="A309" s="63"/>
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A310" s="64"/>
+      <c r="A310" s="63"/>
     </row>
     <row r="311" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A311" s="64"/>
+      <c r="A311" s="63"/>
     </row>
     <row r="312" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A312" s="64"/>
+      <c r="A312" s="63"/>
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A313" s="64"/>
+      <c r="A313" s="63"/>
     </row>
     <row r="314" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A314" s="64"/>
+      <c r="A314" s="63"/>
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A315" s="64"/>
+      <c r="A315" s="63"/>
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A316" s="64"/>
+      <c r="A316" s="63"/>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A317" s="64"/>
+      <c r="A317" s="63"/>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A318" s="64"/>
+      <c r="A318" s="63"/>
     </row>
     <row r="319" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A319" s="64"/>
+      <c r="A319" s="63"/>
     </row>
     <row r="320" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A320" s="64"/>
+      <c r="A320" s="63"/>
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A321" s="64"/>
+      <c r="A321" s="63"/>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A322" s="64"/>
+      <c r="A322" s="63"/>
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A323" s="64"/>
+      <c r="A323" s="63"/>
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A324" s="64"/>
+      <c r="A324" s="63"/>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A325" s="64"/>
+      <c r="A325" s="63"/>
     </row>
     <row r="326" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A326" s="64"/>
+      <c r="A326" s="63"/>
     </row>
     <row r="327" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A327" s="64"/>
+      <c r="A327" s="63"/>
     </row>
     <row r="328" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A328" s="64"/>
+      <c r="A328" s="63"/>
     </row>
     <row r="329" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A329" s="64"/>
+      <c r="A329" s="63"/>
     </row>
     <row r="330" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A330" s="64"/>
+      <c r="A330" s="63"/>
     </row>
     <row r="331" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A331" s="64"/>
+      <c r="A331" s="63"/>
     </row>
     <row r="332" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A332" s="64"/>
+      <c r="A332" s="63"/>
     </row>
     <row r="333" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A333" s="64"/>
+      <c r="A333" s="63"/>
     </row>
     <row r="334" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A334" s="64"/>
+      <c r="A334" s="63"/>
     </row>
     <row r="335" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A335" s="64"/>
+      <c r="A335" s="63"/>
     </row>
     <row r="336" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A336" s="64"/>
+      <c r="A336" s="63"/>
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A337" s="64"/>
+      <c r="A337" s="63"/>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A338" s="64"/>
+      <c r="A338" s="63"/>
     </row>
     <row r="339" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A339" s="64"/>
+      <c r="A339" s="63"/>
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A340" s="64"/>
+      <c r="A340" s="63"/>
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A341" s="64"/>
+      <c r="A341" s="63"/>
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A342" s="64"/>
+      <c r="A342" s="63"/>
     </row>
     <row r="343" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A343" s="64"/>
+      <c r="A343" s="63"/>
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A344" s="64"/>
+      <c r="A344" s="63"/>
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A345" s="64"/>
+      <c r="A345" s="63"/>
     </row>
     <row r="346" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A346" s="64"/>
+      <c r="A346" s="63"/>
     </row>
     <row r="347" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A347" s="64"/>
+      <c r="A347" s="63"/>
     </row>
     <row r="348" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A348" s="64"/>
+      <c r="A348" s="63"/>
     </row>
     <row r="349" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A349" s="64"/>
+      <c r="A349" s="63"/>
     </row>
     <row r="350" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A350" s="64"/>
+      <c r="A350" s="63"/>
     </row>
     <row r="351" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A351" s="64"/>
+      <c r="A351" s="63"/>
     </row>
     <row r="352" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A352" s="64"/>
+      <c r="A352" s="63"/>
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A353" s="64"/>
+      <c r="A353" s="63"/>
     </row>
     <row r="354" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A354" s="64"/>
+      <c r="A354" s="63"/>
     </row>
     <row r="355" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A355" s="64"/>
+      <c r="A355" s="63"/>
     </row>
     <row r="356" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A356" s="64"/>
+      <c r="A356" s="63"/>
     </row>
     <row r="357" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A357" s="64"/>
+      <c r="A357" s="63"/>
     </row>
     <row r="358" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A358" s="64"/>
+      <c r="A358" s="63"/>
     </row>
     <row r="359" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A359" s="64"/>
+      <c r="A359" s="63"/>
     </row>
     <row r="360" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A360" s="64"/>
+      <c r="A360" s="63"/>
     </row>
     <row r="361" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A361" s="64"/>
+      <c r="A361" s="63"/>
     </row>
     <row r="362" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A362" s="64"/>
+      <c r="A362" s="63"/>
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A363" s="64"/>
+      <c r="A363" s="63"/>
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A364" s="64"/>
+      <c r="A364" s="63"/>
     </row>
     <row r="365" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A365" s="64"/>
+      <c r="A365" s="63"/>
     </row>
     <row r="366" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A366" s="64"/>
+      <c r="A366" s="63"/>
     </row>
     <row r="367" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A367" s="64"/>
+      <c r="A367" s="63"/>
     </row>
     <row r="368" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A368" s="64"/>
+      <c r="A368" s="63"/>
     </row>
     <row r="369" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A369" s="64"/>
+      <c r="A369" s="63"/>
     </row>
     <row r="370" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A370" s="64"/>
+      <c r="A370" s="63"/>
     </row>
     <row r="371" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A371" s="64"/>
+      <c r="A371" s="63"/>
     </row>
     <row r="372" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A372" s="64"/>
+      <c r="A372" s="63"/>
     </row>
     <row r="373" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A373" s="64"/>
+      <c r="A373" s="63"/>
     </row>
     <row r="374" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A374" s="64"/>
+      <c r="A374" s="63"/>
     </row>
     <row r="375" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A375" s="64"/>
+      <c r="A375" s="63"/>
     </row>
     <row r="376" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A376" s="64"/>
+      <c r="A376" s="63"/>
     </row>
     <row r="377" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A377" s="64"/>
+      <c r="A377" s="63"/>
     </row>
     <row r="378" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A378" s="64"/>
+      <c r="A378" s="63"/>
     </row>
     <row r="379" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A379" s="64"/>
+      <c r="A379" s="63"/>
     </row>
     <row r="380" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A380" s="64"/>
+      <c r="A380" s="63"/>
     </row>
     <row r="381" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A381" s="64"/>
+      <c r="A381" s="63"/>
     </row>
     <row r="382" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A382" s="64"/>
+      <c r="A382" s="63"/>
     </row>
     <row r="383" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A383" s="64"/>
+      <c r="A383" s="63"/>
     </row>
     <row r="384" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A384" s="64"/>
+      <c r="A384" s="63"/>
     </row>
     <row r="385" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A385" s="64"/>
+      <c r="A385" s="63"/>
     </row>
     <row r="386" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A386" s="64"/>
+      <c r="A386" s="63"/>
     </row>
     <row r="387" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A387" s="64"/>
+      <c r="A387" s="63"/>
     </row>
     <row r="388" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A388" s="64"/>
+      <c r="A388" s="63"/>
     </row>
     <row r="389" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A389" s="64"/>
+      <c r="A389" s="63"/>
     </row>
     <row r="390" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A390" s="64"/>
+      <c r="A390" s="63"/>
     </row>
     <row r="391" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A391" s="64"/>
+      <c r="A391" s="63"/>
     </row>
     <row r="392" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A392" s="64"/>
+      <c r="A392" s="63"/>
     </row>
     <row r="393" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A393" s="64"/>
+      <c r="A393" s="63"/>
     </row>
     <row r="394" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A394" s="64"/>
+      <c r="A394" s="63"/>
     </row>
     <row r="395" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A395" s="64"/>
+      <c r="A395" s="63"/>
     </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A396" s="64"/>
+      <c r="A396" s="63"/>
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A397" s="64"/>
+      <c r="A397" s="63"/>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A398" s="64"/>
+      <c r="A398" s="63"/>
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A399" s="64"/>
+      <c r="A399" s="63"/>
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A400" s="64"/>
+      <c r="A400" s="63"/>
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A401" s="64"/>
+      <c r="A401" s="63"/>
     </row>
     <row r="402" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A402" s="64"/>
+      <c r="A402" s="63"/>
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A403" s="64"/>
+      <c r="A403" s="63"/>
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A404" s="64"/>
+      <c r="A404" s="63"/>
     </row>
     <row r="405" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A405" s="64"/>
+      <c r="A405" s="63"/>
     </row>
     <row r="406" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A406" s="64"/>
+      <c r="A406" s="63"/>
     </row>
     <row r="407" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A407" s="64"/>
+      <c r="A407" s="63"/>
     </row>
     <row r="408" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A408" s="64"/>
+      <c r="A408" s="63"/>
     </row>
     <row r="409" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A409" s="64"/>
+      <c r="A409" s="63"/>
     </row>
     <row r="410" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A410" s="64"/>
+      <c r="A410" s="63"/>
     </row>
     <row r="411" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A411" s="64"/>
+      <c r="A411" s="63"/>
     </row>
     <row r="412" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A412" s="64"/>
+      <c r="A412" s="63"/>
     </row>
     <row r="413" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A413" s="64"/>
+      <c r="A413" s="63"/>
     </row>
     <row r="414" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A414" s="64"/>
+      <c r="A414" s="63"/>
     </row>
     <row r="415" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A415" s="64"/>
+      <c r="A415" s="63"/>
     </row>
     <row r="416" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A416" s="64"/>
+      <c r="A416" s="63"/>
     </row>
     <row r="417" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A417" s="64"/>
+      <c r="A417" s="63"/>
     </row>
     <row r="418" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A418" s="64"/>
+      <c r="A418" s="63"/>
     </row>
     <row r="419" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A419" s="64"/>
+      <c r="A419" s="63"/>
     </row>
     <row r="420" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A420" s="64"/>
+      <c r="A420" s="63"/>
     </row>
     <row r="421" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A421" s="64"/>
+      <c r="A421" s="63"/>
     </row>
     <row r="422" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A422" s="64"/>
+      <c r="A422" s="63"/>
     </row>
     <row r="423" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A423" s="64"/>
+      <c r="A423" s="63"/>
     </row>
     <row r="424" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A424" s="64"/>
+      <c r="A424" s="63"/>
     </row>
     <row r="425" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A425" s="64"/>
+      <c r="A425" s="63"/>
     </row>
     <row r="426" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A426" s="64"/>
+      <c r="A426" s="63"/>
     </row>
     <row r="427" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A427" s="64"/>
+      <c r="A427" s="63"/>
     </row>
     <row r="428" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A428" s="64"/>
+      <c r="A428" s="63"/>
     </row>
     <row r="429" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A429" s="64"/>
+      <c r="A429" s="63"/>
     </row>
     <row r="430" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A430" s="64"/>
+      <c r="A430" s="63"/>
     </row>
     <row r="431" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A431" s="64"/>
+      <c r="A431" s="63"/>
     </row>
     <row r="432" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A432" s="64"/>
+      <c r="A432" s="63"/>
     </row>
     <row r="433" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A433" s="64"/>
+      <c r="A433" s="63"/>
     </row>
     <row r="434" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A434" s="64"/>
+      <c r="A434" s="63"/>
     </row>
     <row r="435" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A435" s="64"/>
+      <c r="A435" s="63"/>
     </row>
     <row r="436" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A436" s="64"/>
+      <c r="A436" s="63"/>
     </row>
     <row r="437" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A437" s="64"/>
+      <c r="A437" s="63"/>
     </row>
     <row r="438" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A438" s="64"/>
+      <c r="A438" s="63"/>
     </row>
     <row r="439" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A439" s="64"/>
+      <c r="A439" s="63"/>
     </row>
     <row r="440" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A440" s="64"/>
+      <c r="A440" s="63"/>
     </row>
     <row r="441" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A441" s="64"/>
+      <c r="A441" s="63"/>
     </row>
     <row r="442" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A442" s="64"/>
+      <c r="A442" s="63"/>
     </row>
     <row r="443" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A443" s="64"/>
+      <c r="A443" s="63"/>
     </row>
     <row r="444" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A444" s="64"/>
+      <c r="A444" s="63"/>
     </row>
     <row r="445" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A445" s="64"/>
+      <c r="A445" s="63"/>
     </row>
     <row r="446" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A446" s="64"/>
+      <c r="A446" s="63"/>
     </row>
     <row r="447" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A447" s="64"/>
+      <c r="A447" s="63"/>
     </row>
     <row r="448" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A448" s="64"/>
+      <c r="A448" s="63"/>
     </row>
     <row r="449" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A449" s="64"/>
+      <c r="A449" s="63"/>
     </row>
     <row r="450" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A450" s="64"/>
+      <c r="A450" s="63"/>
     </row>
     <row r="451" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A451" s="64"/>
+      <c r="A451" s="63"/>
     </row>
     <row r="452" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A452" s="64"/>
+      <c r="A452" s="63"/>
     </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A453" s="64"/>
+      <c r="A453" s="63"/>
     </row>
     <row r="454" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A454" s="64"/>
+      <c r="A454" s="63"/>
     </row>
     <row r="455" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A455" s="64"/>
+      <c r="A455" s="63"/>
     </row>
     <row r="456" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A456" s="64"/>
+      <c r="A456" s="63"/>
     </row>
     <row r="457" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A457" s="64"/>
+      <c r="A457" s="63"/>
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A458" s="64"/>
+      <c r="A458" s="63"/>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A459" s="64"/>
+      <c r="A459" s="63"/>
     </row>
     <row r="460" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A460" s="64"/>
+      <c r="A460" s="63"/>
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A461" s="64"/>
+      <c r="A461" s="63"/>
     </row>
     <row r="462" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A462" s="64"/>
+      <c r="A462" s="63"/>
     </row>
     <row r="463" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A463" s="64"/>
+      <c r="A463" s="63"/>
     </row>
     <row r="464" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A464" s="64"/>
+      <c r="A464" s="63"/>
     </row>
     <row r="465" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A465" s="64"/>
+      <c r="A465" s="63"/>
     </row>
     <row r="466" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A466" s="64"/>
+      <c r="A466" s="63"/>
     </row>
     <row r="467" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A467" s="64"/>
+      <c r="A467" s="63"/>
     </row>
     <row r="468" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A468" s="64"/>
+      <c r="A468" s="63"/>
     </row>
     <row r="469" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A469" s="64"/>
+      <c r="A469" s="63"/>
     </row>
     <row r="470" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A470" s="64"/>
+      <c r="A470" s="63"/>
     </row>
     <row r="471" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A471" s="64"/>
+      <c r="A471" s="63"/>
     </row>
   </sheetData>
   <dataConsolidate/>

</xml_diff>

<commit_message>
se suben cambio para demo
</commit_message>
<xml_diff>
--- a/Documentacion/indicadores revisión junio 11 2014.xlsx
+++ b/Documentacion/indicadores revisión junio 11 2014.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="Ajustes" sheetId="1" r:id="rId1"/>
@@ -293,10 +293,6 @@
   </si>
   <si>
     <t>Anual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indicador de especialización/ Coeficiente de Penetración de Mercado
-</t>
   </si>
   <si>
     <t>IEI = (Xij – Mij) / (Xin)</t>
@@ -1256,15 +1252,19 @@
   <si>
     <t>ID</t>
   </si>
+  <si>
+    <t xml:space="preserve">Indicador de especialización / Coeficiente de Penetración de Mercado
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.000%"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -1546,7 +1546,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="77">
@@ -1668,16 +1668,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1695,7 +1695,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1722,7 +1722,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1733,6 +1733,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1757,9 +1760,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3481,10 +3481,10 @@
   <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3504,15 +3504,15 @@
     <row r="1" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:18" s="10" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="69" t="s">
+      <c r="C2" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="69"/>
+      <c r="D2" s="70"/>
       <c r="E2" s="8" t="s">
         <v>2</v>
       </c>
@@ -3529,31 +3529,31 @@
         <v>6</v>
       </c>
       <c r="J2" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="K2" s="46" t="s">
+        <v>153</v>
+      </c>
+      <c r="L2" s="46" t="s">
+        <v>146</v>
+      </c>
+      <c r="M2" s="46" t="s">
+        <v>156</v>
+      </c>
+      <c r="N2" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="K2" s="46" t="s">
-        <v>154</v>
-      </c>
-      <c r="L2" s="46" t="s">
+      <c r="O2" s="46" t="s">
+        <v>150</v>
+      </c>
+      <c r="P2" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="M2" s="46" t="s">
-        <v>157</v>
-      </c>
-      <c r="N2" s="46" t="s">
-        <v>146</v>
-      </c>
-      <c r="O2" s="46" t="s">
+      <c r="Q2" s="46" t="s">
+        <v>148</v>
+      </c>
+      <c r="R2" s="46" t="s">
         <v>151</v>
-      </c>
-      <c r="P2" s="46" t="s">
-        <v>148</v>
-      </c>
-      <c r="Q2" s="46" t="s">
-        <v>149</v>
-      </c>
-      <c r="R2" s="46" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3572,41 +3572,41 @@
       <c r="E3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="70" t="s">
+      <c r="F3" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="72" t="s">
+      <c r="G3" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="72" t="s">
+      <c r="H3" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="74" t="s">
+      <c r="I3" s="75" t="s">
         <v>14</v>
       </c>
       <c r="J3" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K3" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L3" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M3" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N3" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O3" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P3" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Q3" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R3" s="20"/>
     </row>
@@ -3626,33 +3626,33 @@
       <c r="E4" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="71"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
       <c r="J4" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K4" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L4" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M4" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N4" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O4" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P4" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Q4" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R4" s="20"/>
     </row>
@@ -3675,32 +3675,32 @@
       <c r="F5" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
       <c r="J5" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K5" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L5" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M5" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N5" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O5" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P5" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Q5" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R5" s="20"/>
     </row>
@@ -3733,31 +3733,31 @@
         <v>31</v>
       </c>
       <c r="J6" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K6" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L6" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M6" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N6" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O6" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P6" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Q6" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R6" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3771,7 +3771,7 @@
         <v>33</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E7" s="16" t="s">
         <v>34</v>
@@ -3789,31 +3789,31 @@
         <v>31</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K7" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L7" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M7" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N7" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O7" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P7" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Q7" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R7" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="114" customHeight="1" x14ac:dyDescent="0.2">
@@ -3845,28 +3845,28 @@
         <v>45</v>
       </c>
       <c r="J8" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K8" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L8" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M8" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N8" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O8" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P8" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Q8" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R8" s="20"/>
     </row>
@@ -3875,52 +3875,52 @@
         <v>22</v>
       </c>
       <c r="B9" s="48" t="s">
+        <v>238</v>
+      </c>
+      <c r="C9" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="53" t="s">
+      <c r="D9" s="54" t="s">
+        <v>155</v>
+      </c>
+      <c r="E9" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="54" t="s">
-        <v>156</v>
-      </c>
-      <c r="E9" s="31" t="s">
+      <c r="F9" s="31" t="s">
         <v>48</v>
-      </c>
-      <c r="F9" s="31" t="s">
-        <v>49</v>
       </c>
       <c r="G9" s="32" t="s">
         <v>12</v>
       </c>
       <c r="H9" s="32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I9" s="32" t="s">
         <v>31</v>
       </c>
       <c r="J9" s="53" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K9" s="53" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L9" s="53" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M9" s="53" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N9" s="53" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O9" s="53" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P9" s="53" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Q9" s="53" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R9" s="53"/>
     </row>
@@ -3929,52 +3929,52 @@
         <v>4</v>
       </c>
       <c r="B10" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="D10" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="E10" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="F10" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="G10" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="H10" s="14" t="s">
         <v>56</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>57</v>
       </c>
       <c r="I10" s="23" t="s">
         <v>31</v>
       </c>
       <c r="J10" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K10" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L10" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M10" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N10" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O10" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P10" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Q10" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R10" s="20"/>
     </row>
@@ -3983,31 +3983,31 @@
         <v>5</v>
       </c>
       <c r="B11" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="D11" s="76" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="75" t="s">
+      <c r="E11" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="68" t="s">
+      <c r="F11" s="76" t="s">
         <v>61</v>
       </c>
-      <c r="F11" s="75" t="s">
+      <c r="G11" s="76" t="s">
         <v>62</v>
       </c>
-      <c r="G11" s="75" t="s">
-        <v>63</v>
-      </c>
-      <c r="H11" s="68" t="s">
+      <c r="H11" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="I11" s="68" t="s">
+      <c r="I11" s="69" t="s">
         <v>31</v>
       </c>
       <c r="J11" s="25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K11" s="25">
         <v>15</v>
@@ -4025,19 +4025,19 @@
         <v>6</v>
       </c>
       <c r="B12" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="D12" s="75"/>
-      <c r="E12" s="68"/>
-      <c r="F12" s="75"/>
-      <c r="G12" s="75"/>
-      <c r="H12" s="68"/>
-      <c r="I12" s="68"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="69"/>
       <c r="J12" s="25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K12" s="25">
         <v>1500000</v>
@@ -4059,28 +4059,28 @@
         <v>7</v>
       </c>
       <c r="B13" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="D13" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="E13" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="E13" s="26" t="s">
+      <c r="F13" s="16" t="s">
         <v>69</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>70</v>
       </c>
       <c r="G13" s="21" t="s">
         <v>29</v>
       </c>
       <c r="H13" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I13" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="144" customHeight="1" x14ac:dyDescent="0.2">
@@ -4088,31 +4088,31 @@
         <v>9</v>
       </c>
       <c r="B14" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="D14" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="E14" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="F14" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="G14" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="G14" s="21" t="s">
+      <c r="H14" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="H14" s="21" t="s">
-        <v>78</v>
-      </c>
       <c r="I14" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J14" s="52" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="144" customHeight="1" x14ac:dyDescent="0.2">
@@ -4120,31 +4120,31 @@
         <v>10</v>
       </c>
       <c r="B15" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="D15" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="E15" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="F15" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="F15" s="18" t="s">
-        <v>83</v>
-      </c>
       <c r="G15" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I15" s="23" t="s">
         <v>31</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="89.25" x14ac:dyDescent="0.2">
@@ -4152,25 +4152,25 @@
         <v>11</v>
       </c>
       <c r="B16" s="49" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="D16" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="E16" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="F16" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="F16" s="16" t="s">
+      <c r="G16" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="G16" s="23" t="s">
-        <v>89</v>
-      </c>
       <c r="H16" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I16" s="21" t="s">
         <v>31</v>
@@ -4181,22 +4181,22 @@
         <v>12</v>
       </c>
       <c r="B17" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="D17" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="E17" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="F17" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="G17" s="21" t="s">
         <v>94</v>
-      </c>
-      <c r="G17" s="21" t="s">
-        <v>95</v>
       </c>
       <c r="H17" s="21" t="s">
         <v>44</v>
@@ -4210,25 +4210,25 @@
         <v>13</v>
       </c>
       <c r="B18" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="D18" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="D18" s="29" t="s">
+      <c r="E18" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="E18" s="30" t="s">
+      <c r="F18" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="F18" s="31" t="s">
-        <v>100</v>
-      </c>
       <c r="G18" s="32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H18" s="32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I18" s="32" t="s">
         <v>31</v>
@@ -4239,25 +4239,25 @@
         <v>16</v>
       </c>
       <c r="B19" s="59" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="D19" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="E19" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="E19" s="33" t="s">
+      <c r="F19" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="F19" s="30" t="s">
+      <c r="G19" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="G19" s="32" t="s">
+      <c r="H19" s="32" t="s">
         <v>106</v>
-      </c>
-      <c r="H19" s="32" t="s">
-        <v>107</v>
       </c>
       <c r="I19" s="23" t="s">
         <v>31</v>
@@ -4268,25 +4268,25 @@
         <v>17</v>
       </c>
       <c r="B20" s="59" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="C20" s="33" t="s">
+      <c r="D20" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="D20" s="33" t="s">
+      <c r="E20" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="E20" s="33" t="s">
+      <c r="F20" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="F20" s="33" t="s">
-        <v>112</v>
-      </c>
       <c r="G20" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="H20" s="32" t="s">
         <v>106</v>
-      </c>
-      <c r="H20" s="32" t="s">
-        <v>107</v>
       </c>
       <c r="I20" s="23" t="s">
         <v>31</v>
@@ -4297,25 +4297,25 @@
         <v>15</v>
       </c>
       <c r="B21" s="59" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="C21" s="34" t="s">
+      <c r="D21" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="D21" s="35" t="s">
+      <c r="E21" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="E21" s="36" t="s">
+      <c r="F21" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="F21" s="37" t="s">
-        <v>117</v>
-      </c>
       <c r="G21" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="H21" s="14" t="s">
         <v>56</v>
-      </c>
-      <c r="H21" s="14" t="s">
-        <v>57</v>
       </c>
       <c r="I21" s="23" t="s">
         <v>31</v>
@@ -4326,25 +4326,25 @@
         <v>14</v>
       </c>
       <c r="B22" s="57" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="D22" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="D22" s="38" t="s">
+      <c r="E22" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="E22" s="36" t="s">
+      <c r="F22" s="33" t="s">
         <v>121</v>
       </c>
-      <c r="F22" s="33" t="s">
-        <v>122</v>
-      </c>
       <c r="G22" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H22" s="28" t="s">
         <v>56</v>
-      </c>
-      <c r="H22" s="28" t="s">
-        <v>57</v>
       </c>
       <c r="I22" s="38" t="s">
         <v>31</v>
@@ -4355,25 +4355,25 @@
         <v>20</v>
       </c>
       <c r="B23" s="58" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C23" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="D23" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="D23" s="38" t="s">
+      <c r="E23" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="E23" s="38" t="s">
+      <c r="F23" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="F23" s="31" t="s">
-        <v>126</v>
-      </c>
       <c r="G23" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H23" s="55" t="s">
         <v>56</v>
-      </c>
-      <c r="H23" s="55" t="s">
-        <v>57</v>
       </c>
       <c r="I23" s="38" t="s">
         <v>31</v>
@@ -4384,25 +4384,25 @@
         <v>21</v>
       </c>
       <c r="B24" s="65" t="s">
+        <v>126</v>
+      </c>
+      <c r="C24" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="C24" s="28" t="s">
+      <c r="D24" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="D24" s="32" t="s">
+      <c r="E24" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="E24" s="31" t="s">
+      <c r="F24" s="31" t="s">
         <v>130</v>
-      </c>
-      <c r="F24" s="31" t="s">
-        <v>131</v>
       </c>
       <c r="G24" s="32" t="s">
         <v>12</v>
       </c>
       <c r="H24" s="32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I24" s="32" t="s">
         <v>31</v>
@@ -4413,25 +4413,25 @@
         <v>21</v>
       </c>
       <c r="B25" s="48" t="s">
+        <v>132</v>
+      </c>
+      <c r="C25" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="D25" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="D25" s="23" t="s">
+      <c r="E25" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="E25" s="32" t="s">
+      <c r="F25" s="31" t="s">
         <v>136</v>
-      </c>
-      <c r="F25" s="31" t="s">
-        <v>137</v>
       </c>
       <c r="G25" s="32" t="s">
         <v>12</v>
       </c>
       <c r="H25" s="32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I25" s="21" t="s">
         <v>45</v>
@@ -4441,26 +4441,26 @@
       <c r="A26" s="66">
         <v>23</v>
       </c>
-      <c r="B26" s="76" t="s">
+      <c r="B26" s="68" t="s">
+        <v>138</v>
+      </c>
+      <c r="C26" s="39" t="s">
         <v>139</v>
       </c>
-      <c r="C26" s="39" t="s">
+      <c r="D26" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="D26" s="23" t="s">
+      <c r="E26" s="38" t="s">
         <v>141</v>
       </c>
-      <c r="E26" s="38" t="s">
+      <c r="F26" s="40" t="s">
         <v>142</v>
       </c>
-      <c r="F26" s="40" t="s">
+      <c r="G26" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="H26" s="41" t="s">
         <v>143</v>
-      </c>
-      <c r="G26" s="41" t="s">
-        <v>77</v>
-      </c>
-      <c r="H26" s="41" t="s">
-        <v>144</v>
       </c>
       <c r="I26" s="41" t="s">
         <v>31</v>
@@ -4529,10 +4529,10 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="50" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="50" t="s">
         <v>160</v>
-      </c>
-      <c r="B1" s="50" t="s">
-        <v>161</v>
       </c>
       <c r="C1" s="50">
         <v>2012</v>
@@ -4544,25 +4544,25 @@
         <v>2014</v>
       </c>
       <c r="F1" s="50" t="s">
+        <v>161</v>
+      </c>
+      <c r="G1" s="50" t="s">
         <v>162</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="H1" s="50" t="s">
         <v>163</v>
       </c>
-      <c r="H1" s="50" t="s">
+      <c r="I1" s="50" t="s">
         <v>164</v>
       </c>
-      <c r="I1" s="50" t="s">
+      <c r="J1" s="50" t="s">
         <v>165</v>
       </c>
-      <c r="J1" s="50" t="s">
+      <c r="K1" s="50" t="s">
         <v>166</v>
       </c>
-      <c r="K1" s="50" t="s">
+      <c r="L1" s="50" t="s">
         <v>167</v>
-      </c>
-      <c r="L1" s="50" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -5669,22 +5669,22 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="50" t="s">
+        <v>171</v>
+      </c>
+      <c r="B30" s="50" t="s">
         <v>172</v>
       </c>
-      <c r="B30" s="50" t="s">
+      <c r="C30" s="50" t="s">
         <v>173</v>
       </c>
-      <c r="C30" s="50" t="s">
+      <c r="H30" t="s">
+        <v>147</v>
+      </c>
+      <c r="I30" t="s">
         <v>174</v>
       </c>
-      <c r="H30" t="s">
-        <v>148</v>
-      </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>175</v>
-      </c>
-      <c r="J30" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -5719,13 +5719,13 @@
         <v>204.75</v>
       </c>
       <c r="H32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I32" t="s">
+        <v>174</v>
+      </c>
+      <c r="J32" t="s">
         <v>175</v>
-      </c>
-      <c r="J32" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -5797,103 +5797,103 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="63" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B2" s="60" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="63" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B3" s="61" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="63" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B4" s="61" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="63" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B5" s="61" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="63" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B6" s="61" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="63" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B7" s="61" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="63" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B8" s="61" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="63" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B9" s="61" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="63" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B10" s="61" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="63" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B11" s="61" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="63" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B12" s="61" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="63" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B13" s="61" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H13">
         <v>2010</v>
@@ -5910,10 +5910,10 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="63" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B14" s="61" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H14">
         <v>2011</v>
@@ -5930,10 +5930,10 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="63" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B15" s="61" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H15">
         <v>2012</v>
@@ -5950,10 +5950,10 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="63" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B16" s="61" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H16">
         <v>2013</v>
@@ -5970,77 +5970,77 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="63" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B17" s="61" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="63" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B18" s="61" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="63" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B19" s="61" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="63" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B20" s="61" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="63" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B21" s="61" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="63" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B22" s="61" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="63" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B23" s="61" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="63" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B24" s="61" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="63" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B25" s="61" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I25">
         <f>FIND("-",H25)</f>
@@ -6057,10 +6057,10 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="63" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B26" s="61" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I26" t="e">
         <f t="shared" ref="I26:I75" si="0">FIND("-",H26)</f>
@@ -6077,13 +6077,13 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="63" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B27" s="61" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H27" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I27">
         <f t="shared" si="0"/>
@@ -6100,10 +6100,10 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B28" s="61" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I28" t="e">
         <f t="shared" si="0"/>
@@ -6120,13 +6120,13 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="63" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B29" s="61" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H29" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I29">
         <f t="shared" si="0"/>
@@ -6143,10 +6143,10 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="63" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B30" s="61" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I30" t="e">
         <f t="shared" si="0"/>
@@ -6163,13 +6163,13 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="63" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B31" s="61" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I31">
         <f t="shared" si="0"/>
@@ -6186,10 +6186,10 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="63" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B32" s="61" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I32" t="e">
         <f t="shared" si="0"/>
@@ -6206,13 +6206,13 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="63" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B33" s="61" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H33" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I33">
         <f t="shared" si="0"/>
@@ -6229,10 +6229,10 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="63" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B34" s="61" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I34" t="e">
         <f t="shared" si="0"/>
@@ -6249,13 +6249,13 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="63" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B35" s="61" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H35" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I35">
         <f t="shared" si="0"/>
@@ -6272,10 +6272,10 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="63" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B36" s="61" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I36" t="e">
         <f t="shared" si="0"/>
@@ -6292,13 +6292,13 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B37" s="61" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H37" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I37">
         <f t="shared" si="0"/>
@@ -6315,7 +6315,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="63" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I38" t="e">
         <f t="shared" si="0"/>
@@ -6332,10 +6332,10 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H39" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I39">
         <f t="shared" si="0"/>
@@ -6352,7 +6352,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="63" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I40" t="e">
         <f t="shared" si="0"/>
@@ -6369,10 +6369,10 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="63" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H41" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I41">
         <f t="shared" si="0"/>
@@ -6389,7 +6389,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="63" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I42" t="e">
         <f t="shared" si="0"/>
@@ -6406,7 +6406,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="63" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I43" t="e">
         <f t="shared" si="0"/>
@@ -6423,7 +6423,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="63" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I44" t="e">
         <f t="shared" si="0"/>
@@ -6440,10 +6440,10 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="63" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H45" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I45">
         <f t="shared" si="0"/>
@@ -6460,7 +6460,7 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="63" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I46" t="e">
         <f t="shared" si="0"/>
@@ -6477,10 +6477,10 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="63" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H47" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I47">
         <f t="shared" si="0"/>
@@ -6497,7 +6497,7 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="63" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I48" t="e">
         <f t="shared" si="0"/>
@@ -6514,10 +6514,10 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="63" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H49" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I49">
         <f t="shared" si="0"/>
@@ -6534,7 +6534,7 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="63" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I50" t="e">
         <f t="shared" si="0"/>
@@ -6551,10 +6551,10 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="63" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H51" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I51">
         <f t="shared" si="0"/>
@@ -6571,7 +6571,7 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="63" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I52" t="e">
         <f t="shared" si="0"/>
@@ -6588,10 +6588,10 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="63" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H53" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I53">
         <f t="shared" si="0"/>
@@ -6608,7 +6608,7 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="63" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I54" t="e">
         <f t="shared" si="0"/>
@@ -6625,10 +6625,10 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="63" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H55" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I55">
         <f t="shared" si="0"/>
@@ -6645,7 +6645,7 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="63" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I56" t="e">
         <f t="shared" si="0"/>
@@ -6662,10 +6662,10 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="63" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H57" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I57">
         <f t="shared" si="0"/>
@@ -6682,7 +6682,7 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="63" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I58" t="e">
         <f t="shared" si="0"/>
@@ -6699,7 +6699,7 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="63" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I59" t="e">
         <f t="shared" si="0"/>
@@ -6716,7 +6716,7 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="63" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I60" t="e">
         <f t="shared" si="0"/>
@@ -6733,10 +6733,10 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="63" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H61" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I61">
         <f t="shared" si="0"/>
@@ -6753,7 +6753,7 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="63" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I62" t="e">
         <f t="shared" si="0"/>
@@ -6770,10 +6770,10 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="63" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H63" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I63">
         <f t="shared" si="0"/>
@@ -6790,7 +6790,7 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="63" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I64" t="e">
         <f t="shared" si="0"/>
@@ -6807,10 +6807,10 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="63" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H65" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I65">
         <f t="shared" si="0"/>
@@ -6827,7 +6827,7 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="63" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I66" t="e">
         <f t="shared" si="0"/>
@@ -6844,10 +6844,10 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="63" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H67" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I67">
         <f t="shared" si="0"/>
@@ -6880,7 +6880,7 @@
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="62"/>
       <c r="H69" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I69">
         <f t="shared" si="0"/>
@@ -6913,7 +6913,7 @@
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="62"/>
       <c r="H71" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I71">
         <f t="shared" si="0"/>
@@ -6976,7 +6976,7 @@
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="62"/>
       <c r="H75" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I75">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
se realizan ajustes de indicadores segun comentarios MADR
</commit_message>
<xml_diff>
--- a/Documentacion/indicadores revisión junio 11 2014.xlsx
+++ b/Documentacion/indicadores revisión junio 11 2014.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ajustes" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja2" sheetId="3" r:id="rId3"/>
+    <sheet name="Pendientes" sheetId="4" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId3"/>
+    <sheet name="Hoja2" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ajustes!$A$2:$R$26</definedName>
@@ -22,7 +23,7 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="250">
   <si>
     <t>NOMBRE INDICADOR</t>
   </si>
@@ -1256,6 +1257,39 @@
     <t xml:space="preserve">Indicador de especialización / Coeficiente de Penetración de Mercado
 </t>
   </si>
+  <si>
+    <t>indicador_id</t>
+  </si>
+  <si>
+    <t>comentario</t>
+  </si>
+  <si>
+    <t>Indicador Nombre</t>
+  </si>
+  <si>
+    <t>Balanza Comercial</t>
+  </si>
+  <si>
+    <t>El indicador se calcula por defecto en valores, incluir la opción de calcularlo en cantidades (kg y toneladas).</t>
+  </si>
+  <si>
+    <t>Agregar una opción de consulta comparativa de periodos entre diferentes años, con el fin de no tener que hacer más de una consulta o reproceses en Excel para hacer análisis entre períodos.</t>
+  </si>
+  <si>
+    <t>Balanza Comercial Relativa</t>
+  </si>
+  <si>
+    <t>Agregar una opción de consulta comparativa de períodos entre diferentes años, con el fin de no tener que hacer más de una consulta o reprocesos en Excel para hacer análisis entre períodos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Para el índice de BCR se sugiere utilizar el estilo de gráfica de línea con marcadores. </t>
+  </si>
+  <si>
+    <t>Variación balanza comercial</t>
+  </si>
+  <si>
+    <t>El indicador se calcula por defecto en valores, incluir la opción de calcularlo en cantidades (kg y toneladas)</t>
+  </si>
 </sst>
 </file>
 
@@ -1266,7 +1300,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1420,6 +1454,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1549,7 +1589,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1760,6 +1800,11 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3480,11 +3525,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4514,6 +4559,93 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="102.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="77" t="s">
+        <v>239</v>
+      </c>
+      <c r="B1" s="77" t="s">
+        <v>241</v>
+      </c>
+      <c r="C1" s="77" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C2" s="79" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>245</v>
+      </c>
+      <c r="C3" s="78" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>242</v>
+      </c>
+      <c r="C4" s="78" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>242</v>
+      </c>
+      <c r="C5" s="78" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>248</v>
+      </c>
+      <c r="C6" s="79" t="s">
+        <v>249</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
@@ -5780,7 +5912,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M471"/>
   <sheetViews>

</xml_diff>

<commit_message>
ajustes en textos y formulas de indicadores segunda revision
</commit_message>
<xml_diff>
--- a/Documentacion/indicadores revisión junio 11 2014.xlsx
+++ b/Documentacion/indicadores revisión junio 11 2014.xlsx
@@ -16,6 +16,7 @@
     <sheet name="Pendientes" sheetId="4" r:id="rId2"/>
     <sheet name="Hoja1" sheetId="2" r:id="rId3"/>
     <sheet name="Hoja2" sheetId="3" r:id="rId4"/>
+    <sheet name="Hoja3" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ajustes!$A$2:$R$26</definedName>
@@ -23,7 +24,7 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="251">
   <si>
     <t>NOMBRE INDICADOR</t>
   </si>
@@ -1289,6 +1290,9 @@
   </si>
   <si>
     <t>El indicador se calcula por defecto en valores, incluir la opción de calcularlo en cantidades (kg y toneladas)</t>
+  </si>
+  <si>
+    <t>Por encima de 100%, laPor debajo de 100%, las exportaciones agropecuarias y agroindustriales están creciendo por debajo de las exportaciones totales del país al mundo o a un mercado específico.</t>
   </si>
 </sst>
 </file>
@@ -3526,10 +3530,10 @@
   <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8316,4 +8320,47 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>8356726746</v>
+      </c>
+      <c r="B1">
+        <v>7196639555</v>
+      </c>
+      <c r="C1">
+        <v>7876526541</v>
+      </c>
+      <c r="D1">
+        <f>LINEST(LN(A1:C1))*100</f>
+        <v>-2.9589900231934863</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>250</v>
+      </c>
+      <c r="B6" t="str">
+        <f>CLEAN(TRIM(A6))</f>
+        <v>Por encima de 100%, laPor debajo de 100%, las exportaciones agropecuarias y agroindustriales están creciendo por debajo de las exportaciones totales del país al mundo o a un mercado específico.</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>